<commit_message>
No notable performance improvement in the optimizations, but the code shortened up a bit.
I also changed from a single uniform, uWriteToSecondIntermediateBuffer,
to two uniforms that will be easier to maintain and easier to read:
uIntermediateBufferReadOffset and uIntermediateBufferWriteOffset.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="22">
   <si>
     <t>State</t>
   </si>
@@ -77,9 +77,6 @@
     <t>stddev</t>
   </si>
   <si>
-    <t>IntermediateData uses a single buffer</t>
-  </si>
-  <si>
     <t>GetBitForPrefixScan uses no conditional branching</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>ParallelPrefixScan writes to and from shared memory</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>IntermediateData uses a single buffer (don't know why it's a bit slower now, but it's microseconds)</t>
   </si>
 </sst>
 </file>
@@ -448,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K149"/>
+  <dimension ref="A1:O149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,67 +473,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12714</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>3792</v>
+      </c>
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -541,8 +556,18 @@
         <f>AVERAGE(B16:B47)</f>
         <v>187.28125</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12">
+        <f>AVERAGE(K16:K47)</f>
+        <v>116.0625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1108570</v>
       </c>
@@ -556,16 +581,45 @@
         <f>_xlfn.STDEV.P(B16:B47)</f>
         <v>680.80376368557006</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>882246</v>
+      </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13">
+        <f>_xlfn.STDEV.P(K16:K47)</f>
+        <v>28.20343230441997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <f>MEDIAN(B16:B47)</f>
+        <v>54</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14">
+        <f>MEDIAN(K16:K47)</f>
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -576,43 +630,90 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>228</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
         <v>15</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <f>AVERAGE(B50:B81)</f>
         <v>44.65625</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="B17">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="K17">
+        <v>210</v>
+      </c>
+      <c r="L17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(K50:K81)</f>
+        <v>39.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <f>_xlfn.STDEV.P(B50:B81)</f>
         <v>48.476546761681568</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="J18">
         <v>2</v>
       </c>
-      <c r="B18">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>122</v>
+      </c>
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <f>_xlfn.STDEV.P(K50:K81)</f>
+        <v>50.16332699293379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -623,10 +724,30 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <f>MEDIAN(B50:B81)</f>
+        <v>31</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>96</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19">
+        <f>MEDIAN(K50:K81)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -636,58 +757,111 @@
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>111</v>
+      </c>
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
         <v>15</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <f>AVERAGE(B84:B115)</f>
         <v>28.09375</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22">
+        <v>127</v>
+      </c>
+      <c r="L22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22">
+        <f>AVERAGE(K84:K115)</f>
+        <v>22.96875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <f>_xlfn.STDEV.P(B84:B115)</f>
         <v>7.759507776753626</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="J23">
         <v>7</v>
       </c>
-      <c r="B23">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>106</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23">
+        <f>_xlfn.STDEV.P(K84:K115)</f>
+        <v>3.7789249049828975</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -698,65 +872,144 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <f>MEDIAN(B84:B115)</f>
+        <v>26</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24">
+        <f>MEDIAN(K84:K115)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>9</v>
+      </c>
+      <c r="K25">
+        <v>120</v>
+      </c>
+      <c r="L25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <v>114</v>
+      </c>
+      <c r="L26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
         <v>15</v>
       </c>
-      <c r="F24">
+      <c r="F27">
         <f>AVERAGE(B118:B149)</f>
         <v>74.46875</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="J27">
+        <v>11</v>
+      </c>
+      <c r="K27">
+        <v>112</v>
+      </c>
+      <c r="L27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27">
+        <f>AVERAGE(K118:K149)</f>
+        <v>30.3125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
         <v>16</v>
       </c>
-      <c r="F25">
+      <c r="F28">
         <f>_xlfn.STDEV.P(B118:B149)</f>
         <v>188.87925779036061</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>99</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>11</v>
-      </c>
-      <c r="B27">
-        <v>100</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="J28">
         <v>12</v>
       </c>
-      <c r="B28">
-        <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>114</v>
+      </c>
+      <c r="L28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N28" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28">
+        <f>_xlfn.STDEV.P(K118:K149)</f>
+        <v>22.378054959044139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>13</v>
       </c>
@@ -766,8 +1019,31 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <f>MEDIAN(B118:B149)</f>
+        <v>34</v>
+      </c>
+      <c r="J29">
+        <v>13</v>
+      </c>
+      <c r="K29">
+        <v>101</v>
+      </c>
+      <c r="L29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29">
+        <f>MEDIAN(K118:K149)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14</v>
       </c>
@@ -777,8 +1053,17 @@
       <c r="C30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>14</v>
+      </c>
+      <c r="K30">
+        <v>113</v>
+      </c>
+      <c r="L30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -788,8 +1073,17 @@
       <c r="C31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>15</v>
+      </c>
+      <c r="K31">
+        <v>113</v>
+      </c>
+      <c r="L31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>16</v>
       </c>
@@ -799,8 +1093,17 @@
       <c r="C32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>16</v>
+      </c>
+      <c r="K32">
+        <v>115</v>
+      </c>
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>17</v>
       </c>
@@ -810,8 +1113,17 @@
       <c r="C33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>17</v>
+      </c>
+      <c r="K33">
+        <v>90</v>
+      </c>
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>18</v>
       </c>
@@ -821,8 +1133,17 @@
       <c r="C34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>18</v>
+      </c>
+      <c r="K34">
+        <v>97</v>
+      </c>
+      <c r="L34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>19</v>
       </c>
@@ -832,8 +1153,17 @@
       <c r="C35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>19</v>
+      </c>
+      <c r="K35">
+        <v>99</v>
+      </c>
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -843,8 +1173,17 @@
       <c r="C36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>20</v>
+      </c>
+      <c r="K36">
+        <v>118</v>
+      </c>
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>21</v>
       </c>
@@ -854,8 +1193,17 @@
       <c r="C37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>21</v>
+      </c>
+      <c r="K37">
+        <v>111</v>
+      </c>
+      <c r="L37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>22</v>
       </c>
@@ -865,8 +1213,17 @@
       <c r="C38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>22</v>
+      </c>
+      <c r="K38">
+        <v>117</v>
+      </c>
+      <c r="L38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>23</v>
       </c>
@@ -876,8 +1233,17 @@
       <c r="C39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>23</v>
+      </c>
+      <c r="K39">
+        <v>106</v>
+      </c>
+      <c r="L39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>24</v>
       </c>
@@ -887,8 +1253,17 @@
       <c r="C40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>24</v>
+      </c>
+      <c r="K40">
+        <v>105</v>
+      </c>
+      <c r="L40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>25</v>
       </c>
@@ -898,8 +1273,17 @@
       <c r="C41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>25</v>
+      </c>
+      <c r="K41">
+        <v>112</v>
+      </c>
+      <c r="L41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>26</v>
       </c>
@@ -909,8 +1293,17 @@
       <c r="C42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>26</v>
+      </c>
+      <c r="K42">
+        <v>124</v>
+      </c>
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>27</v>
       </c>
@@ -920,8 +1313,17 @@
       <c r="C43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>27</v>
+      </c>
+      <c r="K43">
+        <v>108</v>
+      </c>
+      <c r="L43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>28</v>
       </c>
@@ -931,8 +1333,17 @@
       <c r="C44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <v>28</v>
+      </c>
+      <c r="K44">
+        <v>125</v>
+      </c>
+      <c r="L44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>29</v>
       </c>
@@ -942,8 +1353,17 @@
       <c r="C45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>29</v>
+      </c>
+      <c r="K45">
+        <v>101</v>
+      </c>
+      <c r="L45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>30</v>
       </c>
@@ -953,8 +1373,17 @@
       <c r="C46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J46">
+        <v>30</v>
+      </c>
+      <c r="K46">
+        <v>96</v>
+      </c>
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>31</v>
       </c>
@@ -964,13 +1393,25 @@
       <c r="C47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <v>31</v>
+      </c>
+      <c r="K47">
+        <v>103</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -980,8 +1421,17 @@
       <c r="C50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>317</v>
+      </c>
+      <c r="L50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -991,8 +1441,17 @@
       <c r="C51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>31</v>
+      </c>
+      <c r="L51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1002,8 +1461,17 @@
       <c r="C52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>32</v>
+      </c>
+      <c r="L52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1013,8 +1481,17 @@
       <c r="C53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J53">
+        <v>3</v>
+      </c>
+      <c r="K53">
+        <v>28</v>
+      </c>
+      <c r="L53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4</v>
       </c>
@@ -1024,8 +1501,17 @@
       <c r="C54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>30</v>
+      </c>
+      <c r="L54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5</v>
       </c>
@@ -1035,8 +1521,17 @@
       <c r="C55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J55">
+        <v>5</v>
+      </c>
+      <c r="K55">
+        <v>28</v>
+      </c>
+      <c r="L55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6</v>
       </c>
@@ -1046,8 +1541,17 @@
       <c r="C56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J56">
+        <v>6</v>
+      </c>
+      <c r="K56">
+        <v>33</v>
+      </c>
+      <c r="L56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1057,8 +1561,17 @@
       <c r="C57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J57">
+        <v>7</v>
+      </c>
+      <c r="K57">
+        <v>29</v>
+      </c>
+      <c r="L57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>8</v>
       </c>
@@ -1068,8 +1581,17 @@
       <c r="C58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J58">
+        <v>8</v>
+      </c>
+      <c r="K58">
+        <v>29</v>
+      </c>
+      <c r="L58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
@@ -1079,8 +1601,17 @@
       <c r="C59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J59">
+        <v>9</v>
+      </c>
+      <c r="K59">
+        <v>33</v>
+      </c>
+      <c r="L59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10</v>
       </c>
@@ -1090,8 +1621,17 @@
       <c r="C60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J60">
+        <v>10</v>
+      </c>
+      <c r="K60">
+        <v>29</v>
+      </c>
+      <c r="L60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>11</v>
       </c>
@@ -1101,8 +1641,17 @@
       <c r="C61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J61">
+        <v>11</v>
+      </c>
+      <c r="K61">
+        <v>27</v>
+      </c>
+      <c r="L61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>12</v>
       </c>
@@ -1112,8 +1661,17 @@
       <c r="C62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J62">
+        <v>12</v>
+      </c>
+      <c r="K62">
+        <v>28</v>
+      </c>
+      <c r="L62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>13</v>
       </c>
@@ -1123,8 +1681,17 @@
       <c r="C63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J63">
+        <v>13</v>
+      </c>
+      <c r="K63">
+        <v>29</v>
+      </c>
+      <c r="L63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14</v>
       </c>
@@ -1134,8 +1701,17 @@
       <c r="C64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J64">
+        <v>14</v>
+      </c>
+      <c r="K64">
+        <v>28</v>
+      </c>
+      <c r="L64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>15</v>
       </c>
@@ -1145,8 +1721,17 @@
       <c r="C65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J65">
+        <v>15</v>
+      </c>
+      <c r="K65">
+        <v>28</v>
+      </c>
+      <c r="L65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>16</v>
       </c>
@@ -1156,8 +1741,17 @@
       <c r="C66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J66">
+        <v>16</v>
+      </c>
+      <c r="K66">
+        <v>30</v>
+      </c>
+      <c r="L66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1167,8 +1761,17 @@
       <c r="C67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J67">
+        <v>17</v>
+      </c>
+      <c r="K67">
+        <v>27</v>
+      </c>
+      <c r="L67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>18</v>
       </c>
@@ -1178,8 +1781,17 @@
       <c r="C68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J68">
+        <v>18</v>
+      </c>
+      <c r="K68">
+        <v>26</v>
+      </c>
+      <c r="L68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>19</v>
       </c>
@@ -1189,8 +1801,17 @@
       <c r="C69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J69">
+        <v>19</v>
+      </c>
+      <c r="K69">
+        <v>28</v>
+      </c>
+      <c r="L69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20</v>
       </c>
@@ -1200,8 +1821,17 @@
       <c r="C70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J70">
+        <v>20</v>
+      </c>
+      <c r="K70">
+        <v>32</v>
+      </c>
+      <c r="L70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>21</v>
       </c>
@@ -1211,8 +1841,17 @@
       <c r="C71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J71">
+        <v>21</v>
+      </c>
+      <c r="K71">
+        <v>29</v>
+      </c>
+      <c r="L71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>22</v>
       </c>
@@ -1222,8 +1861,17 @@
       <c r="C72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J72">
+        <v>22</v>
+      </c>
+      <c r="K72">
+        <v>28</v>
+      </c>
+      <c r="L72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>23</v>
       </c>
@@ -1233,8 +1881,17 @@
       <c r="C73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J73">
+        <v>23</v>
+      </c>
+      <c r="K73">
+        <v>29</v>
+      </c>
+      <c r="L73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>24</v>
       </c>
@@ -1244,8 +1901,17 @@
       <c r="C74" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J74">
+        <v>24</v>
+      </c>
+      <c r="K74">
+        <v>27</v>
+      </c>
+      <c r="L74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>25</v>
       </c>
@@ -1255,8 +1921,17 @@
       <c r="C75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J75">
+        <v>25</v>
+      </c>
+      <c r="K75">
+        <v>55</v>
+      </c>
+      <c r="L75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>26</v>
       </c>
@@ -1266,8 +1941,17 @@
       <c r="C76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J76">
+        <v>26</v>
+      </c>
+      <c r="K76">
+        <v>38</v>
+      </c>
+      <c r="L76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>27</v>
       </c>
@@ -1277,8 +1961,17 @@
       <c r="C77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J77">
+        <v>27</v>
+      </c>
+      <c r="K77">
+        <v>30</v>
+      </c>
+      <c r="L77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>28</v>
       </c>
@@ -1288,8 +1981,17 @@
       <c r="C78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J78">
+        <v>28</v>
+      </c>
+      <c r="K78">
+        <v>32</v>
+      </c>
+      <c r="L78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>29</v>
       </c>
@@ -1299,8 +2001,17 @@
       <c r="C79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J79">
+        <v>29</v>
+      </c>
+      <c r="K79">
+        <v>27</v>
+      </c>
+      <c r="L79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>30</v>
       </c>
@@ -1310,8 +2021,17 @@
       <c r="C80" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J80">
+        <v>30</v>
+      </c>
+      <c r="K80">
+        <v>27</v>
+      </c>
+      <c r="L80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>31</v>
       </c>
@@ -1321,13 +2041,25 @@
       <c r="C81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J81">
+        <v>31</v>
+      </c>
+      <c r="K81">
+        <v>28</v>
+      </c>
+      <c r="L81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -1337,8 +2069,17 @@
       <c r="C84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>37</v>
+      </c>
+      <c r="L84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1</v>
       </c>
@@ -1348,8 +2089,17 @@
       <c r="C85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>23</v>
+      </c>
+      <c r="L85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2</v>
       </c>
@@ -1359,8 +2109,17 @@
       <c r="C86" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J86">
+        <v>2</v>
+      </c>
+      <c r="K86">
+        <v>23</v>
+      </c>
+      <c r="L86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3</v>
       </c>
@@ -1370,8 +2129,17 @@
       <c r="C87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J87">
+        <v>3</v>
+      </c>
+      <c r="K87">
+        <v>22</v>
+      </c>
+      <c r="L87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -1381,8 +2149,17 @@
       <c r="C88" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J88">
+        <v>4</v>
+      </c>
+      <c r="K88">
+        <v>23</v>
+      </c>
+      <c r="L88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>5</v>
       </c>
@@ -1392,8 +2169,17 @@
       <c r="C89" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J89">
+        <v>5</v>
+      </c>
+      <c r="K89">
+        <v>21</v>
+      </c>
+      <c r="L89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>6</v>
       </c>
@@ -1403,8 +2189,17 @@
       <c r="C90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J90">
+        <v>6</v>
+      </c>
+      <c r="K90">
+        <v>25</v>
+      </c>
+      <c r="L90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>7</v>
       </c>
@@ -1414,8 +2209,17 @@
       <c r="C91" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J91">
+        <v>7</v>
+      </c>
+      <c r="K91">
+        <v>22</v>
+      </c>
+      <c r="L91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>8</v>
       </c>
@@ -1425,8 +2229,17 @@
       <c r="C92" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J92">
+        <v>8</v>
+      </c>
+      <c r="K92">
+        <v>21</v>
+      </c>
+      <c r="L92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9</v>
       </c>
@@ -1436,8 +2249,17 @@
       <c r="C93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J93">
+        <v>9</v>
+      </c>
+      <c r="K93">
+        <v>23</v>
+      </c>
+      <c r="L93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>10</v>
       </c>
@@ -1447,8 +2269,17 @@
       <c r="C94" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J94">
+        <v>10</v>
+      </c>
+      <c r="K94">
+        <v>21</v>
+      </c>
+      <c r="L94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>11</v>
       </c>
@@ -1458,8 +2289,17 @@
       <c r="C95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J95">
+        <v>11</v>
+      </c>
+      <c r="K95">
+        <v>21</v>
+      </c>
+      <c r="L95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>12</v>
       </c>
@@ -1469,8 +2309,17 @@
       <c r="C96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J96">
+        <v>12</v>
+      </c>
+      <c r="K96">
+        <v>21</v>
+      </c>
+      <c r="L96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>13</v>
       </c>
@@ -1480,8 +2329,17 @@
       <c r="C97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J97">
+        <v>13</v>
+      </c>
+      <c r="K97">
+        <v>23</v>
+      </c>
+      <c r="L97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>14</v>
       </c>
@@ -1491,8 +2349,17 @@
       <c r="C98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J98">
+        <v>14</v>
+      </c>
+      <c r="K98">
+        <v>21</v>
+      </c>
+      <c r="L98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>15</v>
       </c>
@@ -1502,8 +2369,17 @@
       <c r="C99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J99">
+        <v>15</v>
+      </c>
+      <c r="K99">
+        <v>21</v>
+      </c>
+      <c r="L99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>16</v>
       </c>
@@ -1513,8 +2389,17 @@
       <c r="C100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J100">
+        <v>16</v>
+      </c>
+      <c r="K100">
+        <v>21</v>
+      </c>
+      <c r="L100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>17</v>
       </c>
@@ -1524,8 +2409,17 @@
       <c r="C101" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J101">
+        <v>17</v>
+      </c>
+      <c r="K101">
+        <v>21</v>
+      </c>
+      <c r="L101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>18</v>
       </c>
@@ -1535,8 +2429,17 @@
       <c r="C102" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J102">
+        <v>18</v>
+      </c>
+      <c r="K102">
+        <v>21</v>
+      </c>
+      <c r="L102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>19</v>
       </c>
@@ -1546,8 +2449,17 @@
       <c r="C103" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J103">
+        <v>19</v>
+      </c>
+      <c r="K103">
+        <v>23</v>
+      </c>
+      <c r="L103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>20</v>
       </c>
@@ -1557,8 +2469,17 @@
       <c r="C104" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J104">
+        <v>20</v>
+      </c>
+      <c r="K104">
+        <v>21</v>
+      </c>
+      <c r="L104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>21</v>
       </c>
@@ -1568,8 +2489,17 @@
       <c r="C105" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J105">
+        <v>21</v>
+      </c>
+      <c r="K105">
+        <v>21</v>
+      </c>
+      <c r="L105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>22</v>
       </c>
@@ -1579,8 +2509,17 @@
       <c r="C106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J106">
+        <v>22</v>
+      </c>
+      <c r="K106">
+        <v>21</v>
+      </c>
+      <c r="L106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>23</v>
       </c>
@@ -1590,8 +2529,17 @@
       <c r="C107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J107">
+        <v>23</v>
+      </c>
+      <c r="K107">
+        <v>21</v>
+      </c>
+      <c r="L107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>24</v>
       </c>
@@ -1601,8 +2549,17 @@
       <c r="C108" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J108">
+        <v>24</v>
+      </c>
+      <c r="K108">
+        <v>21</v>
+      </c>
+      <c r="L108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>25</v>
       </c>
@@ -1612,8 +2569,17 @@
       <c r="C109" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J109">
+        <v>25</v>
+      </c>
+      <c r="K109">
+        <v>34</v>
+      </c>
+      <c r="L109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>26</v>
       </c>
@@ -1623,8 +2589,17 @@
       <c r="C110" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J110">
+        <v>26</v>
+      </c>
+      <c r="K110">
+        <v>29</v>
+      </c>
+      <c r="L110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>27</v>
       </c>
@@ -1634,8 +2609,17 @@
       <c r="C111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J111">
+        <v>27</v>
+      </c>
+      <c r="K111">
+        <v>21</v>
+      </c>
+      <c r="L111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>28</v>
       </c>
@@ -1645,8 +2629,17 @@
       <c r="C112" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J112">
+        <v>28</v>
+      </c>
+      <c r="K112">
+        <v>28</v>
+      </c>
+      <c r="L112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>29</v>
       </c>
@@ -1656,8 +2649,17 @@
       <c r="C113" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J113">
+        <v>29</v>
+      </c>
+      <c r="K113">
+        <v>21</v>
+      </c>
+      <c r="L113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>30</v>
       </c>
@@ -1667,8 +2669,17 @@
       <c r="C114" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J114">
+        <v>30</v>
+      </c>
+      <c r="K114">
+        <v>21</v>
+      </c>
+      <c r="L114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>31</v>
       </c>
@@ -1678,13 +2689,25 @@
       <c r="C115" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J115">
+        <v>31</v>
+      </c>
+      <c r="K115">
+        <v>22</v>
+      </c>
+      <c r="L115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>0</v>
       </c>
@@ -1694,8 +2717,17 @@
       <c r="C118" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>154</v>
+      </c>
+      <c r="L118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1</v>
       </c>
@@ -1705,8 +2737,17 @@
       <c r="C119" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="K119">
+        <v>32</v>
+      </c>
+      <c r="L119" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2</v>
       </c>
@@ -1716,8 +2757,17 @@
       <c r="C120" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J120">
+        <v>2</v>
+      </c>
+      <c r="K120">
+        <v>26</v>
+      </c>
+      <c r="L120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>3</v>
       </c>
@@ -1727,8 +2777,17 @@
       <c r="C121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J121">
+        <v>3</v>
+      </c>
+      <c r="K121">
+        <v>26</v>
+      </c>
+      <c r="L121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>4</v>
       </c>
@@ -1738,8 +2797,17 @@
       <c r="C122" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J122">
+        <v>4</v>
+      </c>
+      <c r="K122">
+        <v>27</v>
+      </c>
+      <c r="L122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>5</v>
       </c>
@@ -1749,8 +2817,17 @@
       <c r="C123" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J123">
+        <v>5</v>
+      </c>
+      <c r="K123">
+        <v>27</v>
+      </c>
+      <c r="L123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>6</v>
       </c>
@@ -1760,8 +2837,17 @@
       <c r="C124" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J124">
+        <v>6</v>
+      </c>
+      <c r="K124">
+        <v>24</v>
+      </c>
+      <c r="L124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>7</v>
       </c>
@@ -1771,8 +2857,17 @@
       <c r="C125" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J125">
+        <v>7</v>
+      </c>
+      <c r="K125">
+        <v>32</v>
+      </c>
+      <c r="L125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>8</v>
       </c>
@@ -1782,8 +2877,17 @@
       <c r="C126" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J126">
+        <v>8</v>
+      </c>
+      <c r="K126">
+        <v>25</v>
+      </c>
+      <c r="L126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>9</v>
       </c>
@@ -1793,8 +2897,17 @@
       <c r="C127" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J127">
+        <v>9</v>
+      </c>
+      <c r="K127">
+        <v>36</v>
+      </c>
+      <c r="L127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>10</v>
       </c>
@@ -1804,8 +2917,17 @@
       <c r="C128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J128">
+        <v>10</v>
+      </c>
+      <c r="K128">
+        <v>25</v>
+      </c>
+      <c r="L128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>11</v>
       </c>
@@ -1815,8 +2937,17 @@
       <c r="C129" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J129">
+        <v>11</v>
+      </c>
+      <c r="K129">
+        <v>25</v>
+      </c>
+      <c r="L129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>12</v>
       </c>
@@ -1826,8 +2957,17 @@
       <c r="C130" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J130">
+        <v>12</v>
+      </c>
+      <c r="K130">
+        <v>25</v>
+      </c>
+      <c r="L130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>13</v>
       </c>
@@ -1837,8 +2977,17 @@
       <c r="C131" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J131">
+        <v>13</v>
+      </c>
+      <c r="K131">
+        <v>26</v>
+      </c>
+      <c r="L131" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>14</v>
       </c>
@@ -1848,8 +2997,17 @@
       <c r="C132" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J132">
+        <v>14</v>
+      </c>
+      <c r="K132">
+        <v>25</v>
+      </c>
+      <c r="L132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>15</v>
       </c>
@@ -1859,8 +3017,17 @@
       <c r="C133" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J133">
+        <v>15</v>
+      </c>
+      <c r="K133">
+        <v>23</v>
+      </c>
+      <c r="L133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>16</v>
       </c>
@@ -1870,8 +3037,17 @@
       <c r="C134" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J134">
+        <v>16</v>
+      </c>
+      <c r="K134">
+        <v>25</v>
+      </c>
+      <c r="L134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>17</v>
       </c>
@@ -1881,8 +3057,17 @@
       <c r="C135" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J135">
+        <v>17</v>
+      </c>
+      <c r="K135">
+        <v>24</v>
+      </c>
+      <c r="L135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>18</v>
       </c>
@@ -1892,8 +3077,17 @@
       <c r="C136" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J136">
+        <v>18</v>
+      </c>
+      <c r="K136">
+        <v>24</v>
+      </c>
+      <c r="L136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>19</v>
       </c>
@@ -1903,8 +3097,17 @@
       <c r="C137" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J137">
+        <v>19</v>
+      </c>
+      <c r="K137">
+        <v>26</v>
+      </c>
+      <c r="L137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>20</v>
       </c>
@@ -1914,8 +3117,17 @@
       <c r="C138" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J138">
+        <v>20</v>
+      </c>
+      <c r="K138">
+        <v>27</v>
+      </c>
+      <c r="L138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>21</v>
       </c>
@@ -1925,8 +3137,17 @@
       <c r="C139" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J139">
+        <v>21</v>
+      </c>
+      <c r="K139">
+        <v>25</v>
+      </c>
+      <c r="L139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>22</v>
       </c>
@@ -1936,8 +3157,17 @@
       <c r="C140" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J140">
+        <v>22</v>
+      </c>
+      <c r="K140">
+        <v>25</v>
+      </c>
+      <c r="L140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>23</v>
       </c>
@@ -1947,8 +3177,17 @@
       <c r="C141" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J141">
+        <v>23</v>
+      </c>
+      <c r="K141">
+        <v>26</v>
+      </c>
+      <c r="L141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>24</v>
       </c>
@@ -1958,8 +3197,17 @@
       <c r="C142" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J142">
+        <v>24</v>
+      </c>
+      <c r="K142">
+        <v>23</v>
+      </c>
+      <c r="L142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>25</v>
       </c>
@@ -1969,8 +3217,17 @@
       <c r="C143" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J143">
+        <v>25</v>
+      </c>
+      <c r="K143">
+        <v>26</v>
+      </c>
+      <c r="L143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>26</v>
       </c>
@@ -1980,8 +3237,17 @@
       <c r="C144" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J144">
+        <v>26</v>
+      </c>
+      <c r="K144">
+        <v>25</v>
+      </c>
+      <c r="L144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>27</v>
       </c>
@@ -1991,8 +3257,17 @@
       <c r="C145" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J145">
+        <v>27</v>
+      </c>
+      <c r="K145">
+        <v>25</v>
+      </c>
+      <c r="L145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>28</v>
       </c>
@@ -2002,8 +3277,17 @@
       <c r="C146" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J146">
+        <v>28</v>
+      </c>
+      <c r="K146">
+        <v>28</v>
+      </c>
+      <c r="L146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>29</v>
       </c>
@@ -2013,8 +3297,17 @@
       <c r="C147" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J147">
+        <v>29</v>
+      </c>
+      <c r="K147">
+        <v>26</v>
+      </c>
+      <c r="L147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>30</v>
       </c>
@@ -2024,8 +3317,17 @@
       <c r="C148" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J148">
+        <v>30</v>
+      </c>
+      <c r="K148">
+        <v>27</v>
+      </c>
+      <c r="L148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>31</v>
       </c>
@@ -2035,8 +3337,20 @@
       <c r="C149" t="s">
         <v>9</v>
       </c>
+      <c r="J149">
+        <v>31</v>
+      </c>
+      <c r="K149">
+        <v>30</v>
+      </c>
+      <c r="L149" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="G28:G59">
+    <sortCondition ref="G28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Now ParallelPrefixScan works in shared memory.
And I am getting a slight performance drop (32 prefix scans over each
bit of 1,000,000 items, and the median duration increased from ~55
microseconds to ~115.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="24">
   <si>
     <t>State</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>IntermediateData uses a single buffer (don't know why it's a bit slower now, but it's microseconds)</t>
+  </si>
+  <si>
+    <t>total sort time</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O149"/>
+  <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,449 +523,388 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>12714</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>23</v>
       </c>
       <c r="J10">
-        <v>3792</v>
+        <v>1478367</v>
       </c>
       <c r="K10" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <f>AVERAGE(B16:B47)</f>
-        <v>187.28125</v>
+        <v>8</v>
       </c>
       <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12">
-        <f>AVERAGE(K16:K47)</f>
-        <v>116.0625</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1108570</v>
+        <v>12714</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13">
-        <f>_xlfn.STDEV.P(B16:B47)</f>
-        <v>680.80376368557006</v>
-      </c>
       <c r="J13">
-        <v>882246</v>
+        <v>3386</v>
       </c>
       <c r="K13" t="s">
         <v>9</v>
-      </c>
-      <c r="N13" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13">
-        <f>_xlfn.STDEV.P(K16:K47)</f>
-        <v>28.20343230441997</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14">
-        <f>MEDIAN(B16:B47)</f>
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="N14" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14">
-        <f>MEDIAN(K16:K47)</f>
-        <v>111.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(B19:B50)</f>
+        <v>187.28125</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15">
+        <f>AVERAGE(K19:K50)</f>
+        <v>122.96875</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>3974</v>
-      </c>
-      <c r="C16" t="s">
+        <v>1108570</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <f>_xlfn.STDEV.P(B19:B50)</f>
+        <v>680.80376368557006</v>
       </c>
       <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>228</v>
-      </c>
-      <c r="L16" t="s">
+        <v>905057</v>
+      </c>
+      <c r="K16" t="s">
         <v>9</v>
       </c>
       <c r="N16" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="O16">
+        <f>_xlfn.STDEV.P(K19:K50)</f>
+        <v>28.351018913568169</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <f>AVERAGE(B50:B81)</f>
-        <v>44.65625</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>210</v>
-      </c>
-      <c r="L17" t="s">
-        <v>9</v>
+        <f>MEDIAN(B19:B50)</f>
+        <v>54</v>
       </c>
       <c r="N17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O17">
-        <f>AVERAGE(K50:K81)</f>
-        <v>39.125</v>
+        <f>MEDIAN(K19:K50)</f>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18">
-        <f>_xlfn.STDEV.P(B50:B81)</f>
-        <v>48.476546761681568</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18">
-        <v>122</v>
-      </c>
-      <c r="L18" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18" t="s">
-        <v>16</v>
-      </c>
-      <c r="O18">
-        <f>_xlfn.STDEV.P(K50:K81)</f>
-        <v>50.16332699293379</v>
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B19">
-        <v>36</v>
+        <v>3974</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19">
-        <f>MEDIAN(B50:B81)</f>
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>96</v>
+        <v>248</v>
       </c>
       <c r="L19" t="s">
         <v>9</v>
       </c>
       <c r="N19" t="s">
-        <v>20</v>
-      </c>
-      <c r="O19">
-        <f>MEDIAN(K50:K81)</f>
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <f>AVERAGE(B53:B84)</f>
+        <v>44.65625</v>
+      </c>
       <c r="J20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="L20" t="s">
         <v>9</v>
+      </c>
+      <c r="N20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20">
+        <f>AVERAGE(K53:K84)</f>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <f>_xlfn.STDEV.P(B53:B84)</f>
+        <v>48.476546761681568</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K21">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="L21" t="s">
         <v>9</v>
       </c>
       <c r="N21" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="O21">
+        <f>_xlfn.STDEV.P(K53:K84)</f>
+        <v>64.919180524710882</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F22">
-        <f>AVERAGE(B84:B115)</f>
-        <v>28.09375</v>
+        <f>MEDIAN(B53:B84)</f>
+        <v>31</v>
       </c>
       <c r="J22">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K22">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="L22" t="s">
         <v>9</v>
       </c>
       <c r="N22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O22">
-        <f>AVERAGE(K84:K115)</f>
-        <v>22.96875</v>
+        <f>MEDIAN(K53:K84)</f>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23">
-        <f>_xlfn.STDEV.P(B84:B115)</f>
-        <v>7.759507776753626</v>
-      </c>
       <c r="J23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K23">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="L23" t="s">
         <v>9</v>
-      </c>
-      <c r="N23" t="s">
-        <v>16</v>
-      </c>
-      <c r="O23">
-        <f>_xlfn.STDEV.P(K84:K115)</f>
-        <v>3.7789249049828975</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <f>MEDIAN(B84:B115)</f>
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J24">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K24">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="L24" t="s">
         <v>9</v>
       </c>
       <c r="N24" t="s">
-        <v>20</v>
-      </c>
-      <c r="O24">
-        <f>MEDIAN(K84:K115)</f>
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f>AVERAGE(B87:B118)</f>
+        <v>28.09375</v>
+      </c>
       <c r="J25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K25">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="L25" t="s">
         <v>9</v>
+      </c>
+      <c r="N25" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25">
+        <f>AVERAGE(K87:K118)</f>
+        <v>24.9375</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B26">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <f>_xlfn.STDEV.P(B87:B118)</f>
+        <v>7.759507776753626</v>
       </c>
       <c r="J26">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K26">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="L26" t="s">
         <v>9</v>
       </c>
       <c r="N26" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="O26">
+        <f>_xlfn.STDEV.P(K87:K118)</f>
+        <v>5.6950499339338547</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F27">
-        <f>AVERAGE(B118:B149)</f>
-        <v>74.46875</v>
+        <f>MEDIAN(B87:B118)</f>
+        <v>26</v>
       </c>
       <c r="J27">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K27">
         <v>112</v>
@@ -968,156 +913,176 @@
         <v>9</v>
       </c>
       <c r="N27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O27">
-        <f>AVERAGE(K118:K149)</f>
-        <v>30.3125</v>
+        <f>MEDIAN(K87:K118)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28">
-        <f>_xlfn.STDEV.P(B118:B149)</f>
-        <v>188.87925779036061</v>
-      </c>
       <c r="J28">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K28">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L28" t="s">
         <v>9</v>
-      </c>
-      <c r="N28" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28">
-        <f>_xlfn.STDEV.P(K118:K149)</f>
-        <v>22.378054959044139</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B29">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29">
-        <f>MEDIAN(B118:B149)</f>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J29">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K29">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L29" t="s">
         <v>9</v>
       </c>
       <c r="N29" t="s">
-        <v>20</v>
-      </c>
-      <c r="O29">
-        <f>MEDIAN(K118:K149)</f>
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B30">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
       </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <f>AVERAGE(B121:B152)</f>
+        <v>74.46875</v>
+      </c>
       <c r="J30">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K30">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="L30" t="s">
         <v>9</v>
+      </c>
+      <c r="N30" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30">
+        <f>AVERAGE(K121:K152)</f>
+        <v>109.90625</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <f>_xlfn.STDEV.P(B121:B152)</f>
+        <v>188.87925779036061</v>
+      </c>
       <c r="J31">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K31">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="L31" t="s">
         <v>9</v>
+      </c>
+      <c r="N31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31">
+        <f>_xlfn.STDEV.P(K121:K152)</f>
+        <v>36.83439236552573</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B32">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
       </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <f>MEDIAN(B121:B152)</f>
+        <v>34</v>
+      </c>
       <c r="J32">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K32">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="L32" t="s">
         <v>9</v>
+      </c>
+      <c r="N32" t="s">
+        <v>20</v>
+      </c>
+      <c r="O32">
+        <f>MEDIAN(K121:K152)</f>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B33">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
       </c>
       <c r="J33">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K33">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="L33" t="s">
         <v>9</v>
@@ -1125,19 +1090,19 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="J34">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K34">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="L34" t="s">
         <v>9</v>
@@ -1145,19 +1110,19 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B35">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="J35">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K35">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="L35" t="s">
         <v>9</v>
@@ -1165,19 +1130,19 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
       </c>
       <c r="J36">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K36">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="L36" t="s">
         <v>9</v>
@@ -1185,19 +1150,19 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B37">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
       </c>
       <c r="J37">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K37">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="L37" t="s">
         <v>9</v>
@@ -1205,19 +1170,19 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B38">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
       </c>
       <c r="J38">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K38">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="L38" t="s">
         <v>9</v>
@@ -1225,19 +1190,19 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B39">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
       <c r="J39">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K39">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L39" t="s">
         <v>9</v>
@@ -1245,19 +1210,19 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B40">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
       </c>
       <c r="J40">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K40">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="L40" t="s">
         <v>9</v>
@@ -1265,19 +1230,19 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B41">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="J41">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K41">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="L41" t="s">
         <v>9</v>
@@ -1285,19 +1250,19 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B42">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
       </c>
       <c r="J42">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K42">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="L42" t="s">
         <v>9</v>
@@ -1305,19 +1270,19 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B43">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="J43">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K43">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L43" t="s">
         <v>9</v>
@@ -1325,19 +1290,19 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B44">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
       <c r="J44">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K44">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="L44" t="s">
         <v>9</v>
@@ -1345,19 +1310,19 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B45">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
       </c>
       <c r="J45">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K45">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="L45" t="s">
         <v>9</v>
@@ -1365,19 +1330,19 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B46">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
       <c r="J46">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K46">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L46" t="s">
         <v>9</v>
@@ -1385,107 +1350,107 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B47">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
       </c>
       <c r="J47">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K47">
+        <v>167</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>29</v>
+      </c>
+      <c r="B48">
+        <v>86</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <v>29</v>
+      </c>
+      <c r="K48">
+        <v>121</v>
+      </c>
+      <c r="L48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>30</v>
+      </c>
+      <c r="B49">
         <v>103</v>
       </c>
-      <c r="L47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>12</v>
-      </c>
-      <c r="J49" t="s">
-        <v>12</v>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <v>30</v>
+      </c>
+      <c r="K49">
+        <v>126</v>
+      </c>
+      <c r="L49" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B50">
-        <v>303</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K50">
-        <v>317</v>
+        <v>127</v>
       </c>
       <c r="L50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51">
-        <v>27</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-      <c r="K51">
-        <v>31</v>
-      </c>
-      <c r="L51" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="B52">
-        <v>33</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="J52">
-        <v>2</v>
-      </c>
-      <c r="K52">
-        <v>32</v>
-      </c>
-      <c r="L52" t="s">
-        <v>9</v>
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="J52" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B53">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
       </c>
       <c r="J53">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
@@ -1493,19 +1458,19 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B54">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
       </c>
       <c r="J54">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K54">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="L54" t="s">
         <v>9</v>
@@ -1513,19 +1478,19 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B55">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
       </c>
       <c r="J55">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K55">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
@@ -1533,19 +1498,19 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B56">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
       </c>
       <c r="J56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K56">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="L56" t="s">
         <v>9</v>
@@ -1553,19 +1518,19 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B57">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
       </c>
       <c r="J57">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K57">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="L57" t="s">
         <v>9</v>
@@ -1573,7 +1538,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B58">
         <v>28</v>
@@ -1582,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="J58">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K58">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -1593,19 +1558,19 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B59">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="J59">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K59">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -1613,19 +1578,19 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B60">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
       </c>
       <c r="J60">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K60">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="L60" t="s">
         <v>9</v>
@@ -1633,7 +1598,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B61">
         <v>28</v>
@@ -1642,10 +1607,10 @@
         <v>9</v>
       </c>
       <c r="J61">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K61">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="L61" t="s">
         <v>9</v>
@@ -1653,7 +1618,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B62">
         <v>30</v>
@@ -1662,10 +1627,10 @@
         <v>9</v>
       </c>
       <c r="J62">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K62">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="L62" t="s">
         <v>9</v>
@@ -1673,19 +1638,19 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B63">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
       </c>
       <c r="J63">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K63">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="L63" t="s">
         <v>9</v>
@@ -1693,19 +1658,19 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B64">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
       </c>
       <c r="J64">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K64">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="L64" t="s">
         <v>9</v>
@@ -1713,19 +1678,19 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B65">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
       </c>
       <c r="J65">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K65">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="L65" t="s">
         <v>9</v>
@@ -1733,19 +1698,19 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B66">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
       </c>
       <c r="J66">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K66">
-        <v>30</v>
+        <v>129</v>
       </c>
       <c r="L66" t="s">
         <v>9</v>
@@ -1753,19 +1718,19 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B67">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
       </c>
       <c r="J67">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K67">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="L67" t="s">
         <v>9</v>
@@ -1773,19 +1738,19 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B68">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="J68">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K68">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
@@ -1793,19 +1758,19 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B69">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
       </c>
       <c r="J69">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K69">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="L69" t="s">
         <v>9</v>
@@ -1813,19 +1778,19 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B70">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
       </c>
       <c r="J70">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K70">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="L70" t="s">
         <v>9</v>
@@ -1833,19 +1798,19 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B71">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
       </c>
       <c r="J71">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K71">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="L71" t="s">
         <v>9</v>
@@ -1853,19 +1818,19 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B72">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
       </c>
       <c r="J72">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K72">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="L72" t="s">
         <v>9</v>
@@ -1873,19 +1838,19 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B73">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
       </c>
       <c r="J73">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K73">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="L73" t="s">
         <v>9</v>
@@ -1893,19 +1858,19 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B74">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
       </c>
       <c r="J74">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K74">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="L74" t="s">
         <v>9</v>
@@ -1913,19 +1878,19 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B75">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
       </c>
       <c r="J75">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K75">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="L75" t="s">
         <v>9</v>
@@ -1933,19 +1898,19 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B76">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
       </c>
       <c r="J76">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K76">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="L76" t="s">
         <v>9</v>
@@ -1953,19 +1918,19 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B77">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
       </c>
       <c r="J77">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K77">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="L77" t="s">
         <v>9</v>
@@ -1973,19 +1938,19 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B78">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C78" t="s">
         <v>9</v>
       </c>
       <c r="J78">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K78">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="L78" t="s">
         <v>9</v>
@@ -1993,19 +1958,19 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B79">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
       </c>
       <c r="J79">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K79">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="L79" t="s">
         <v>9</v>
@@ -2013,19 +1978,19 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B80">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
       </c>
       <c r="J80">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K80">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="L80" t="s">
         <v>9</v>
@@ -2033,107 +1998,107 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B81">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C81" t="s">
         <v>9</v>
       </c>
       <c r="J81">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K81">
+        <v>87</v>
+      </c>
+      <c r="L81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>29</v>
+      </c>
+      <c r="B82">
+        <v>27</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="J82">
+        <v>29</v>
+      </c>
+      <c r="K82">
+        <v>89</v>
+      </c>
+      <c r="L82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>30</v>
+      </c>
+      <c r="B83">
         <v>28</v>
       </c>
-      <c r="L81" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>13</v>
-      </c>
-      <c r="J83" t="s">
-        <v>13</v>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="J83">
+        <v>30</v>
+      </c>
+      <c r="K83">
+        <v>131</v>
+      </c>
+      <c r="L83" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
       </c>
       <c r="J84">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K84">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="L84" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>1</v>
-      </c>
-      <c r="B85">
-        <v>23</v>
-      </c>
-      <c r="C85" t="s">
-        <v>9</v>
-      </c>
-      <c r="J85">
-        <v>1</v>
-      </c>
-      <c r="K85">
-        <v>23</v>
-      </c>
-      <c r="L85" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <v>2</v>
-      </c>
-      <c r="B86">
-        <v>28</v>
-      </c>
-      <c r="C86" t="s">
-        <v>9</v>
-      </c>
-      <c r="J86">
-        <v>2</v>
-      </c>
-      <c r="K86">
-        <v>23</v>
-      </c>
-      <c r="L86" t="s">
-        <v>9</v>
+      <c r="A86" t="s">
+        <v>13</v>
+      </c>
+      <c r="J86" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B87">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
       </c>
       <c r="J87">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K87">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L87" t="s">
         <v>9</v>
@@ -2141,19 +2106,19 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B88">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="J88">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K88">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L88" t="s">
         <v>9</v>
@@ -2161,19 +2126,19 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B89">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C89" t="s">
         <v>9</v>
       </c>
       <c r="J89">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K89">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L89" t="s">
         <v>9</v>
@@ -2181,16 +2146,16 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B90">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
       </c>
       <c r="J90">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K90">
         <v>25</v>
@@ -2201,19 +2166,19 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B91">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
       </c>
       <c r="J91">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K91">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L91" t="s">
         <v>9</v>
@@ -2221,7 +2186,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B92">
         <v>25</v>
@@ -2230,7 +2195,7 @@
         <v>9</v>
       </c>
       <c r="J92">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K92">
         <v>21</v>
@@ -2241,19 +2206,19 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B93">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
       </c>
       <c r="J93">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K93">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L93" t="s">
         <v>9</v>
@@ -2261,19 +2226,19 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B94">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C94" t="s">
         <v>9</v>
       </c>
       <c r="J94">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K94">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="L94" t="s">
         <v>9</v>
@@ -2281,19 +2246,19 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B95">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C95" t="s">
         <v>9</v>
       </c>
       <c r="J95">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K95">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L95" t="s">
         <v>9</v>
@@ -2301,19 +2266,19 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B96">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
       </c>
       <c r="J96">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K96">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="L96" t="s">
         <v>9</v>
@@ -2321,19 +2286,19 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B97">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
       </c>
       <c r="J97">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K97">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L97" t="s">
         <v>9</v>
@@ -2341,7 +2306,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B98">
         <v>21</v>
@@ -2350,10 +2315,10 @@
         <v>9</v>
       </c>
       <c r="J98">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K98">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L98" t="s">
         <v>9</v>
@@ -2361,19 +2326,19 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B99">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="J99">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K99">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="L99" t="s">
         <v>9</v>
@@ -2381,19 +2346,19 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B100">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
       </c>
       <c r="J100">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K100">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="L100" t="s">
         <v>9</v>
@@ -2401,19 +2366,19 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B101">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
       </c>
       <c r="J101">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K101">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L101" t="s">
         <v>9</v>
@@ -2421,19 +2386,19 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B102">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
       </c>
       <c r="J102">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K102">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L102" t="s">
         <v>9</v>
@@ -2441,19 +2406,19 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B103">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
       </c>
       <c r="J103">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K103">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L103" t="s">
         <v>9</v>
@@ -2461,19 +2426,19 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B104">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C104" t="s">
         <v>9</v>
       </c>
       <c r="J104">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K104">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L104" t="s">
         <v>9</v>
@@ -2481,19 +2446,19 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B105">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
       </c>
       <c r="J105">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K105">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L105" t="s">
         <v>9</v>
@@ -2501,19 +2466,19 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B106">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
       </c>
       <c r="J106">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K106">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L106" t="s">
         <v>9</v>
@@ -2521,16 +2486,16 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B107">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
       </c>
       <c r="J107">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K107">
         <v>21</v>
@@ -2541,19 +2506,19 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B108">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
       </c>
       <c r="J108">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K108">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L108" t="s">
         <v>9</v>
@@ -2561,19 +2526,19 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B109">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
       </c>
       <c r="J109">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K109">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="L109" t="s">
         <v>9</v>
@@ -2581,19 +2546,19 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B110">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
       </c>
       <c r="J110">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K110">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L110" t="s">
         <v>9</v>
@@ -2601,19 +2566,19 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B111">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
       </c>
       <c r="J111">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K111">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L111" t="s">
         <v>9</v>
@@ -2621,19 +2586,19 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B112">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
       </c>
       <c r="J112">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K112">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="L112" t="s">
         <v>9</v>
@@ -2641,19 +2606,19 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B113">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
       </c>
       <c r="J113">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K113">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L113" t="s">
         <v>9</v>
@@ -2661,19 +2626,19 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B114">
+        <v>34</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="J114">
+        <v>27</v>
+      </c>
+      <c r="K114">
         <v>22</v>
-      </c>
-      <c r="C114" t="s">
-        <v>9</v>
-      </c>
-      <c r="J114">
-        <v>30</v>
-      </c>
-      <c r="K114">
-        <v>21</v>
       </c>
       <c r="L114" t="s">
         <v>9</v>
@@ -2681,107 +2646,104 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B115">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
       </c>
       <c r="J115">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K115">
+        <v>25</v>
+      </c>
+      <c r="L115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>29</v>
+      </c>
+      <c r="B116">
+        <v>20</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="J116">
+        <v>29</v>
+      </c>
+      <c r="K116">
+        <v>23</v>
+      </c>
+      <c r="L116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>30</v>
+      </c>
+      <c r="B117">
         <v>22</v>
       </c>
-      <c r="L115" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>14</v>
-      </c>
-      <c r="J117" t="s">
-        <v>14</v>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="J117">
+        <v>30</v>
+      </c>
+      <c r="K117">
+        <v>23</v>
+      </c>
+      <c r="L117" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B118">
-        <v>186</v>
+        <v>21</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
       </c>
       <c r="J118">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K118">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="L118" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>1</v>
-      </c>
-      <c r="B119">
-        <v>34</v>
-      </c>
-      <c r="C119" t="s">
-        <v>9</v>
-      </c>
-      <c r="J119">
-        <v>1</v>
-      </c>
-      <c r="K119">
-        <v>32</v>
-      </c>
-      <c r="L119" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <v>2</v>
-      </c>
-      <c r="B120">
-        <v>34</v>
-      </c>
-      <c r="C120" t="s">
-        <v>9</v>
-      </c>
-      <c r="J120">
-        <v>2</v>
-      </c>
-      <c r="K120">
-        <v>26</v>
-      </c>
-      <c r="L120" t="s">
-        <v>9</v>
+      <c r="A120" t="s">
+        <v>14</v>
+      </c>
+      <c r="J120" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B121">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
       </c>
-      <c r="J121">
-        <v>3</v>
-      </c>
       <c r="K121">
-        <v>26</v>
+        <v>305</v>
       </c>
       <c r="L121" t="s">
         <v>9</v>
@@ -2789,19 +2751,19 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B122">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C122" t="s">
         <v>9</v>
       </c>
       <c r="J122">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K122">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="L122" t="s">
         <v>9</v>
@@ -2809,19 +2771,19 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B123">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
       </c>
       <c r="J123">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K123">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="L123" t="s">
         <v>9</v>
@@ -2829,19 +2791,19 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B124">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C124" t="s">
         <v>9</v>
       </c>
       <c r="J124">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K124">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="L124" t="s">
         <v>9</v>
@@ -2849,19 +2811,19 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B125">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
       </c>
       <c r="J125">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K125">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="L125" t="s">
         <v>9</v>
@@ -2869,7 +2831,7 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B126">
         <v>28</v>
@@ -2878,10 +2840,10 @@
         <v>9</v>
       </c>
       <c r="J126">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K126">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="L126" t="s">
         <v>9</v>
@@ -2889,19 +2851,19 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B127">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
       </c>
       <c r="J127">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K127">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="L127" t="s">
         <v>9</v>
@@ -2909,19 +2871,19 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B128">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
       </c>
       <c r="J128">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K128">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="L128" t="s">
         <v>9</v>
@@ -2929,7 +2891,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B129">
         <v>28</v>
@@ -2938,10 +2900,10 @@
         <v>9</v>
       </c>
       <c r="J129">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K129">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="L129" t="s">
         <v>9</v>
@@ -2949,19 +2911,19 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B130">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
       </c>
       <c r="J130">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K130">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="L130" t="s">
         <v>9</v>
@@ -2969,19 +2931,19 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B131">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
       </c>
       <c r="J131">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K131">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="L131" t="s">
         <v>9</v>
@@ -2989,19 +2951,19 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B132">
-        <v>1114</v>
+        <v>28</v>
       </c>
       <c r="C132" t="s">
         <v>9</v>
       </c>
       <c r="J132">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K132">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="L132" t="s">
         <v>9</v>
@@ -3009,19 +2971,19 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B133">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
       </c>
       <c r="J133">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K133">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="L133" t="s">
         <v>9</v>
@@ -3029,19 +2991,19 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B134">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
       </c>
       <c r="J134">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K134">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="L134" t="s">
         <v>9</v>
@@ -3049,19 +3011,19 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B135">
-        <v>30</v>
+        <v>1114</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
       </c>
       <c r="J135">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K135">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="L135" t="s">
         <v>9</v>
@@ -3069,19 +3031,19 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B136">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
       </c>
       <c r="J136">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K136">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="L136" t="s">
         <v>9</v>
@@ -3089,19 +3051,19 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B137">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
       </c>
       <c r="J137">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K137">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="L137" t="s">
         <v>9</v>
@@ -3109,19 +3071,19 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B138">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
       </c>
       <c r="J138">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K138">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="L138" t="s">
         <v>9</v>
@@ -3129,19 +3091,19 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B139">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
       </c>
       <c r="J139">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K139">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="L139" t="s">
         <v>9</v>
@@ -3149,19 +3111,19 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B140">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
       </c>
       <c r="J140">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K140">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="L140" t="s">
         <v>9</v>
@@ -3169,19 +3131,19 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B141">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
       </c>
       <c r="J141">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K141">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="L141" t="s">
         <v>9</v>
@@ -3189,19 +3151,19 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B142">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
       </c>
       <c r="J142">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K142">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="L142" t="s">
         <v>9</v>
@@ -3209,7 +3171,7 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B143">
         <v>43</v>
@@ -3218,10 +3180,10 @@
         <v>9</v>
       </c>
       <c r="J143">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K143">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="L143" t="s">
         <v>9</v>
@@ -3229,19 +3191,19 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B144">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
       </c>
       <c r="J144">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K144">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="L144" t="s">
         <v>9</v>
@@ -3249,19 +3211,19 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B145">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
       </c>
       <c r="J145">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K145">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="L145" t="s">
         <v>9</v>
@@ -3269,19 +3231,19 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B146">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
       </c>
       <c r="J146">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K146">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="L146" t="s">
         <v>9</v>
@@ -3289,19 +3251,19 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B147">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
       </c>
       <c r="J147">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K147">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="L147" t="s">
         <v>9</v>
@@ -3309,19 +3271,19 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B148">
+        <v>42</v>
+      </c>
+      <c r="C148" t="s">
+        <v>9</v>
+      </c>
+      <c r="J148">
         <v>27</v>
       </c>
-      <c r="C148" t="s">
-        <v>9</v>
-      </c>
-      <c r="J148">
-        <v>30</v>
-      </c>
       <c r="K148">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="L148" t="s">
         <v>9</v>
@@ -3329,27 +3291,87 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149">
+        <v>28</v>
+      </c>
+      <c r="B149">
+        <v>37</v>
+      </c>
+      <c r="C149" t="s">
+        <v>9</v>
+      </c>
+      <c r="J149">
+        <v>28</v>
+      </c>
+      <c r="K149">
+        <v>96</v>
+      </c>
+      <c r="L149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>29</v>
+      </c>
+      <c r="B150">
+        <v>24</v>
+      </c>
+      <c r="C150" t="s">
+        <v>9</v>
+      </c>
+      <c r="J150">
+        <v>29</v>
+      </c>
+      <c r="K150">
+        <v>98</v>
+      </c>
+      <c r="L150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>30</v>
+      </c>
+      <c r="B151">
+        <v>27</v>
+      </c>
+      <c r="C151" t="s">
+        <v>9</v>
+      </c>
+      <c r="J151">
+        <v>30</v>
+      </c>
+      <c r="K151">
+        <v>101</v>
+      </c>
+      <c r="L151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A152">
         <v>31</v>
       </c>
-      <c r="B149">
+      <c r="B152">
         <v>25</v>
       </c>
-      <c r="C149" t="s">
-        <v>9</v>
-      </c>
-      <c r="J149">
+      <c r="C152" t="s">
+        <v>9</v>
+      </c>
+      <c r="J152">
         <v>31</v>
       </c>
-      <c r="K149">
-        <v>30</v>
-      </c>
-      <c r="L149" t="s">
+      <c r="K152">
+        <v>115</v>
+      </c>
+      <c r="L152" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="G28:G59">
-    <sortCondition ref="G28"/>
+  <sortState ref="G31:G62">
+    <sortCondition ref="G31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ahem.  Now PROPERLY profiling my optimizations.  Still not really noticeable.
I was still copying data back to the "check" buffers in the sorting
loop.  Whoops.  Disabled that and it ran faster.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="23">
   <si>
     <t>State</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>total sort time</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
 </sst>
 </file>
@@ -459,13 +456,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -487,7 +484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -495,7 +492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -503,7 +500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -511,17 +508,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -529,9 +526,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>23</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>145615</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
       </c>
       <c r="J10">
         <v>1478367</v>
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -548,9 +548,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12714</v>
+        <v>9179</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -562,85 +562,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15">
-        <f>AVERAGE(B19:B50)</f>
-        <v>187.28125</v>
-      </c>
       <c r="J15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15">
-        <f>AVERAGE(K19:K50)</f>
-        <v>122.96875</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1108570</v>
+        <v>1105355</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16">
-        <f>_xlfn.STDEV.P(B19:B50)</f>
-        <v>680.80376368557006</v>
       </c>
       <c r="J16">
         <v>905057</v>
       </c>
       <c r="K16" t="s">
         <v>9</v>
-      </c>
-      <c r="N16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16">
-        <f>_xlfn.STDEV.P(K19:K50)</f>
-        <v>28.351018913568169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17">
-        <f>MEDIAN(B19:B50)</f>
-        <v>54</v>
-      </c>
-      <c r="N17" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17">
-        <f>MEDIAN(K19:K50)</f>
-        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
       <c r="J18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -649,13 +603,17 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>3974</v>
+        <v>6774</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <f>AVERAGE(B19:B50)</f>
+        <v>322</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -667,7 +625,11 @@
         <v>9</v>
       </c>
       <c r="N19" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(K19:K50)</f>
+        <v>122.96875</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -675,17 +637,17 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F20">
-        <f>AVERAGE(B53:B84)</f>
-        <v>44.65625</v>
+        <f>_xlfn.STDEV.P(B19:B50)</f>
+        <v>1161.360893521045</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -697,11 +659,11 @@
         <v>9</v>
       </c>
       <c r="N20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O20">
-        <f>AVERAGE(K53:K84)</f>
-        <v>106</v>
+        <f>_xlfn.STDEV.P(K19:K50)</f>
+        <v>28.351018913568169</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -709,17 +671,17 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F21">
-        <f>_xlfn.STDEV.P(B53:B84)</f>
-        <v>48.476546761681568</v>
+        <f>MEDIAN(B19:B50)</f>
+        <v>118</v>
       </c>
       <c r="J21">
         <v>2</v>
@@ -731,11 +693,11 @@
         <v>9</v>
       </c>
       <c r="N21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O21">
-        <f>_xlfn.STDEV.P(K53:K84)</f>
-        <v>64.919180524710882</v>
+        <f>MEDIAN(K19:K50)</f>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -748,13 +710,6 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22">
-        <f>MEDIAN(B53:B84)</f>
-        <v>31</v>
-      </c>
       <c r="J22">
         <v>3</v>
       </c>
@@ -763,13 +718,6 @@
       </c>
       <c r="L22" t="s">
         <v>9</v>
-      </c>
-      <c r="N22" t="s">
-        <v>20</v>
-      </c>
-      <c r="O22">
-        <f>MEDIAN(K53:K84)</f>
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -782,6 +730,9 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
       <c r="J23">
         <v>4</v>
       </c>
@@ -790,6 +741,9 @@
       </c>
       <c r="L23" t="s">
         <v>9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -803,7 +757,11 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <f>AVERAGE(B53:B84)</f>
+        <v>73.40625</v>
       </c>
       <c r="J24">
         <v>5</v>
@@ -815,7 +773,11 @@
         <v>9</v>
       </c>
       <c r="N24" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="O24">
+        <f>AVERAGE(K53:K84)</f>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -823,17 +785,17 @@
         <v>6</v>
       </c>
       <c r="B25">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <f>AVERAGE(B87:B118)</f>
-        <v>28.09375</v>
+        <f>_xlfn.STDEV.P(B53:B84)</f>
+        <v>51.786134350205174</v>
       </c>
       <c r="J25">
         <v>6</v>
@@ -845,11 +807,11 @@
         <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O25">
-        <f>AVERAGE(K87:K118)</f>
-        <v>24.9375</v>
+        <f>_xlfn.STDEV.P(K53:K84)</f>
+        <v>64.919180524710882</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -857,17 +819,17 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F26">
-        <f>_xlfn.STDEV.P(B87:B118)</f>
-        <v>7.759507776753626</v>
+        <f>MEDIAN(B53:B84)</f>
+        <v>78</v>
       </c>
       <c r="J26">
         <v>7</v>
@@ -879,11 +841,11 @@
         <v>9</v>
       </c>
       <c r="N26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O26">
-        <f>_xlfn.STDEV.P(K87:K118)</f>
-        <v>5.6950499339338547</v>
+        <f>MEDIAN(K53:K84)</f>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -891,17 +853,10 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27">
-        <f>MEDIAN(B87:B118)</f>
-        <v>26</v>
       </c>
       <c r="J27">
         <v>8</v>
@@ -912,23 +867,19 @@
       <c r="L27" t="s">
         <v>9</v>
       </c>
-      <c r="N27" t="s">
-        <v>20</v>
-      </c>
-      <c r="O27">
-        <f>MEDIAN(K87:K118)</f>
-        <v>23</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
       <c r="B28">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
       </c>
       <c r="J28">
         <v>9</v>
@@ -938,6 +889,9 @@
       </c>
       <c r="L28" t="s">
         <v>9</v>
+      </c>
+      <c r="N28" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -945,13 +899,17 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(B87:B118)</f>
+        <v>54.4375</v>
       </c>
       <c r="J29">
         <v>10</v>
@@ -963,7 +921,11 @@
         <v>9</v>
       </c>
       <c r="N29" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="O29">
+        <f>AVERAGE(K87:K118)</f>
+        <v>24.9375</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -971,17 +933,17 @@
         <v>11</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30">
-        <f>AVERAGE(B121:B152)</f>
-        <v>74.46875</v>
+        <f>_xlfn.STDEV.P(B87:B118)</f>
+        <v>27.960840362013442</v>
       </c>
       <c r="J30">
         <v>11</v>
@@ -993,11 +955,11 @@
         <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O30">
-        <f>AVERAGE(K121:K152)</f>
-        <v>109.90625</v>
+        <f>_xlfn.STDEV.P(K87:K118)</f>
+        <v>5.6950499339338547</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1005,17 +967,17 @@
         <v>12</v>
       </c>
       <c r="B31">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F31">
-        <f>_xlfn.STDEV.P(B121:B152)</f>
-        <v>188.87925779036061</v>
+        <f>MEDIAN(B87:B118)</f>
+        <v>63</v>
       </c>
       <c r="J31">
         <v>12</v>
@@ -1027,11 +989,11 @@
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O31">
-        <f>_xlfn.STDEV.P(K121:K152)</f>
-        <v>36.83439236552573</v>
+        <f>MEDIAN(K87:K118)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -1039,17 +1001,10 @@
         <v>13</v>
       </c>
       <c r="B32">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32">
-        <f>MEDIAN(B121:B152)</f>
-        <v>34</v>
       </c>
       <c r="J32">
         <v>13</v>
@@ -1060,100 +1015,141 @@
       <c r="L32" t="s">
         <v>9</v>
       </c>
-      <c r="N32" t="s">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>228</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33">
+        <v>114</v>
+      </c>
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>323</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <f>AVERAGE(B121:B152)</f>
+        <v>150.28125</v>
+      </c>
+      <c r="J34">
+        <v>15</v>
+      </c>
+      <c r="K34">
+        <v>106</v>
+      </c>
+      <c r="L34" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" t="s">
+        <v>15</v>
+      </c>
+      <c r="O34">
+        <f>AVERAGE(K121:K152)</f>
+        <v>109.90625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35">
+        <f>_xlfn.STDEV.P(B121:B152)</f>
+        <v>456.18172327312448</v>
+      </c>
+      <c r="J35">
+        <v>16</v>
+      </c>
+      <c r="K35">
+        <v>115</v>
+      </c>
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" t="s">
+        <v>16</v>
+      </c>
+      <c r="O35">
+        <f>_xlfn.STDEV.P(K121:K152)</f>
+        <v>36.83439236552573</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>119</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
         <v>20</v>
       </c>
-      <c r="O32">
+      <c r="F36">
+        <f>MEDIAN(B121:B152)</f>
+        <v>75.5</v>
+      </c>
+      <c r="J36">
+        <v>17</v>
+      </c>
+      <c r="K36">
+        <v>122</v>
+      </c>
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36">
         <f>MEDIAN(K121:K152)</f>
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>14</v>
-      </c>
-      <c r="B33">
-        <v>83</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33">
-        <v>14</v>
-      </c>
-      <c r="K33">
-        <v>114</v>
-      </c>
-      <c r="L33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>15</v>
-      </c>
-      <c r="B34">
-        <v>134</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34">
-        <v>15</v>
-      </c>
-      <c r="K34">
-        <v>106</v>
-      </c>
-      <c r="L34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>16</v>
-      </c>
-      <c r="B35">
-        <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35">
-        <v>16</v>
-      </c>
-      <c r="K35">
-        <v>115</v>
-      </c>
-      <c r="L35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>17</v>
-      </c>
-      <c r="B36">
-        <v>45</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36">
-        <v>17</v>
-      </c>
-      <c r="K36">
-        <v>122</v>
-      </c>
-      <c r="L36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>18</v>
       </c>
       <c r="B37">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -1168,12 +1164,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>19</v>
       </c>
       <c r="B38">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -1188,12 +1184,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1208,12 +1204,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21</v>
       </c>
       <c r="B40">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1228,12 +1224,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22</v>
       </c>
       <c r="B41">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -1248,12 +1244,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>23</v>
       </c>
       <c r="B42">
-        <v>100</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1268,12 +1264,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>24</v>
       </c>
       <c r="B43">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -1288,12 +1284,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>25</v>
       </c>
       <c r="B44">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1308,12 +1304,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>26</v>
       </c>
       <c r="B45">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1328,12 +1324,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>27</v>
       </c>
       <c r="B46">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1348,12 +1344,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>28</v>
       </c>
       <c r="B47">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -1368,12 +1364,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>29</v>
       </c>
       <c r="B48">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1393,7 +1389,7 @@
         <v>30</v>
       </c>
       <c r="B49">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1413,7 +1409,7 @@
         <v>31</v>
       </c>
       <c r="B50">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
@@ -1441,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="B53">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -1461,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="B54">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
@@ -1481,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="B55">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -1501,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="B56">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -1541,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -1561,7 +1557,7 @@
         <v>6</v>
       </c>
       <c r="B59">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -1581,7 +1577,7 @@
         <v>7</v>
       </c>
       <c r="B60">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -1641,7 +1637,7 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -1681,7 +1677,7 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -1701,7 +1697,7 @@
         <v>13</v>
       </c>
       <c r="B66">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -1721,7 +1717,7 @@
         <v>14</v>
       </c>
       <c r="B67">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
@@ -1741,7 +1737,7 @@
         <v>15</v>
       </c>
       <c r="B68">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
@@ -1761,7 +1757,7 @@
         <v>16</v>
       </c>
       <c r="B69">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -1781,7 +1777,7 @@
         <v>17</v>
       </c>
       <c r="B70">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
@@ -1801,7 +1797,7 @@
         <v>18</v>
       </c>
       <c r="B71">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -1821,7 +1817,7 @@
         <v>19</v>
       </c>
       <c r="B72">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -1841,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B73">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
@@ -1861,7 +1857,7 @@
         <v>21</v>
       </c>
       <c r="B74">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -1881,7 +1877,7 @@
         <v>22</v>
       </c>
       <c r="B75">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -1901,7 +1897,7 @@
         <v>23</v>
       </c>
       <c r="B76">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -1921,7 +1917,7 @@
         <v>24</v>
       </c>
       <c r="B77">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -1941,7 +1937,7 @@
         <v>25</v>
       </c>
       <c r="B78">
-        <v>52</v>
+        <v>157</v>
       </c>
       <c r="C78" t="s">
         <v>9</v>
@@ -1961,7 +1957,7 @@
         <v>26</v>
       </c>
       <c r="B79">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -1981,7 +1977,7 @@
         <v>27</v>
       </c>
       <c r="B80">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
@@ -2001,7 +1997,7 @@
         <v>28</v>
       </c>
       <c r="B81">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
         <v>9</v>
@@ -2021,7 +2017,7 @@
         <v>29</v>
       </c>
       <c r="B82">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
@@ -2041,7 +2037,7 @@
         <v>30</v>
       </c>
       <c r="B83">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C83" t="s">
         <v>9</v>
@@ -2061,7 +2057,7 @@
         <v>31</v>
       </c>
       <c r="B84">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -2089,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="B87">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
@@ -2129,7 +2125,7 @@
         <v>2</v>
       </c>
       <c r="B89">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C89" t="s">
         <v>9</v>
@@ -2149,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="B90">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
@@ -2269,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="B96">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
@@ -2289,7 +2285,7 @@
         <v>10</v>
       </c>
       <c r="B97">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
@@ -2309,7 +2305,7 @@
         <v>11</v>
       </c>
       <c r="B98">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C98" t="s">
         <v>9</v>
@@ -2329,7 +2325,7 @@
         <v>12</v>
       </c>
       <c r="B99">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
@@ -2349,7 +2345,7 @@
         <v>13</v>
       </c>
       <c r="B100">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -2369,7 +2365,7 @@
         <v>14</v>
       </c>
       <c r="B101">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C101" t="s">
         <v>9</v>
@@ -2389,7 +2385,7 @@
         <v>15</v>
       </c>
       <c r="B102">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
@@ -2409,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="B103">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
@@ -2429,7 +2425,7 @@
         <v>17</v>
       </c>
       <c r="B104">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C104" t="s">
         <v>9</v>
@@ -2449,7 +2445,7 @@
         <v>18</v>
       </c>
       <c r="B105">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
@@ -2469,7 +2465,7 @@
         <v>19</v>
       </c>
       <c r="B106">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
@@ -2489,7 +2485,7 @@
         <v>20</v>
       </c>
       <c r="B107">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -2509,7 +2505,7 @@
         <v>21</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
@@ -2529,7 +2525,7 @@
         <v>22</v>
       </c>
       <c r="B109">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
@@ -2549,7 +2545,7 @@
         <v>23</v>
       </c>
       <c r="B110">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
@@ -2569,7 +2565,7 @@
         <v>24</v>
       </c>
       <c r="B111">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
@@ -2589,7 +2585,7 @@
         <v>25</v>
       </c>
       <c r="B112">
-        <v>44</v>
+        <v>122</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
@@ -2609,7 +2605,7 @@
         <v>26</v>
       </c>
       <c r="B113">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -2629,7 +2625,7 @@
         <v>27</v>
       </c>
       <c r="B114">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -2649,7 +2645,7 @@
         <v>28</v>
       </c>
       <c r="B115">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -2669,7 +2665,7 @@
         <v>29</v>
       </c>
       <c r="B116">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
@@ -2689,7 +2685,7 @@
         <v>30</v>
       </c>
       <c r="B117">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C117" t="s">
         <v>9</v>
@@ -2709,7 +2705,7 @@
         <v>31</v>
       </c>
       <c r="B118">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -2737,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="B121">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -2754,7 +2750,7 @@
         <v>1</v>
       </c>
       <c r="B122">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C122" t="s">
         <v>9</v>
@@ -2774,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="B123">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
@@ -2794,7 +2790,7 @@
         <v>3</v>
       </c>
       <c r="B124">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C124" t="s">
         <v>9</v>
@@ -2814,7 +2810,7 @@
         <v>4</v>
       </c>
       <c r="B125">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C125" t="s">
         <v>9</v>
@@ -2834,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="B126">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C126" t="s">
         <v>9</v>
@@ -2854,7 +2850,7 @@
         <v>6</v>
       </c>
       <c r="B127">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
@@ -2874,7 +2870,7 @@
         <v>7</v>
       </c>
       <c r="B128">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -2894,7 +2890,7 @@
         <v>8</v>
       </c>
       <c r="B129">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C129" t="s">
         <v>9</v>
@@ -2914,7 +2910,7 @@
         <v>9</v>
       </c>
       <c r="B130">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -2934,7 +2930,7 @@
         <v>10</v>
       </c>
       <c r="B131">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
@@ -2974,7 +2970,7 @@
         <v>12</v>
       </c>
       <c r="B133">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
@@ -2994,7 +2990,7 @@
         <v>13</v>
       </c>
       <c r="B134">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
@@ -3014,7 +3010,7 @@
         <v>14</v>
       </c>
       <c r="B135">
-        <v>1114</v>
+        <v>2682</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -3034,7 +3030,7 @@
         <v>15</v>
       </c>
       <c r="B136">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -3054,7 +3050,7 @@
         <v>16</v>
       </c>
       <c r="B137">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
@@ -3074,7 +3070,7 @@
         <v>17</v>
       </c>
       <c r="B138">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
@@ -3094,7 +3090,7 @@
         <v>18</v>
       </c>
       <c r="B139">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
@@ -3114,7 +3110,7 @@
         <v>19</v>
       </c>
       <c r="B140">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
@@ -3134,7 +3130,7 @@
         <v>20</v>
       </c>
       <c r="B141">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
@@ -3154,7 +3150,7 @@
         <v>21</v>
       </c>
       <c r="B142">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -3174,7 +3170,7 @@
         <v>22</v>
       </c>
       <c r="B143">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
@@ -3194,7 +3190,7 @@
         <v>23</v>
       </c>
       <c r="B144">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
@@ -3214,7 +3210,7 @@
         <v>24</v>
       </c>
       <c r="B145">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
@@ -3234,7 +3230,7 @@
         <v>25</v>
       </c>
       <c r="B146">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
@@ -3254,7 +3250,7 @@
         <v>26</v>
       </c>
       <c r="B147">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
@@ -3274,7 +3270,7 @@
         <v>27</v>
       </c>
       <c r="B148">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -3294,7 +3290,7 @@
         <v>28</v>
       </c>
       <c r="B149">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -3314,7 +3310,7 @@
         <v>29</v>
       </c>
       <c r="B150">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C150" t="s">
         <v>9</v>
@@ -3334,7 +3330,7 @@
         <v>30</v>
       </c>
       <c r="B151">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C151" t="s">
         <v>9</v>
@@ -3354,7 +3350,7 @@
         <v>31</v>
       </c>
       <c r="B152">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="C152" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Figured out how to initialize a shared memory array to 0 without running over other threads' data.
It seems that the declaration of a shared memory array is visible to all
threads in a work group, but the initialization happens per thread.  To
prevent race conditions between giving the array initial values and late
threads running those initial values over with 0, make everyone wait.

Also trying to figure out the memory bank conflict avoidance thing from
the GPU Gems article in chapter 39 that I am following.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="27">
   <si>
     <t>State</t>
   </si>
@@ -92,7 +92,19 @@
     <t>IntermediateData uses a single buffer (don't know why it's a bit slower now, but it's microseconds)</t>
   </si>
   <si>
-    <t>total sort time</t>
+    <t>total</t>
+  </si>
+  <si>
+    <t>total sort time (by std::chrono)</t>
+  </si>
+  <si>
+    <t>total sort time (by sum of parts)</t>
+  </si>
+  <si>
+    <t>??why the difference??</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -456,13 +468,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -484,7 +496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -492,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -500,7 +512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -508,39 +520,59 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>145615</v>
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
+      <c r="D10">
+        <f>SUM(F37,F31,F25,F19)</f>
+        <v>19204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
       <c r="J10">
-        <v>1478367</v>
+        <v>392545</v>
       </c>
       <c r="K10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <f>SUM(O37,O31,O25,O19)</f>
+        <v>6237</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -548,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9179</v>
       </c>
@@ -556,13 +588,13 @@
         <v>9</v>
       </c>
       <c r="J13">
-        <v>3386</v>
+        <v>3798</v>
       </c>
       <c r="K13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -570,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1105355</v>
       </c>
@@ -578,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="J16">
-        <v>905057</v>
+        <v>879025</v>
       </c>
       <c r="K16" t="s">
         <v>9</v>
@@ -609,27 +641,27 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F19">
-        <f>AVERAGE(B19:B50)</f>
-        <v>322</v>
+        <f>SUM(B19:B50)</f>
+        <v>10304</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="L19" t="s">
         <v>9</v>
       </c>
       <c r="N19" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="O19">
-        <f>AVERAGE(K19:K50)</f>
-        <v>122.96875</v>
+        <f>SUM(K19:K50)</f>
+        <v>1359</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -643,27 +675,27 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20">
-        <f>_xlfn.STDEV.P(B19:B50)</f>
-        <v>1161.360893521045</v>
+        <f>AVERAGE(B19:B50)</f>
+        <v>322</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
       <c r="K20">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>9</v>
       </c>
       <c r="N20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O20">
-        <f>_xlfn.STDEV.P(K19:K50)</f>
-        <v>28.351018913568169</v>
+        <f>AVERAGE(K19:K50)</f>
+        <v>42.46875</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -677,27 +709,27 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F21">
-        <f>MEDIAN(B19:B50)</f>
-        <v>118</v>
+        <f>_xlfn.STDEV.P(B19:B50)</f>
+        <v>1161.360893521045</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
       <c r="K21">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L21" t="s">
         <v>9</v>
       </c>
       <c r="N21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O21">
-        <f>MEDIAN(K19:K50)</f>
-        <v>115</v>
+        <f>_xlfn.STDEV.P(K19:K50)</f>
+        <v>49.851018278842609</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -710,14 +742,28 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f>MEDIAN(B19:B50)</f>
+        <v>118</v>
+      </c>
       <c r="J22">
         <v>3</v>
       </c>
       <c r="K22">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="L22" t="s">
         <v>9</v>
+      </c>
+      <c r="N22" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <f>MEDIAN(K19:K50)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -730,20 +776,14 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
       <c r="J23">
         <v>4</v>
       </c>
       <c r="K23">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="L23" t="s">
         <v>9</v>
-      </c>
-      <c r="N23" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -757,27 +797,19 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24">
-        <f>AVERAGE(B53:B84)</f>
-        <v>73.40625</v>
+        <v>12</v>
       </c>
       <c r="J24">
         <v>5</v>
       </c>
       <c r="K24">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="L24" t="s">
         <v>9</v>
       </c>
       <c r="N24" t="s">
-        <v>15</v>
-      </c>
-      <c r="O24">
-        <f>AVERAGE(K53:K84)</f>
-        <v>106</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -791,27 +823,27 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F25">
-        <f>_xlfn.STDEV.P(B53:B84)</f>
-        <v>51.786134350205174</v>
+        <f>SUM(B53:B84)</f>
+        <v>2349</v>
       </c>
       <c r="J25">
         <v>6</v>
       </c>
       <c r="K25">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="L25" t="s">
         <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="O25">
-        <f>_xlfn.STDEV.P(K53:K84)</f>
-        <v>64.919180524710882</v>
+        <f>SUM(K53:K84)</f>
+        <v>1343</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -825,27 +857,27 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F26">
-        <f>MEDIAN(B53:B84)</f>
-        <v>78</v>
+        <f>AVERAGE(B53:B84)</f>
+        <v>73.40625</v>
       </c>
       <c r="J26">
         <v>7</v>
       </c>
       <c r="K26">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="L26" t="s">
         <v>9</v>
       </c>
       <c r="N26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O26">
-        <f>MEDIAN(K53:K84)</f>
-        <v>91</v>
+        <f>AVERAGE(K53:K84)</f>
+        <v>41.96875</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -858,14 +890,28 @@
       <c r="C27" t="s">
         <v>9</v>
       </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <f>_xlfn.STDEV.P(B53:B84)</f>
+        <v>51.786134350205174</v>
+      </c>
       <c r="J27">
         <v>8</v>
       </c>
       <c r="K27">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="L27" t="s">
         <v>9</v>
+      </c>
+      <c r="N27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27">
+        <f>_xlfn.STDEV.P(K53:K84)</f>
+        <v>49.768516890073187</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -879,19 +925,27 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <f>MEDIAN(B53:B84)</f>
+        <v>78</v>
       </c>
       <c r="J28">
         <v>9</v>
       </c>
       <c r="K28">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="L28" t="s">
         <v>9</v>
       </c>
       <c r="N28" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="O28">
+        <f>MEDIAN(K53:K84)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -904,28 +958,14 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29">
-        <f>AVERAGE(B87:B118)</f>
-        <v>54.4375</v>
-      </c>
       <c r="J29">
         <v>10</v>
       </c>
       <c r="K29">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L29" t="s">
         <v>9</v>
-      </c>
-      <c r="N29" t="s">
-        <v>15</v>
-      </c>
-      <c r="O29">
-        <f>AVERAGE(K87:K118)</f>
-        <v>24.9375</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -939,27 +979,19 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30">
-        <f>_xlfn.STDEV.P(B87:B118)</f>
-        <v>27.960840362013442</v>
+        <v>13</v>
       </c>
       <c r="J30">
         <v>11</v>
       </c>
       <c r="K30">
-        <v>144</v>
+        <v>27</v>
       </c>
       <c r="L30" t="s">
         <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30">
-        <f>_xlfn.STDEV.P(K87:K118)</f>
-        <v>5.6950499339338547</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -973,27 +1005,27 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F31">
-        <f>MEDIAN(B87:B118)</f>
-        <v>63</v>
+        <f>SUM(B87:B118)</f>
+        <v>1742</v>
       </c>
       <c r="J31">
         <v>12</v>
       </c>
       <c r="K31">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="L31" t="s">
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O31">
-        <f>MEDIAN(K87:K118)</f>
-        <v>23</v>
+        <f>SUM(K87:K118)</f>
+        <v>866</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -1006,14 +1038,28 @@
       <c r="C32" t="s">
         <v>9</v>
       </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <f>AVERAGE(B87:B118)</f>
+        <v>54.4375</v>
+      </c>
       <c r="J32">
         <v>13</v>
       </c>
       <c r="K32">
-        <v>147</v>
+        <v>35</v>
       </c>
       <c r="L32" t="s">
         <v>9</v>
+      </c>
+      <c r="N32" t="s">
+        <v>15</v>
+      </c>
+      <c r="O32">
+        <f>AVERAGE(K87:K118)</f>
+        <v>27.0625</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -1027,19 +1073,27 @@
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <f>_xlfn.STDEV.P(B87:B118)</f>
+        <v>27.960840362013442</v>
       </c>
       <c r="J33">
         <v>14</v>
       </c>
       <c r="K33">
-        <v>114</v>
+        <v>30</v>
       </c>
       <c r="L33" t="s">
         <v>9</v>
       </c>
       <c r="N33" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="O33">
+        <f>_xlfn.STDEV.P(K87:K118)</f>
+        <v>7.8019929345007739</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -1053,27 +1107,27 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F34">
-        <f>AVERAGE(B121:B152)</f>
-        <v>150.28125</v>
+        <f>MEDIAN(B87:B118)</f>
+        <v>63</v>
       </c>
       <c r="J34">
         <v>15</v>
       </c>
       <c r="K34">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="L34" t="s">
         <v>9</v>
       </c>
       <c r="N34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O34">
-        <f>AVERAGE(K121:K152)</f>
-        <v>109.90625</v>
+        <f>MEDIAN(K87:K118)</f>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -1086,28 +1140,14 @@
       <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="E35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35">
-        <f>_xlfn.STDEV.P(B121:B152)</f>
-        <v>456.18172327312448</v>
-      </c>
       <c r="J35">
         <v>16</v>
       </c>
       <c r="K35">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="L35" t="s">
         <v>9</v>
-      </c>
-      <c r="N35" t="s">
-        <v>16</v>
-      </c>
-      <c r="O35">
-        <f>_xlfn.STDEV.P(K121:K152)</f>
-        <v>36.83439236552573</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -1121,27 +1161,19 @@
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36">
-        <f>MEDIAN(B121:B152)</f>
-        <v>75.5</v>
+        <v>14</v>
       </c>
       <c r="J36">
         <v>17</v>
       </c>
       <c r="K36">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="L36" t="s">
         <v>9</v>
       </c>
       <c r="N36" t="s">
-        <v>20</v>
-      </c>
-      <c r="O36">
-        <f>MEDIAN(K121:K152)</f>
-        <v>101</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -1154,14 +1186,28 @@
       <c r="C37" t="s">
         <v>9</v>
       </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <f>SUM(B121:B152)</f>
+        <v>4809</v>
+      </c>
       <c r="J37">
         <v>18</v>
       </c>
       <c r="K37">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="L37" t="s">
         <v>9</v>
+      </c>
+      <c r="N37" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37">
+        <f>SUM(K121:K152)</f>
+        <v>2669</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -1174,14 +1220,28 @@
       <c r="C38" t="s">
         <v>9</v>
       </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <f>AVERAGE(B121:B152)</f>
+        <v>150.28125</v>
+      </c>
       <c r="J38">
         <v>19</v>
       </c>
       <c r="K38">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="L38" t="s">
         <v>9</v>
+      </c>
+      <c r="N38" t="s">
+        <v>15</v>
+      </c>
+      <c r="O38">
+        <f>AVERAGE(K121:K152)</f>
+        <v>83.40625</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -1194,14 +1254,28 @@
       <c r="C39" t="s">
         <v>9</v>
       </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39">
+        <f>_xlfn.STDEV.P(B121:B152)</f>
+        <v>456.18172327312448</v>
+      </c>
       <c r="J39">
         <v>20</v>
       </c>
       <c r="K39">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="L39" t="s">
         <v>9</v>
+      </c>
+      <c r="N39" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39">
+        <f>_xlfn.STDEV.P(K121:K152)</f>
+        <v>275.55578602333412</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -1214,14 +1288,28 @@
       <c r="C40" t="s">
         <v>9</v>
       </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <f>MEDIAN(B121:B152)</f>
+        <v>75.5</v>
+      </c>
       <c r="J40">
         <v>21</v>
       </c>
       <c r="K40">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="L40" t="s">
         <v>9</v>
+      </c>
+      <c r="N40" t="s">
+        <v>20</v>
+      </c>
+      <c r="O40">
+        <f>MEDIAN(K121:K152)</f>
+        <v>28.5</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -1238,7 +1326,7 @@
         <v>22</v>
       </c>
       <c r="K41">
-        <v>150</v>
+        <v>28</v>
       </c>
       <c r="L41" t="s">
         <v>9</v>
@@ -1258,7 +1346,7 @@
         <v>23</v>
       </c>
       <c r="K42">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="L42" t="s">
         <v>9</v>
@@ -1278,7 +1366,7 @@
         <v>24</v>
       </c>
       <c r="K43">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="L43" t="s">
         <v>9</v>
@@ -1298,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="K44">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="L44" t="s">
         <v>9</v>
@@ -1318,7 +1406,7 @@
         <v>26</v>
       </c>
       <c r="K45">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="L45" t="s">
         <v>9</v>
@@ -1338,7 +1426,7 @@
         <v>27</v>
       </c>
       <c r="K46">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="L46" t="s">
         <v>9</v>
@@ -1358,7 +1446,7 @@
         <v>28</v>
       </c>
       <c r="K47">
-        <v>167</v>
+        <v>31</v>
       </c>
       <c r="L47" t="s">
         <v>9</v>
@@ -1378,7 +1466,7 @@
         <v>29</v>
       </c>
       <c r="K48">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="L48" t="s">
         <v>9</v>
@@ -1398,7 +1486,7 @@
         <v>30</v>
       </c>
       <c r="K49">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="L49" t="s">
         <v>9</v>
@@ -1418,7 +1506,7 @@
         <v>31</v>
       </c>
       <c r="K50">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="L50" t="s">
         <v>9</v>
@@ -1446,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>462</v>
+        <v>293</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
@@ -1466,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="L54" t="s">
         <v>9</v>
@@ -1486,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="K55">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
@@ -1506,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="K56">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="L56" t="s">
         <v>9</v>
@@ -1526,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="K57">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="L57" t="s">
         <v>9</v>
@@ -1546,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="K58">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -1566,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="K59">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -1586,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="K60">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="L60" t="s">
         <v>9</v>
@@ -1606,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="K61">
-        <v>118</v>
+        <v>25</v>
       </c>
       <c r="L61" t="s">
         <v>9</v>
@@ -1626,7 +1714,7 @@
         <v>9</v>
       </c>
       <c r="K62">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="L62" t="s">
         <v>9</v>
@@ -1646,7 +1734,7 @@
         <v>10</v>
       </c>
       <c r="K63">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="L63" t="s">
         <v>9</v>
@@ -1666,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="K64">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="L64" t="s">
         <v>9</v>
@@ -1686,7 +1774,7 @@
         <v>12</v>
       </c>
       <c r="K65">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="L65" t="s">
         <v>9</v>
@@ -1706,7 +1794,7 @@
         <v>13</v>
       </c>
       <c r="K66">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="L66" t="s">
         <v>9</v>
@@ -1726,7 +1814,7 @@
         <v>14</v>
       </c>
       <c r="K67">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="L67" t="s">
         <v>9</v>
@@ -1746,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="K68">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
@@ -1766,7 +1854,7 @@
         <v>16</v>
       </c>
       <c r="K69">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="L69" t="s">
         <v>9</v>
@@ -1786,7 +1874,7 @@
         <v>17</v>
       </c>
       <c r="K70">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="L70" t="s">
         <v>9</v>
@@ -1806,7 +1894,7 @@
         <v>18</v>
       </c>
       <c r="K71">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="L71" t="s">
         <v>9</v>
@@ -1826,7 +1914,7 @@
         <v>19</v>
       </c>
       <c r="K72">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="L72" t="s">
         <v>9</v>
@@ -1846,7 +1934,7 @@
         <v>20</v>
       </c>
       <c r="K73">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="L73" t="s">
         <v>9</v>
@@ -1866,7 +1954,7 @@
         <v>21</v>
       </c>
       <c r="K74">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="L74" t="s">
         <v>9</v>
@@ -1886,7 +1974,7 @@
         <v>22</v>
       </c>
       <c r="K75">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="L75" t="s">
         <v>9</v>
@@ -1906,7 +1994,7 @@
         <v>23</v>
       </c>
       <c r="K76">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="L76" t="s">
         <v>9</v>
@@ -1926,7 +2014,7 @@
         <v>24</v>
       </c>
       <c r="K77">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="L77" t="s">
         <v>9</v>
@@ -1946,7 +2034,7 @@
         <v>25</v>
       </c>
       <c r="K78">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="L78" t="s">
         <v>9</v>
@@ -1966,7 +2054,7 @@
         <v>26</v>
       </c>
       <c r="K79">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="L79" t="s">
         <v>9</v>
@@ -1986,7 +2074,7 @@
         <v>27</v>
       </c>
       <c r="K80">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="L80" t="s">
         <v>9</v>
@@ -2006,7 +2094,7 @@
         <v>28</v>
       </c>
       <c r="K81">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="L81" t="s">
         <v>9</v>
@@ -2026,7 +2114,7 @@
         <v>29</v>
       </c>
       <c r="K82">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="L82" t="s">
         <v>9</v>
@@ -2046,7 +2134,7 @@
         <v>30</v>
       </c>
       <c r="K83">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="L83" t="s">
         <v>9</v>
@@ -2066,7 +2154,7 @@
         <v>31</v>
       </c>
       <c r="K84">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="L84" t="s">
         <v>9</v>
@@ -2094,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="L87" t="s">
         <v>9</v>
@@ -2114,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="K88">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L88" t="s">
         <v>9</v>
@@ -2154,7 +2242,7 @@
         <v>3</v>
       </c>
       <c r="K90">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L90" t="s">
         <v>9</v>
@@ -2174,7 +2262,7 @@
         <v>4</v>
       </c>
       <c r="K91">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L91" t="s">
         <v>9</v>
@@ -2194,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="K92">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L92" t="s">
         <v>9</v>
@@ -2234,7 +2322,7 @@
         <v>7</v>
       </c>
       <c r="K94">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L94" t="s">
         <v>9</v>
@@ -2254,7 +2342,7 @@
         <v>8</v>
       </c>
       <c r="K95">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L95" t="s">
         <v>9</v>
@@ -2274,7 +2362,7 @@
         <v>9</v>
       </c>
       <c r="K96">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L96" t="s">
         <v>9</v>
@@ -2294,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="K97">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L97" t="s">
         <v>9</v>
@@ -2334,7 +2422,7 @@
         <v>12</v>
       </c>
       <c r="K99">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="L99" t="s">
         <v>9</v>
@@ -2354,7 +2442,7 @@
         <v>13</v>
       </c>
       <c r="K100">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="L100" t="s">
         <v>9</v>
@@ -2374,7 +2462,7 @@
         <v>14</v>
       </c>
       <c r="K101">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L101" t="s">
         <v>9</v>
@@ -2394,7 +2482,7 @@
         <v>15</v>
       </c>
       <c r="K102">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L102" t="s">
         <v>9</v>
@@ -2414,7 +2502,7 @@
         <v>16</v>
       </c>
       <c r="K103">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L103" t="s">
         <v>9</v>
@@ -2434,7 +2522,7 @@
         <v>17</v>
       </c>
       <c r="K104">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L104" t="s">
         <v>9</v>
@@ -2454,7 +2542,7 @@
         <v>18</v>
       </c>
       <c r="K105">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L105" t="s">
         <v>9</v>
@@ -2474,7 +2562,7 @@
         <v>19</v>
       </c>
       <c r="K106">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="L106" t="s">
         <v>9</v>
@@ -2494,7 +2582,7 @@
         <v>20</v>
       </c>
       <c r="K107">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L107" t="s">
         <v>9</v>
@@ -2514,7 +2602,7 @@
         <v>21</v>
       </c>
       <c r="K108">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L108" t="s">
         <v>9</v>
@@ -2534,7 +2622,7 @@
         <v>22</v>
       </c>
       <c r="K109">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L109" t="s">
         <v>9</v>
@@ -2554,7 +2642,7 @@
         <v>23</v>
       </c>
       <c r="K110">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="L110" t="s">
         <v>9</v>
@@ -2574,7 +2662,7 @@
         <v>24</v>
       </c>
       <c r="K111">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L111" t="s">
         <v>9</v>
@@ -2594,7 +2682,7 @@
         <v>25</v>
       </c>
       <c r="K112">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="L112" t="s">
         <v>9</v>
@@ -2614,7 +2702,7 @@
         <v>26</v>
       </c>
       <c r="K113">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L113" t="s">
         <v>9</v>
@@ -2634,7 +2722,7 @@
         <v>27</v>
       </c>
       <c r="K114">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L114" t="s">
         <v>9</v>
@@ -2654,7 +2742,7 @@
         <v>28</v>
       </c>
       <c r="K115">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L115" t="s">
         <v>9</v>
@@ -2674,7 +2762,7 @@
         <v>29</v>
       </c>
       <c r="K116">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L116" t="s">
         <v>9</v>
@@ -2694,7 +2782,7 @@
         <v>30</v>
       </c>
       <c r="K117">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L117" t="s">
         <v>9</v>
@@ -2714,7 +2802,7 @@
         <v>31</v>
       </c>
       <c r="K118">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="L118" t="s">
         <v>9</v>
@@ -2738,8 +2826,11 @@
       <c r="C121" t="s">
         <v>9</v>
       </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
       <c r="K121">
-        <v>305</v>
+        <v>148</v>
       </c>
       <c r="L121" t="s">
         <v>9</v>
@@ -2759,7 +2850,7 @@
         <v>1</v>
       </c>
       <c r="K122">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="L122" t="s">
         <v>9</v>
@@ -2779,7 +2870,7 @@
         <v>2</v>
       </c>
       <c r="K123">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="L123" t="s">
         <v>9</v>
@@ -2799,7 +2890,7 @@
         <v>3</v>
       </c>
       <c r="K124">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="L124" t="s">
         <v>9</v>
@@ -2819,7 +2910,7 @@
         <v>4</v>
       </c>
       <c r="K125">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="L125" t="s">
         <v>9</v>
@@ -2839,7 +2930,7 @@
         <v>5</v>
       </c>
       <c r="K126">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="L126" t="s">
         <v>9</v>
@@ -2859,7 +2950,7 @@
         <v>6</v>
       </c>
       <c r="K127">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="L127" t="s">
         <v>9</v>
@@ -2879,7 +2970,7 @@
         <v>7</v>
       </c>
       <c r="K128">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="L128" t="s">
         <v>9</v>
@@ -2899,7 +2990,7 @@
         <v>8</v>
       </c>
       <c r="K129">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="L129" t="s">
         <v>9</v>
@@ -2919,7 +3010,7 @@
         <v>9</v>
       </c>
       <c r="K130">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="L130" t="s">
         <v>9</v>
@@ -2939,7 +3030,7 @@
         <v>10</v>
       </c>
       <c r="K131">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="L131" t="s">
         <v>9</v>
@@ -2959,7 +3050,7 @@
         <v>11</v>
       </c>
       <c r="K132">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="L132" t="s">
         <v>9</v>
@@ -2979,7 +3070,7 @@
         <v>12</v>
       </c>
       <c r="K133">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L133" t="s">
         <v>9</v>
@@ -2999,7 +3090,7 @@
         <v>13</v>
       </c>
       <c r="K134">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="L134" t="s">
         <v>9</v>
@@ -3019,7 +3110,7 @@
         <v>14</v>
       </c>
       <c r="K135">
-        <v>114</v>
+        <v>1613</v>
       </c>
       <c r="L135" t="s">
         <v>9</v>
@@ -3039,7 +3130,7 @@
         <v>15</v>
       </c>
       <c r="K136">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="L136" t="s">
         <v>9</v>
@@ -3059,7 +3150,7 @@
         <v>16</v>
       </c>
       <c r="K137">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="L137" t="s">
         <v>9</v>
@@ -3079,7 +3170,7 @@
         <v>17</v>
       </c>
       <c r="K138">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="L138" t="s">
         <v>9</v>
@@ -3099,7 +3190,7 @@
         <v>18</v>
       </c>
       <c r="K139">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="L139" t="s">
         <v>9</v>
@@ -3119,7 +3210,7 @@
         <v>19</v>
       </c>
       <c r="K140">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="L140" t="s">
         <v>9</v>
@@ -3139,7 +3230,7 @@
         <v>20</v>
       </c>
       <c r="K141">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="L141" t="s">
         <v>9</v>
@@ -3159,7 +3250,7 @@
         <v>21</v>
       </c>
       <c r="K142">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="L142" t="s">
         <v>9</v>
@@ -3179,7 +3270,7 @@
         <v>22</v>
       </c>
       <c r="K143">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="L143" t="s">
         <v>9</v>
@@ -3199,7 +3290,7 @@
         <v>23</v>
       </c>
       <c r="K144">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="L144" t="s">
         <v>9</v>
@@ -3219,7 +3310,7 @@
         <v>24</v>
       </c>
       <c r="K145">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="L145" t="s">
         <v>9</v>
@@ -3239,7 +3330,7 @@
         <v>25</v>
       </c>
       <c r="K146">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="L146" t="s">
         <v>9</v>
@@ -3259,7 +3350,7 @@
         <v>26</v>
       </c>
       <c r="K147">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="L147" t="s">
         <v>9</v>
@@ -3279,7 +3370,7 @@
         <v>27</v>
       </c>
       <c r="K148">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="L148" t="s">
         <v>9</v>
@@ -3299,7 +3390,7 @@
         <v>28</v>
       </c>
       <c r="K149">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="L149" t="s">
         <v>9</v>
@@ -3319,7 +3410,7 @@
         <v>29</v>
       </c>
       <c r="K150">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="L150" t="s">
         <v>9</v>
@@ -3339,7 +3430,7 @@
         <v>30</v>
       </c>
       <c r="K151">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="L151" t="s">
         <v>9</v>
@@ -3359,7 +3450,7 @@
         <v>31</v>
       </c>
       <c r="K152">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="L152" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Did the "eliminate memory bank conflict" thing, but it doesn't seem to have netted me any performance gain.
durations.txt has the numbers after running through 2x parallel sorts
over 1,000,000 scrambled numbers, and Optimization Timings.xlsx has the
timings from the implementation without the memory bank conflict
avoidance algorithm.  Ignore the 1st item being large.  That's just due
to (I think) system -> GPU memory transfers on the first run.  I wonder
if there is something to avoid memory bank conflicts built into the
driver...Don't know.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="M10">
         <f>SUM(O37,O31,O25,O19)</f>
-        <v>6237</v>
+        <v>7504</v>
       </c>
       <c r="N10" t="s">
         <v>25</v>
@@ -843,7 +843,7 @@
       </c>
       <c r="O25">
         <f>SUM(K53:K84)</f>
-        <v>1343</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -877,7 +877,7 @@
       </c>
       <c r="O26">
         <f>AVERAGE(K53:K84)</f>
-        <v>41.96875</v>
+        <v>81.5625</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
       </c>
       <c r="O27">
         <f>_xlfn.STDEV.P(K53:K84)</f>
-        <v>49.768516890073187</v>
+        <v>250.36734729942322</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -945,7 +945,7 @@
       </c>
       <c r="O28">
         <f>MEDIAN(K53:K84)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>293</v>
+        <v>1464</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L54" t="s">
         <v>9</v>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="K55">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
@@ -1594,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="K56">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="L56" t="s">
         <v>9</v>
@@ -1614,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="K57">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L57" t="s">
         <v>9</v>
@@ -1634,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="K58">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -1654,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="K59">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -1674,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="K60">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L60" t="s">
         <v>9</v>
@@ -1694,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="K61">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L61" t="s">
         <v>9</v>
@@ -1714,7 +1714,7 @@
         <v>9</v>
       </c>
       <c r="K62">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L62" t="s">
         <v>9</v>
@@ -1734,7 +1734,7 @@
         <v>10</v>
       </c>
       <c r="K63">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L63" t="s">
         <v>9</v>
@@ -1754,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="K64">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L64" t="s">
         <v>9</v>
@@ -1774,7 +1774,7 @@
         <v>12</v>
       </c>
       <c r="K65">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L65" t="s">
         <v>9</v>
@@ -1794,7 +1794,7 @@
         <v>13</v>
       </c>
       <c r="K66">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L66" t="s">
         <v>9</v>
@@ -1814,7 +1814,7 @@
         <v>14</v>
       </c>
       <c r="K67">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L67" t="s">
         <v>9</v>
@@ -1834,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="K68">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
@@ -1874,7 +1874,7 @@
         <v>17</v>
       </c>
       <c r="K70">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L70" t="s">
         <v>9</v>
@@ -1954,7 +1954,7 @@
         <v>21</v>
       </c>
       <c r="K74">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L74" t="s">
         <v>9</v>
@@ -1974,7 +1974,7 @@
         <v>22</v>
       </c>
       <c r="K75">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L75" t="s">
         <v>9</v>
@@ -2014,7 +2014,7 @@
         <v>24</v>
       </c>
       <c r="K77">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L77" t="s">
         <v>9</v>
@@ -2034,7 +2034,7 @@
         <v>25</v>
       </c>
       <c r="K78">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="L78" t="s">
         <v>9</v>
@@ -2054,7 +2054,7 @@
         <v>26</v>
       </c>
       <c r="K79">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L79" t="s">
         <v>9</v>
@@ -2074,7 +2074,7 @@
         <v>27</v>
       </c>
       <c r="K80">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L80" t="s">
         <v>9</v>
@@ -2094,7 +2094,7 @@
         <v>28</v>
       </c>
       <c r="K81">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="L81" t="s">
         <v>9</v>
@@ -2114,7 +2114,7 @@
         <v>29</v>
       </c>
       <c r="K82">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L82" t="s">
         <v>9</v>
@@ -2134,7 +2134,7 @@
         <v>30</v>
       </c>
       <c r="K83">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="L83" t="s">
         <v>9</v>
@@ -2154,7 +2154,7 @@
         <v>31</v>
       </c>
       <c r="K84">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="L84" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Got 1,000,000 item sort time from ~400,000 microseconds to ~5,000.
Eliminated time checking, std::vector<...> and other variable
declarations, and the printf(...) at the end of each loop, and the total
sort time dropped like a rock.  It doesn't matter if I'm using my
implementation of the conflict elimination algorithm or not, I'm still
getting ~5,000 microseconds (~5 milliseconds), which I am pleased about.
I think that I'll go back to the non-conflict-elimination algorithm.  It
requires less explanation.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="30">
   <si>
     <t>State</t>
   </si>
@@ -89,9 +89,6 @@
     <t>median</t>
   </si>
   <si>
-    <t>IntermediateData uses a single buffer (don't know why it's a bit slower now, but it's microseconds)</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>IntermediateData uses a single buffer</t>
+  </si>
+  <si>
+    <t>Note: These early results may be tainted by my only running the parallel sort once.  On the first run, data is loaded from system -&gt; GPU, but not if I run the sort a second time</t>
+  </si>
+  <si>
+    <t>ParallelPrefixScan writes to and from shared memory AND eleminates memory conflicts</t>
+  </si>
+  <si>
+    <t>These results are from running parallel sort a second time</t>
   </si>
 </sst>
 </file>
@@ -466,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O152"/>
+  <dimension ref="A1:X152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="O60" sqref="O60"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,66 +496,98 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="K4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
       <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
         <v>23</v>
       </c>
-      <c r="M9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>22</v>
+      </c>
+      <c r="V9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -556,7 +597,7 @@
         <v>19204</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10">
         <v>392545</v>
@@ -569,18 +610,34 @@
         <v>7504</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="S10">
+        <v>455535</v>
+      </c>
+      <c r="T10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10">
+        <f>SUM(X37,X31,X25,X19)</f>
+        <v>4487</v>
+      </c>
+      <c r="W10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="J12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9179</v>
       </c>
@@ -593,16 +650,25 @@
       <c r="K13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S13">
+        <v>98</v>
+      </c>
+      <c r="T13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1105355</v>
       </c>
@@ -615,8 +681,14 @@
       <c r="K16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S16">
+        <v>894672</v>
+      </c>
+      <c r="T16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -629,8 +701,14 @@
       <c r="N18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>11</v>
+      </c>
+      <c r="W18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -641,7 +719,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19">
         <f>SUM(B19:B50)</f>
@@ -657,14 +735,30 @@
         <v>9</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O19">
         <f>SUM(K19:K50)</f>
         <v>1359</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>32</v>
+      </c>
+      <c r="U19" t="s">
+        <v>9</v>
+      </c>
+      <c r="W19" t="s">
+        <v>21</v>
+      </c>
+      <c r="X19">
+        <f>SUM(T19:T50)</f>
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -697,8 +791,24 @@
         <f>AVERAGE(K19:K50)</f>
         <v>42.46875</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>47</v>
+      </c>
+      <c r="U20" t="s">
+        <v>9</v>
+      </c>
+      <c r="W20" t="s">
+        <v>15</v>
+      </c>
+      <c r="X20">
+        <f>AVERAGE(T19:T50)</f>
+        <v>43.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -731,8 +841,24 @@
         <f>_xlfn.STDEV.P(K19:K50)</f>
         <v>49.851018278842609</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S21">
+        <v>2</v>
+      </c>
+      <c r="T21">
+        <v>46</v>
+      </c>
+      <c r="U21" t="s">
+        <v>9</v>
+      </c>
+      <c r="W21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X21">
+        <f>_xlfn.STDEV.P(T19:T50)</f>
+        <v>15.817316460133179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -765,8 +891,24 @@
         <f>MEDIAN(K19:K50)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>38</v>
+      </c>
+      <c r="U22" t="s">
+        <v>9</v>
+      </c>
+      <c r="W22" t="s">
+        <v>20</v>
+      </c>
+      <c r="X22">
+        <f>MEDIAN(T19:T50)</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -785,8 +927,17 @@
       <c r="L23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S23">
+        <v>4</v>
+      </c>
+      <c r="T23">
+        <v>37</v>
+      </c>
+      <c r="U23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -811,8 +962,20 @@
       <c r="N24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S24">
+        <v>5</v>
+      </c>
+      <c r="T24">
+        <v>50</v>
+      </c>
+      <c r="U24" t="s">
+        <v>9</v>
+      </c>
+      <c r="W24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -823,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25">
         <f>SUM(B53:B84)</f>
@@ -839,14 +1002,30 @@
         <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O25">
         <f>SUM(K53:K84)</f>
         <v>2610</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S25">
+        <v>6</v>
+      </c>
+      <c r="T25">
+        <v>39</v>
+      </c>
+      <c r="U25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W25" t="s">
+        <v>21</v>
+      </c>
+      <c r="X25">
+        <f>SUM(T53:T84)</f>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -879,8 +1058,24 @@
         <f>AVERAGE(K53:K84)</f>
         <v>81.5625</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S26">
+        <v>7</v>
+      </c>
+      <c r="T26">
+        <v>50</v>
+      </c>
+      <c r="U26" t="s">
+        <v>9</v>
+      </c>
+      <c r="W26" t="s">
+        <v>15</v>
+      </c>
+      <c r="X26">
+        <f>AVERAGE(T53:T84)</f>
+        <v>35.03125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -913,8 +1108,24 @@
         <f>_xlfn.STDEV.P(K53:K84)</f>
         <v>250.36734729942322</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S27">
+        <v>8</v>
+      </c>
+      <c r="T27">
+        <v>46</v>
+      </c>
+      <c r="U27" t="s">
+        <v>9</v>
+      </c>
+      <c r="W27" t="s">
+        <v>16</v>
+      </c>
+      <c r="X27">
+        <f>_xlfn.STDEV.P(T53:T84)</f>
+        <v>15.611462885889329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -947,8 +1158,24 @@
         <f>MEDIAN(K53:K84)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S28">
+        <v>9</v>
+      </c>
+      <c r="T28">
+        <v>40</v>
+      </c>
+      <c r="U28" t="s">
+        <v>9</v>
+      </c>
+      <c r="W28" t="s">
+        <v>20</v>
+      </c>
+      <c r="X28">
+        <f>MEDIAN(T53:T84)</f>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -967,8 +1194,17 @@
       <c r="L29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S29">
+        <v>10</v>
+      </c>
+      <c r="T29">
+        <v>38</v>
+      </c>
+      <c r="U29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
@@ -993,8 +1229,20 @@
       <c r="N30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S30">
+        <v>11</v>
+      </c>
+      <c r="T30">
+        <v>29</v>
+      </c>
+      <c r="U30" t="s">
+        <v>9</v>
+      </c>
+      <c r="W30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1005,7 +1253,7 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31">
         <f>SUM(B87:B118)</f>
@@ -1021,14 +1269,30 @@
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O31">
         <f>SUM(K87:K118)</f>
         <v>866</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S31">
+        <v>12</v>
+      </c>
+      <c r="T31">
+        <v>29</v>
+      </c>
+      <c r="U31" t="s">
+        <v>9</v>
+      </c>
+      <c r="W31" t="s">
+        <v>21</v>
+      </c>
+      <c r="X31">
+        <f>SUM(T87:T118)</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>13</v>
       </c>
@@ -1061,8 +1325,24 @@
         <f>AVERAGE(K87:K118)</f>
         <v>27.0625</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S32">
+        <v>13</v>
+      </c>
+      <c r="T32">
+        <v>36</v>
+      </c>
+      <c r="U32" t="s">
+        <v>9</v>
+      </c>
+      <c r="W32" t="s">
+        <v>15</v>
+      </c>
+      <c r="X32">
+        <f>AVERAGE(T87:T118)</f>
+        <v>28.6875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1095,8 +1375,24 @@
         <f>_xlfn.STDEV.P(K87:K118)</f>
         <v>7.8019929345007739</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S33">
+        <v>14</v>
+      </c>
+      <c r="T33">
+        <v>37</v>
+      </c>
+      <c r="U33" t="s">
+        <v>9</v>
+      </c>
+      <c r="W33" t="s">
+        <v>16</v>
+      </c>
+      <c r="X33">
+        <f>_xlfn.STDEV.P(T87:T118)</f>
+        <v>5.2881796253531332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -1129,8 +1425,24 @@
         <f>MEDIAN(K87:K118)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S34">
+        <v>15</v>
+      </c>
+      <c r="T34">
+        <v>31</v>
+      </c>
+      <c r="U34" t="s">
+        <v>9</v>
+      </c>
+      <c r="W34" t="s">
+        <v>20</v>
+      </c>
+      <c r="X34">
+        <f>MEDIAN(T87:T118)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1149,8 +1461,17 @@
       <c r="L35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S35">
+        <v>16</v>
+      </c>
+      <c r="T35">
+        <v>63</v>
+      </c>
+      <c r="U35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>17</v>
       </c>
@@ -1175,8 +1496,20 @@
       <c r="N36" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S36">
+        <v>17</v>
+      </c>
+      <c r="T36">
+        <v>37</v>
+      </c>
+      <c r="U36" t="s">
+        <v>9</v>
+      </c>
+      <c r="W36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>18</v>
       </c>
@@ -1187,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F37">
         <f>SUM(B121:B152)</f>
@@ -1203,14 +1536,30 @@
         <v>9</v>
       </c>
       <c r="N37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O37">
         <f>SUM(K121:K152)</f>
         <v>2669</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S37">
+        <v>18</v>
+      </c>
+      <c r="T37">
+        <v>36</v>
+      </c>
+      <c r="U37" t="s">
+        <v>9</v>
+      </c>
+      <c r="W37" t="s">
+        <v>21</v>
+      </c>
+      <c r="X37">
+        <f>SUM(T121:T152)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>19</v>
       </c>
@@ -1243,8 +1592,24 @@
         <f>AVERAGE(K121:K152)</f>
         <v>83.40625</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S38">
+        <v>19</v>
+      </c>
+      <c r="T38">
+        <v>63</v>
+      </c>
+      <c r="U38" t="s">
+        <v>9</v>
+      </c>
+      <c r="W38" t="s">
+        <v>15</v>
+      </c>
+      <c r="X38">
+        <f>AVERAGE(T121:T152)</f>
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -1277,8 +1642,24 @@
         <f>_xlfn.STDEV.P(K121:K152)</f>
         <v>275.55578602333412</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S39">
+        <v>20</v>
+      </c>
+      <c r="T39">
+        <v>33</v>
+      </c>
+      <c r="U39" t="s">
+        <v>9</v>
+      </c>
+      <c r="W39" t="s">
+        <v>16</v>
+      </c>
+      <c r="X39">
+        <f>_xlfn.STDEV.P(T121:T152)</f>
+        <v>4.3874821936960613</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21</v>
       </c>
@@ -1311,8 +1692,24 @@
         <f>MEDIAN(K121:K152)</f>
         <v>28.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S40">
+        <v>21</v>
+      </c>
+      <c r="T40">
+        <v>42</v>
+      </c>
+      <c r="U40" t="s">
+        <v>9</v>
+      </c>
+      <c r="W40" t="s">
+        <v>20</v>
+      </c>
+      <c r="X40">
+        <f>MEDIAN(T121:T152)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22</v>
       </c>
@@ -1331,8 +1728,17 @@
       <c r="L41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S41">
+        <v>22</v>
+      </c>
+      <c r="T41">
+        <v>32</v>
+      </c>
+      <c r="U41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>23</v>
       </c>
@@ -1351,8 +1757,17 @@
       <c r="L42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S42">
+        <v>23</v>
+      </c>
+      <c r="T42">
+        <v>31</v>
+      </c>
+      <c r="U42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>24</v>
       </c>
@@ -1371,8 +1786,17 @@
       <c r="L43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S43">
+        <v>24</v>
+      </c>
+      <c r="T43">
+        <v>37</v>
+      </c>
+      <c r="U43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>25</v>
       </c>
@@ -1391,8 +1815,17 @@
       <c r="L44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S44">
+        <v>25</v>
+      </c>
+      <c r="T44">
+        <v>36</v>
+      </c>
+      <c r="U44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>26</v>
       </c>
@@ -1411,8 +1844,17 @@
       <c r="L45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S45">
+        <v>26</v>
+      </c>
+      <c r="T45">
+        <v>31</v>
+      </c>
+      <c r="U45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>27</v>
       </c>
@@ -1431,8 +1873,17 @@
       <c r="L46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S46">
+        <v>27</v>
+      </c>
+      <c r="T46">
+        <v>56</v>
+      </c>
+      <c r="U46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>28</v>
       </c>
@@ -1451,8 +1902,17 @@
       <c r="L47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S47">
+        <v>28</v>
+      </c>
+      <c r="T47">
+        <v>113</v>
+      </c>
+      <c r="U47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>29</v>
       </c>
@@ -1471,8 +1931,17 @@
       <c r="L48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S48">
+        <v>29</v>
+      </c>
+      <c r="T48">
+        <v>62</v>
+      </c>
+      <c r="U48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>30</v>
       </c>
@@ -1491,8 +1960,17 @@
       <c r="L49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S49">
+        <v>30</v>
+      </c>
+      <c r="T49">
+        <v>51</v>
+      </c>
+      <c r="U49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>31</v>
       </c>
@@ -1511,16 +1989,28 @@
       <c r="L50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S50">
+        <v>31</v>
+      </c>
+      <c r="T50">
+        <v>36</v>
+      </c>
+      <c r="U50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
       <c r="J52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -1539,8 +2029,17 @@
       <c r="L53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>26</v>
+      </c>
+      <c r="U53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1559,8 +2058,17 @@
       <c r="L54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="T54">
+        <v>28</v>
+      </c>
+      <c r="U54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1579,8 +2087,17 @@
       <c r="L55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S55">
+        <v>2</v>
+      </c>
+      <c r="T55">
+        <v>25</v>
+      </c>
+      <c r="U55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1599,8 +2116,17 @@
       <c r="L56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S56">
+        <v>3</v>
+      </c>
+      <c r="T56">
+        <v>112</v>
+      </c>
+      <c r="U56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1619,8 +2145,17 @@
       <c r="L57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>32</v>
+      </c>
+      <c r="U57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5</v>
       </c>
@@ -1639,8 +2174,17 @@
       <c r="L58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S58">
+        <v>5</v>
+      </c>
+      <c r="T58">
+        <v>38</v>
+      </c>
+      <c r="U58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>6</v>
       </c>
@@ -1659,8 +2203,17 @@
       <c r="L59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S59">
+        <v>6</v>
+      </c>
+      <c r="T59">
+        <v>37</v>
+      </c>
+      <c r="U59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
@@ -1679,8 +2232,17 @@
       <c r="L60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S60">
+        <v>7</v>
+      </c>
+      <c r="T60">
+        <v>34</v>
+      </c>
+      <c r="U60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1699,8 +2261,17 @@
       <c r="L61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S61">
+        <v>8</v>
+      </c>
+      <c r="T61">
+        <v>54</v>
+      </c>
+      <c r="U61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>9</v>
       </c>
@@ -1719,8 +2290,17 @@
       <c r="L62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S62">
+        <v>9</v>
+      </c>
+      <c r="T62">
+        <v>26</v>
+      </c>
+      <c r="U62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10</v>
       </c>
@@ -1739,8 +2319,17 @@
       <c r="L63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S63">
+        <v>10</v>
+      </c>
+      <c r="T63">
+        <v>30</v>
+      </c>
+      <c r="U63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>11</v>
       </c>
@@ -1759,8 +2348,17 @@
       <c r="L64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S64">
+        <v>11</v>
+      </c>
+      <c r="T64">
+        <v>30</v>
+      </c>
+      <c r="U64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>12</v>
       </c>
@@ -1779,8 +2377,17 @@
       <c r="L65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S65">
+        <v>12</v>
+      </c>
+      <c r="T65">
+        <v>29</v>
+      </c>
+      <c r="U65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>13</v>
       </c>
@@ -1799,8 +2406,17 @@
       <c r="L66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S66">
+        <v>13</v>
+      </c>
+      <c r="T66">
+        <v>32</v>
+      </c>
+      <c r="U66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -1819,8 +2435,17 @@
       <c r="L67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S67">
+        <v>14</v>
+      </c>
+      <c r="T67">
+        <v>29</v>
+      </c>
+      <c r="U67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>15</v>
       </c>
@@ -1839,8 +2464,17 @@
       <c r="L68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S68">
+        <v>15</v>
+      </c>
+      <c r="T68">
+        <v>23</v>
+      </c>
+      <c r="U68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>16</v>
       </c>
@@ -1859,8 +2493,17 @@
       <c r="L69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S69">
+        <v>16</v>
+      </c>
+      <c r="T69">
+        <v>39</v>
+      </c>
+      <c r="U69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>17</v>
       </c>
@@ -1879,8 +2522,17 @@
       <c r="L70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S70">
+        <v>17</v>
+      </c>
+      <c r="T70">
+        <v>33</v>
+      </c>
+      <c r="U70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -1899,8 +2551,17 @@
       <c r="L71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S71">
+        <v>18</v>
+      </c>
+      <c r="T71">
+        <v>30</v>
+      </c>
+      <c r="U71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>19</v>
       </c>
@@ -1919,8 +2580,17 @@
       <c r="L72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S72">
+        <v>19</v>
+      </c>
+      <c r="T72">
+        <v>43</v>
+      </c>
+      <c r="U72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>20</v>
       </c>
@@ -1939,8 +2609,17 @@
       <c r="L73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S73">
+        <v>20</v>
+      </c>
+      <c r="T73">
+        <v>23</v>
+      </c>
+      <c r="U73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>21</v>
       </c>
@@ -1959,8 +2638,17 @@
       <c r="L74" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S74">
+        <v>21</v>
+      </c>
+      <c r="T74">
+        <v>30</v>
+      </c>
+      <c r="U74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>22</v>
       </c>
@@ -1979,8 +2667,17 @@
       <c r="L75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S75">
+        <v>22</v>
+      </c>
+      <c r="T75">
+        <v>31</v>
+      </c>
+      <c r="U75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>23</v>
       </c>
@@ -1999,8 +2696,17 @@
       <c r="L76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S76">
+        <v>23</v>
+      </c>
+      <c r="T76">
+        <v>31</v>
+      </c>
+      <c r="U76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24</v>
       </c>
@@ -2019,8 +2725,17 @@
       <c r="L77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S77">
+        <v>24</v>
+      </c>
+      <c r="T77">
+        <v>30</v>
+      </c>
+      <c r="U77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>25</v>
       </c>
@@ -2039,8 +2754,17 @@
       <c r="L78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S78">
+        <v>25</v>
+      </c>
+      <c r="T78">
+        <v>30</v>
+      </c>
+      <c r="U78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>26</v>
       </c>
@@ -2059,8 +2783,17 @@
       <c r="L79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S79">
+        <v>26</v>
+      </c>
+      <c r="T79">
+        <v>34</v>
+      </c>
+      <c r="U79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>27</v>
       </c>
@@ -2079,8 +2812,17 @@
       <c r="L80" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S80">
+        <v>27</v>
+      </c>
+      <c r="T80">
+        <v>35</v>
+      </c>
+      <c r="U80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>28</v>
       </c>
@@ -2099,8 +2841,17 @@
       <c r="L81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S81">
+        <v>28</v>
+      </c>
+      <c r="T81">
+        <v>55</v>
+      </c>
+      <c r="U81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>29</v>
       </c>
@@ -2119,8 +2870,17 @@
       <c r="L82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S82">
+        <v>29</v>
+      </c>
+      <c r="T82">
+        <v>26</v>
+      </c>
+      <c r="U82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>30</v>
       </c>
@@ -2139,8 +2899,17 @@
       <c r="L83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S83">
+        <v>30</v>
+      </c>
+      <c r="T83">
+        <v>28</v>
+      </c>
+      <c r="U83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>31</v>
       </c>
@@ -2159,16 +2928,28 @@
       <c r="L84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S84">
+        <v>31</v>
+      </c>
+      <c r="T84">
+        <v>38</v>
+      </c>
+      <c r="U84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>13</v>
       </c>
       <c r="J86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
@@ -2187,8 +2968,17 @@
       <c r="L87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S87">
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <v>21</v>
+      </c>
+      <c r="U87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1</v>
       </c>
@@ -2207,8 +2997,17 @@
       <c r="L88" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S88">
+        <v>1</v>
+      </c>
+      <c r="T88">
+        <v>26</v>
+      </c>
+      <c r="U88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -2227,8 +3026,17 @@
       <c r="L89" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S89">
+        <v>2</v>
+      </c>
+      <c r="T89">
+        <v>34</v>
+      </c>
+      <c r="U89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3</v>
       </c>
@@ -2247,8 +3055,17 @@
       <c r="L90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S90">
+        <v>3</v>
+      </c>
+      <c r="T90">
+        <v>23</v>
+      </c>
+      <c r="U90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2267,8 +3084,17 @@
       <c r="L91" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S91">
+        <v>4</v>
+      </c>
+      <c r="T91">
+        <v>31</v>
+      </c>
+      <c r="U91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>5</v>
       </c>
@@ -2287,8 +3113,17 @@
       <c r="L92" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S92">
+        <v>5</v>
+      </c>
+      <c r="T92">
+        <v>27</v>
+      </c>
+      <c r="U92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>6</v>
       </c>
@@ -2307,8 +3142,17 @@
       <c r="L93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S93">
+        <v>6</v>
+      </c>
+      <c r="T93">
+        <v>37</v>
+      </c>
+      <c r="U93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>7</v>
       </c>
@@ -2327,8 +3171,17 @@
       <c r="L94" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S94">
+        <v>7</v>
+      </c>
+      <c r="T94">
+        <v>33</v>
+      </c>
+      <c r="U94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>8</v>
       </c>
@@ -2347,8 +3200,17 @@
       <c r="L95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S95">
+        <v>8</v>
+      </c>
+      <c r="T95">
+        <v>29</v>
+      </c>
+      <c r="U95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9</v>
       </c>
@@ -2367,8 +3229,17 @@
       <c r="L96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S96">
+        <v>9</v>
+      </c>
+      <c r="T96">
+        <v>33</v>
+      </c>
+      <c r="U96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10</v>
       </c>
@@ -2387,8 +3258,17 @@
       <c r="L97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S97">
+        <v>10</v>
+      </c>
+      <c r="T97">
+        <v>26</v>
+      </c>
+      <c r="U97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>11</v>
       </c>
@@ -2407,8 +3287,17 @@
       <c r="L98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S98">
+        <v>11</v>
+      </c>
+      <c r="T98">
+        <v>36</v>
+      </c>
+      <c r="U98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>12</v>
       </c>
@@ -2427,8 +3316,17 @@
       <c r="L99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S99">
+        <v>12</v>
+      </c>
+      <c r="T99">
+        <v>26</v>
+      </c>
+      <c r="U99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>13</v>
       </c>
@@ -2447,8 +3345,17 @@
       <c r="L100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S100">
+        <v>13</v>
+      </c>
+      <c r="T100">
+        <v>28</v>
+      </c>
+      <c r="U100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>14</v>
       </c>
@@ -2467,8 +3374,17 @@
       <c r="L101" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S101">
+        <v>14</v>
+      </c>
+      <c r="T101">
+        <v>26</v>
+      </c>
+      <c r="U101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>15</v>
       </c>
@@ -2487,8 +3403,17 @@
       <c r="L102" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S102">
+        <v>15</v>
+      </c>
+      <c r="T102">
+        <v>26</v>
+      </c>
+      <c r="U102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>16</v>
       </c>
@@ -2507,8 +3432,17 @@
       <c r="L103" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S103">
+        <v>16</v>
+      </c>
+      <c r="T103">
+        <v>28</v>
+      </c>
+      <c r="U103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>17</v>
       </c>
@@ -2527,8 +3461,17 @@
       <c r="L104" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S104">
+        <v>17</v>
+      </c>
+      <c r="T104">
+        <v>28</v>
+      </c>
+      <c r="U104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>18</v>
       </c>
@@ -2547,8 +3490,17 @@
       <c r="L105" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S105">
+        <v>18</v>
+      </c>
+      <c r="T105">
+        <v>26</v>
+      </c>
+      <c r="U105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>19</v>
       </c>
@@ -2567,8 +3519,17 @@
       <c r="L106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S106">
+        <v>19</v>
+      </c>
+      <c r="T106">
+        <v>44</v>
+      </c>
+      <c r="U106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>20</v>
       </c>
@@ -2587,8 +3548,17 @@
       <c r="L107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S107">
+        <v>20</v>
+      </c>
+      <c r="T107">
+        <v>27</v>
+      </c>
+      <c r="U107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>21</v>
       </c>
@@ -2607,8 +3577,17 @@
       <c r="L108" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S108">
+        <v>21</v>
+      </c>
+      <c r="T108">
+        <v>26</v>
+      </c>
+      <c r="U108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>22</v>
       </c>
@@ -2627,8 +3606,17 @@
       <c r="L109" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S109">
+        <v>22</v>
+      </c>
+      <c r="T109">
+        <v>26</v>
+      </c>
+      <c r="U109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>23</v>
       </c>
@@ -2647,8 +3635,17 @@
       <c r="L110" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S110">
+        <v>23</v>
+      </c>
+      <c r="T110">
+        <v>26</v>
+      </c>
+      <c r="U110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>24</v>
       </c>
@@ -2667,8 +3664,17 @@
       <c r="L111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S111">
+        <v>24</v>
+      </c>
+      <c r="T111">
+        <v>29</v>
+      </c>
+      <c r="U111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>25</v>
       </c>
@@ -2687,8 +3693,17 @@
       <c r="L112" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S112">
+        <v>25</v>
+      </c>
+      <c r="T112">
+        <v>26</v>
+      </c>
+      <c r="U112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>26</v>
       </c>
@@ -2707,8 +3722,17 @@
       <c r="L113" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S113">
+        <v>26</v>
+      </c>
+      <c r="T113">
+        <v>31</v>
+      </c>
+      <c r="U113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>27</v>
       </c>
@@ -2727,8 +3751,17 @@
       <c r="L114" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S114">
+        <v>27</v>
+      </c>
+      <c r="T114">
+        <v>41</v>
+      </c>
+      <c r="U114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>28</v>
       </c>
@@ -2747,8 +3780,17 @@
       <c r="L115" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S115">
+        <v>28</v>
+      </c>
+      <c r="T115">
+        <v>30</v>
+      </c>
+      <c r="U115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>29</v>
       </c>
@@ -2767,8 +3809,17 @@
       <c r="L116" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S116">
+        <v>29</v>
+      </c>
+      <c r="T116">
+        <v>21</v>
+      </c>
+      <c r="U116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>30</v>
       </c>
@@ -2787,8 +3838,17 @@
       <c r="L117" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S117">
+        <v>30</v>
+      </c>
+      <c r="T117">
+        <v>20</v>
+      </c>
+      <c r="U117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>31</v>
       </c>
@@ -2807,16 +3867,28 @@
       <c r="L118" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S118">
+        <v>31</v>
+      </c>
+      <c r="T118">
+        <v>27</v>
+      </c>
+      <c r="U118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>14</v>
       </c>
       <c r="J120" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S120" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>0</v>
       </c>
@@ -2835,8 +3907,17 @@
       <c r="L121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S121">
+        <v>0</v>
+      </c>
+      <c r="T121">
+        <v>26</v>
+      </c>
+      <c r="U121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1</v>
       </c>
@@ -2855,8 +3936,17 @@
       <c r="L122" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S122">
+        <v>1</v>
+      </c>
+      <c r="T122">
+        <v>41</v>
+      </c>
+      <c r="U122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2</v>
       </c>
@@ -2875,8 +3965,17 @@
       <c r="L123" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S123">
+        <v>2</v>
+      </c>
+      <c r="T123">
+        <v>34</v>
+      </c>
+      <c r="U123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>3</v>
       </c>
@@ -2895,8 +3994,17 @@
       <c r="L124" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S124">
+        <v>3</v>
+      </c>
+      <c r="T124">
+        <v>32</v>
+      </c>
+      <c r="U124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>4</v>
       </c>
@@ -2915,8 +4023,17 @@
       <c r="L125" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S125">
+        <v>4</v>
+      </c>
+      <c r="T125">
+        <v>34</v>
+      </c>
+      <c r="U125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -2935,8 +4052,17 @@
       <c r="L126" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S126">
+        <v>5</v>
+      </c>
+      <c r="T126">
+        <v>36</v>
+      </c>
+      <c r="U126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>6</v>
       </c>
@@ -2955,8 +4081,17 @@
       <c r="L127" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S127">
+        <v>6</v>
+      </c>
+      <c r="T127">
+        <v>34</v>
+      </c>
+      <c r="U127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>7</v>
       </c>
@@ -2975,8 +4110,17 @@
       <c r="L128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S128">
+        <v>7</v>
+      </c>
+      <c r="T128">
+        <v>32</v>
+      </c>
+      <c r="U128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>8</v>
       </c>
@@ -2995,8 +4139,17 @@
       <c r="L129" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S129">
+        <v>8</v>
+      </c>
+      <c r="T129">
+        <v>44</v>
+      </c>
+      <c r="U129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>9</v>
       </c>
@@ -3015,8 +4168,17 @@
       <c r="L130" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S130">
+        <v>9</v>
+      </c>
+      <c r="T130">
+        <v>39</v>
+      </c>
+      <c r="U130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>10</v>
       </c>
@@ -3035,8 +4197,17 @@
       <c r="L131" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S131">
+        <v>10</v>
+      </c>
+      <c r="T131">
+        <v>30</v>
+      </c>
+      <c r="U131" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>11</v>
       </c>
@@ -3055,8 +4226,17 @@
       <c r="L132" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S132">
+        <v>11</v>
+      </c>
+      <c r="T132">
+        <v>30</v>
+      </c>
+      <c r="U132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>12</v>
       </c>
@@ -3075,8 +4255,17 @@
       <c r="L133" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S133">
+        <v>12</v>
+      </c>
+      <c r="T133">
+        <v>34</v>
+      </c>
+      <c r="U133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>13</v>
       </c>
@@ -3095,8 +4284,17 @@
       <c r="L134" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S134">
+        <v>13</v>
+      </c>
+      <c r="T134">
+        <v>39</v>
+      </c>
+      <c r="U134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>14</v>
       </c>
@@ -3115,8 +4313,17 @@
       <c r="L135" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S135">
+        <v>14</v>
+      </c>
+      <c r="T135">
+        <v>30</v>
+      </c>
+      <c r="U135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>15</v>
       </c>
@@ -3135,8 +4342,17 @@
       <c r="L136" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S136">
+        <v>15</v>
+      </c>
+      <c r="T136">
+        <v>31</v>
+      </c>
+      <c r="U136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>16</v>
       </c>
@@ -3155,8 +4371,17 @@
       <c r="L137" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S137">
+        <v>16</v>
+      </c>
+      <c r="T137">
+        <v>42</v>
+      </c>
+      <c r="U137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>17</v>
       </c>
@@ -3175,8 +4400,17 @@
       <c r="L138" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S138">
+        <v>17</v>
+      </c>
+      <c r="T138">
+        <v>35</v>
+      </c>
+      <c r="U138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>18</v>
       </c>
@@ -3195,8 +4429,17 @@
       <c r="L139" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S139">
+        <v>18</v>
+      </c>
+      <c r="T139">
+        <v>30</v>
+      </c>
+      <c r="U139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>19</v>
       </c>
@@ -3215,8 +4458,17 @@
       <c r="L140" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S140">
+        <v>19</v>
+      </c>
+      <c r="T140">
+        <v>34</v>
+      </c>
+      <c r="U140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>20</v>
       </c>
@@ -3235,8 +4487,17 @@
       <c r="L141" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S141">
+        <v>20</v>
+      </c>
+      <c r="T141">
+        <v>30</v>
+      </c>
+      <c r="U141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>21</v>
       </c>
@@ -3255,8 +4516,17 @@
       <c r="L142" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S142">
+        <v>21</v>
+      </c>
+      <c r="T142">
+        <v>30</v>
+      </c>
+      <c r="U142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>22</v>
       </c>
@@ -3275,8 +4545,17 @@
       <c r="L143" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S143">
+        <v>22</v>
+      </c>
+      <c r="T143">
+        <v>30</v>
+      </c>
+      <c r="U143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>23</v>
       </c>
@@ -3295,8 +4574,17 @@
       <c r="L144" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S144">
+        <v>23</v>
+      </c>
+      <c r="T144">
+        <v>30</v>
+      </c>
+      <c r="U144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>24</v>
       </c>
@@ -3315,8 +4603,17 @@
       <c r="L145" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S145">
+        <v>24</v>
+      </c>
+      <c r="T145">
+        <v>31</v>
+      </c>
+      <c r="U145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>25</v>
       </c>
@@ -3335,8 +4632,17 @@
       <c r="L146" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S146">
+        <v>25</v>
+      </c>
+      <c r="T146">
+        <v>30</v>
+      </c>
+      <c r="U146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>26</v>
       </c>
@@ -3355,8 +4661,17 @@
       <c r="L147" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S147">
+        <v>26</v>
+      </c>
+      <c r="T147">
+        <v>37</v>
+      </c>
+      <c r="U147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>27</v>
       </c>
@@ -3375,8 +4690,17 @@
       <c r="L148" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S148">
+        <v>27</v>
+      </c>
+      <c r="T148">
+        <v>35</v>
+      </c>
+      <c r="U148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>28</v>
       </c>
@@ -3395,8 +4719,17 @@
       <c r="L149" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S149">
+        <v>28</v>
+      </c>
+      <c r="T149">
+        <v>28</v>
+      </c>
+      <c r="U149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>29</v>
       </c>
@@ -3415,8 +4748,17 @@
       <c r="L150" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S150">
+        <v>29</v>
+      </c>
+      <c r="T150">
+        <v>25</v>
+      </c>
+      <c r="U150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>30</v>
       </c>
@@ -3435,8 +4777,17 @@
       <c r="L151" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S151">
+        <v>30</v>
+      </c>
+      <c r="T151">
+        <v>35</v>
+      </c>
+      <c r="U151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>31</v>
       </c>
@@ -3453,6 +4804,15 @@
         <v>28</v>
       </c>
       <c r="L152" t="s">
+        <v>9</v>
+      </c>
+      <c r="S152">
+        <v>31</v>
+      </c>
+      <c r="T152">
+        <v>36</v>
+      </c>
+      <c r="U152" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now sorting original data as well: ~5.4ms.
I don't know why, but the sum of the durations of all the shaders +
copying the sorted original data from the copy buffer back to its
original buffer is ~5.8ms.  I don't know where those extra ~400
microseconds came from.
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="33">
   <si>
     <t>State</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>These results are from running parallel sort a second time</t>
+  </si>
+  <si>
+    <t>Sorting original data when finished according to sorted IntermediateData</t>
+  </si>
+  <si>
+    <t>copy original data back from copy buffer</t>
+  </si>
+  <si>
+    <t>sort original data into copy buffer</t>
   </si>
 </sst>
 </file>
@@ -475,15 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X152"/>
+  <dimension ref="A1:AG152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,8 +511,14 @@
       <c r="T1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -513,8 +528,11 @@
       <c r="T2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -524,8 +542,11 @@
       <c r="T3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -535,8 +556,11 @@
       <c r="T4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -546,26 +570,35 @@
       <c r="T5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AC7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -584,8 +617,14 @@
       <c r="V9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -625,8 +664,20 @@
       <c r="W10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB10">
+        <v>5332</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF10">
+        <v>137</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -636,8 +687,14 @@
       <c r="S12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9179</v>
       </c>
@@ -657,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -667,8 +724,11 @@
       <c r="S15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1105355</v>
       </c>
@@ -687,8 +747,14 @@
       <c r="T16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB16">
+        <v>894672</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -707,8 +773,14 @@
       <c r="W18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -757,8 +829,24 @@
         <f>SUM(T19:T50)</f>
         <v>1384</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>32</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG19">
+        <f>SUM(AC19:AC50)</f>
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -807,8 +895,24 @@
         <f>AVERAGE(T19:T50)</f>
         <v>43.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>47</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG20">
+        <f>AVERAGE(AC19:AC50)</f>
+        <v>43.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -857,8 +961,24 @@
         <f>_xlfn.STDEV.P(T19:T50)</f>
         <v>15.817316460133179</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB21">
+        <v>2</v>
+      </c>
+      <c r="AC21">
+        <v>46</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG21">
+        <f>_xlfn.STDEV.P(AC19:AC50)</f>
+        <v>15.817316460133179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -907,8 +1027,24 @@
         <f>MEDIAN(T19:T50)</f>
         <v>37.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB22">
+        <v>3</v>
+      </c>
+      <c r="AC22">
+        <v>38</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG22">
+        <f>MEDIAN(AC19:AC50)</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -936,8 +1072,17 @@
       <c r="U23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB23">
+        <v>4</v>
+      </c>
+      <c r="AC23">
+        <v>37</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -974,8 +1119,20 @@
       <c r="W24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB24">
+        <v>5</v>
+      </c>
+      <c r="AC24">
+        <v>50</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1024,8 +1181,24 @@
         <f>SUM(T53:T84)</f>
         <v>1121</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB25">
+        <v>6</v>
+      </c>
+      <c r="AC25">
+        <v>39</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG25">
+        <f>SUM(AC53:AC84)</f>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1074,8 +1247,24 @@
         <f>AVERAGE(T53:T84)</f>
         <v>35.03125</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB26">
+        <v>7</v>
+      </c>
+      <c r="AC26">
+        <v>50</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG26">
+        <f>AVERAGE(AC53:AC84)</f>
+        <v>35.03125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1124,8 +1313,24 @@
         <f>_xlfn.STDEV.P(T53:T84)</f>
         <v>15.611462885889329</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB27">
+        <v>8</v>
+      </c>
+      <c r="AC27">
+        <v>46</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG27">
+        <f>_xlfn.STDEV.P(AC53:AC84)</f>
+        <v>15.611462885889329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1174,8 +1379,24 @@
         <f>MEDIAN(T53:T84)</f>
         <v>30.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB28">
+        <v>9</v>
+      </c>
+      <c r="AC28">
+        <v>40</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG28">
+        <f>MEDIAN(AC53:AC84)</f>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1203,8 +1424,17 @@
       <c r="U29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB29">
+        <v>10</v>
+      </c>
+      <c r="AC29">
+        <v>38</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
@@ -1241,8 +1471,20 @@
       <c r="W30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB30">
+        <v>11</v>
+      </c>
+      <c r="AC30">
+        <v>29</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1291,8 +1533,24 @@
         <f>SUM(T87:T118)</f>
         <v>918</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB31">
+        <v>12</v>
+      </c>
+      <c r="AC31">
+        <v>29</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG31">
+        <f>SUM(AC87:AC118)</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>13</v>
       </c>
@@ -1341,8 +1599,24 @@
         <f>AVERAGE(T87:T118)</f>
         <v>28.6875</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB32">
+        <v>13</v>
+      </c>
+      <c r="AC32">
+        <v>36</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG32">
+        <f>AVERAGE(AC87:AC118)</f>
+        <v>28.6875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1391,8 +1665,24 @@
         <f>_xlfn.STDEV.P(T87:T118)</f>
         <v>5.2881796253531332</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB33">
+        <v>14</v>
+      </c>
+      <c r="AC33">
+        <v>37</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG33">
+        <f>_xlfn.STDEV.P(AC87:AC118)</f>
+        <v>5.2881796253531332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -1441,8 +1731,24 @@
         <f>MEDIAN(T87:T118)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB34">
+        <v>15</v>
+      </c>
+      <c r="AC34">
+        <v>31</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG34">
+        <f>MEDIAN(AC87:AC118)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1470,8 +1776,17 @@
       <c r="U35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB35">
+        <v>16</v>
+      </c>
+      <c r="AC35">
+        <v>63</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>17</v>
       </c>
@@ -1508,8 +1823,20 @@
       <c r="W36" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB36">
+        <v>17</v>
+      </c>
+      <c r="AC36">
+        <v>37</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>18</v>
       </c>
@@ -1558,8 +1885,24 @@
         <f>SUM(T121:T152)</f>
         <v>1064</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB37">
+        <v>18</v>
+      </c>
+      <c r="AC37">
+        <v>36</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG37">
+        <f>SUM(AC121:AC152)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>19</v>
       </c>
@@ -1608,8 +1951,24 @@
         <f>AVERAGE(T121:T152)</f>
         <v>33.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB38">
+        <v>19</v>
+      </c>
+      <c r="AC38">
+        <v>63</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG38">
+        <f>AVERAGE(AC121:AC152)</f>
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -1658,8 +2017,24 @@
         <f>_xlfn.STDEV.P(T121:T152)</f>
         <v>4.3874821936960613</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB39">
+        <v>20</v>
+      </c>
+      <c r="AC39">
+        <v>33</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG39">
+        <f>_xlfn.STDEV.P(AC121:AC152)</f>
+        <v>4.3874821936960613</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21</v>
       </c>
@@ -1708,8 +2083,24 @@
         <f>MEDIAN(T121:T152)</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB40">
+        <v>21</v>
+      </c>
+      <c r="AC40">
+        <v>42</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG40">
+        <f>MEDIAN(AC121:AC152)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22</v>
       </c>
@@ -1737,8 +2128,17 @@
       <c r="U41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB41">
+        <v>22</v>
+      </c>
+      <c r="AC41">
+        <v>32</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>23</v>
       </c>
@@ -1766,8 +2166,17 @@
       <c r="U42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB42">
+        <v>23</v>
+      </c>
+      <c r="AC42">
+        <v>31</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>24</v>
       </c>
@@ -1795,8 +2204,17 @@
       <c r="U43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB43">
+        <v>24</v>
+      </c>
+      <c r="AC43">
+        <v>37</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>25</v>
       </c>
@@ -1824,8 +2242,17 @@
       <c r="U44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB44">
+        <v>25</v>
+      </c>
+      <c r="AC44">
+        <v>36</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>26</v>
       </c>
@@ -1853,8 +2280,17 @@
       <c r="U45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB45">
+        <v>26</v>
+      </c>
+      <c r="AC45">
+        <v>31</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>27</v>
       </c>
@@ -1882,8 +2318,17 @@
       <c r="U46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB46">
+        <v>27</v>
+      </c>
+      <c r="AC46">
+        <v>56</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>28</v>
       </c>
@@ -1911,8 +2356,17 @@
       <c r="U47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AB47">
+        <v>28</v>
+      </c>
+      <c r="AC47">
+        <v>113</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>29</v>
       </c>
@@ -1940,8 +2394,17 @@
       <c r="U48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB48">
+        <v>29</v>
+      </c>
+      <c r="AC48">
+        <v>62</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>30</v>
       </c>
@@ -1969,8 +2432,17 @@
       <c r="U49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB49">
+        <v>30</v>
+      </c>
+      <c r="AC49">
+        <v>51</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>31</v>
       </c>
@@ -1998,8 +2470,17 @@
       <c r="U50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB50">
+        <v>31</v>
+      </c>
+      <c r="AC50">
+        <v>36</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2009,8 +2490,11 @@
       <c r="S52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -2038,8 +2522,17 @@
       <c r="U53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB53">
+        <v>0</v>
+      </c>
+      <c r="AC53">
+        <v>26</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2067,8 +2560,17 @@
       <c r="U54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB54">
+        <v>1</v>
+      </c>
+      <c r="AC54">
+        <v>28</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -2096,8 +2598,17 @@
       <c r="U55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB55">
+        <v>2</v>
+      </c>
+      <c r="AC55">
+        <v>25</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2125,8 +2636,17 @@
       <c r="U56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB56">
+        <v>3</v>
+      </c>
+      <c r="AC56">
+        <v>112</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4</v>
       </c>
@@ -2154,8 +2674,17 @@
       <c r="U57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB57">
+        <v>4</v>
+      </c>
+      <c r="AC57">
+        <v>32</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5</v>
       </c>
@@ -2183,8 +2712,17 @@
       <c r="U58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB58">
+        <v>5</v>
+      </c>
+      <c r="AC58">
+        <v>38</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2212,8 +2750,17 @@
       <c r="U59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB59">
+        <v>6</v>
+      </c>
+      <c r="AC59">
+        <v>37</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
@@ -2241,8 +2788,17 @@
       <c r="U60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB60">
+        <v>7</v>
+      </c>
+      <c r="AC60">
+        <v>34</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>8</v>
       </c>
@@ -2270,8 +2826,17 @@
       <c r="U61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB61">
+        <v>8</v>
+      </c>
+      <c r="AC61">
+        <v>54</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>9</v>
       </c>
@@ -2299,8 +2864,17 @@
       <c r="U62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB62">
+        <v>9</v>
+      </c>
+      <c r="AC62">
+        <v>26</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10</v>
       </c>
@@ -2328,8 +2902,17 @@
       <c r="U63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB63">
+        <v>10</v>
+      </c>
+      <c r="AC63">
+        <v>30</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>11</v>
       </c>
@@ -2357,8 +2940,17 @@
       <c r="U64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB64">
+        <v>11</v>
+      </c>
+      <c r="AC64">
+        <v>30</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>12</v>
       </c>
@@ -2386,8 +2978,17 @@
       <c r="U65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB65">
+        <v>12</v>
+      </c>
+      <c r="AC65">
+        <v>29</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>13</v>
       </c>
@@ -2415,8 +3016,17 @@
       <c r="U66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB66">
+        <v>13</v>
+      </c>
+      <c r="AC66">
+        <v>32</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -2444,8 +3054,17 @@
       <c r="U67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB67">
+        <v>14</v>
+      </c>
+      <c r="AC67">
+        <v>29</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>15</v>
       </c>
@@ -2473,8 +3092,17 @@
       <c r="U68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB68">
+        <v>15</v>
+      </c>
+      <c r="AC68">
+        <v>23</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>16</v>
       </c>
@@ -2502,8 +3130,17 @@
       <c r="U69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB69">
+        <v>16</v>
+      </c>
+      <c r="AC69">
+        <v>39</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>17</v>
       </c>
@@ -2531,8 +3168,17 @@
       <c r="U70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB70">
+        <v>17</v>
+      </c>
+      <c r="AC70">
+        <v>33</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -2560,8 +3206,17 @@
       <c r="U71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB71">
+        <v>18</v>
+      </c>
+      <c r="AC71">
+        <v>30</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>19</v>
       </c>
@@ -2589,8 +3244,17 @@
       <c r="U72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB72">
+        <v>19</v>
+      </c>
+      <c r="AC72">
+        <v>43</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>20</v>
       </c>
@@ -2618,8 +3282,17 @@
       <c r="U73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB73">
+        <v>20</v>
+      </c>
+      <c r="AC73">
+        <v>23</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>21</v>
       </c>
@@ -2647,8 +3320,17 @@
       <c r="U74" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB74">
+        <v>21</v>
+      </c>
+      <c r="AC74">
+        <v>30</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>22</v>
       </c>
@@ -2676,8 +3358,17 @@
       <c r="U75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB75">
+        <v>22</v>
+      </c>
+      <c r="AC75">
+        <v>31</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>23</v>
       </c>
@@ -2705,8 +3396,17 @@
       <c r="U76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB76">
+        <v>23</v>
+      </c>
+      <c r="AC76">
+        <v>31</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24</v>
       </c>
@@ -2734,8 +3434,17 @@
       <c r="U77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB77">
+        <v>24</v>
+      </c>
+      <c r="AC77">
+        <v>30</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>25</v>
       </c>
@@ -2763,8 +3472,17 @@
       <c r="U78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB78">
+        <v>25</v>
+      </c>
+      <c r="AC78">
+        <v>30</v>
+      </c>
+      <c r="AD78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>26</v>
       </c>
@@ -2792,8 +3510,17 @@
       <c r="U79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB79">
+        <v>26</v>
+      </c>
+      <c r="AC79">
+        <v>34</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>27</v>
       </c>
@@ -2821,8 +3548,17 @@
       <c r="U80" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB80">
+        <v>27</v>
+      </c>
+      <c r="AC80">
+        <v>35</v>
+      </c>
+      <c r="AD80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>28</v>
       </c>
@@ -2850,8 +3586,17 @@
       <c r="U81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB81">
+        <v>28</v>
+      </c>
+      <c r="AC81">
+        <v>55</v>
+      </c>
+      <c r="AD81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>29</v>
       </c>
@@ -2879,8 +3624,17 @@
       <c r="U82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB82">
+        <v>29</v>
+      </c>
+      <c r="AC82">
+        <v>26</v>
+      </c>
+      <c r="AD82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>30</v>
       </c>
@@ -2908,8 +3662,17 @@
       <c r="U83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB83">
+        <v>30</v>
+      </c>
+      <c r="AC83">
+        <v>28</v>
+      </c>
+      <c r="AD83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>31</v>
       </c>
@@ -2937,8 +3700,17 @@
       <c r="U84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB84">
+        <v>31</v>
+      </c>
+      <c r="AC84">
+        <v>38</v>
+      </c>
+      <c r="AD84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -2948,8 +3720,11 @@
       <c r="S86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
@@ -2977,8 +3752,17 @@
       <c r="U87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB87">
+        <v>0</v>
+      </c>
+      <c r="AC87">
+        <v>21</v>
+      </c>
+      <c r="AD87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1</v>
       </c>
@@ -3006,8 +3790,17 @@
       <c r="U88" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB88">
+        <v>1</v>
+      </c>
+      <c r="AC88">
+        <v>26</v>
+      </c>
+      <c r="AD88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -3035,8 +3828,17 @@
       <c r="U89" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB89">
+        <v>2</v>
+      </c>
+      <c r="AC89">
+        <v>34</v>
+      </c>
+      <c r="AD89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3</v>
       </c>
@@ -3064,8 +3866,17 @@
       <c r="U90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB90">
+        <v>3</v>
+      </c>
+      <c r="AC90">
+        <v>23</v>
+      </c>
+      <c r="AD90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -3093,8 +3904,17 @@
       <c r="U91" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB91">
+        <v>4</v>
+      </c>
+      <c r="AC91">
+        <v>31</v>
+      </c>
+      <c r="AD91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>5</v>
       </c>
@@ -3122,8 +3942,17 @@
       <c r="U92" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB92">
+        <v>5</v>
+      </c>
+      <c r="AC92">
+        <v>27</v>
+      </c>
+      <c r="AD92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>6</v>
       </c>
@@ -3151,8 +3980,17 @@
       <c r="U93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB93">
+        <v>6</v>
+      </c>
+      <c r="AC93">
+        <v>37</v>
+      </c>
+      <c r="AD93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>7</v>
       </c>
@@ -3180,8 +4018,17 @@
       <c r="U94" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB94">
+        <v>7</v>
+      </c>
+      <c r="AC94">
+        <v>33</v>
+      </c>
+      <c r="AD94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>8</v>
       </c>
@@ -3209,8 +4056,17 @@
       <c r="U95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB95">
+        <v>8</v>
+      </c>
+      <c r="AC95">
+        <v>29</v>
+      </c>
+      <c r="AD95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9</v>
       </c>
@@ -3238,8 +4094,17 @@
       <c r="U96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB96">
+        <v>9</v>
+      </c>
+      <c r="AC96">
+        <v>33</v>
+      </c>
+      <c r="AD96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10</v>
       </c>
@@ -3267,8 +4132,17 @@
       <c r="U97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB97">
+        <v>10</v>
+      </c>
+      <c r="AC97">
+        <v>26</v>
+      </c>
+      <c r="AD97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>11</v>
       </c>
@@ -3296,8 +4170,17 @@
       <c r="U98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB98">
+        <v>11</v>
+      </c>
+      <c r="AC98">
+        <v>36</v>
+      </c>
+      <c r="AD98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>12</v>
       </c>
@@ -3325,8 +4208,17 @@
       <c r="U99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB99">
+        <v>12</v>
+      </c>
+      <c r="AC99">
+        <v>26</v>
+      </c>
+      <c r="AD99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>13</v>
       </c>
@@ -3354,8 +4246,17 @@
       <c r="U100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB100">
+        <v>13</v>
+      </c>
+      <c r="AC100">
+        <v>28</v>
+      </c>
+      <c r="AD100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>14</v>
       </c>
@@ -3383,8 +4284,17 @@
       <c r="U101" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB101">
+        <v>14</v>
+      </c>
+      <c r="AC101">
+        <v>26</v>
+      </c>
+      <c r="AD101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>15</v>
       </c>
@@ -3412,8 +4322,17 @@
       <c r="U102" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB102">
+        <v>15</v>
+      </c>
+      <c r="AC102">
+        <v>26</v>
+      </c>
+      <c r="AD102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>16</v>
       </c>
@@ -3441,8 +4360,17 @@
       <c r="U103" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB103">
+        <v>16</v>
+      </c>
+      <c r="AC103">
+        <v>28</v>
+      </c>
+      <c r="AD103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>17</v>
       </c>
@@ -3470,8 +4398,17 @@
       <c r="U104" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB104">
+        <v>17</v>
+      </c>
+      <c r="AC104">
+        <v>28</v>
+      </c>
+      <c r="AD104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>18</v>
       </c>
@@ -3499,8 +4436,17 @@
       <c r="U105" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB105">
+        <v>18</v>
+      </c>
+      <c r="AC105">
+        <v>26</v>
+      </c>
+      <c r="AD105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>19</v>
       </c>
@@ -3528,8 +4474,17 @@
       <c r="U106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB106">
+        <v>19</v>
+      </c>
+      <c r="AC106">
+        <v>44</v>
+      </c>
+      <c r="AD106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>20</v>
       </c>
@@ -3557,8 +4512,17 @@
       <c r="U107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB107">
+        <v>20</v>
+      </c>
+      <c r="AC107">
+        <v>27</v>
+      </c>
+      <c r="AD107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>21</v>
       </c>
@@ -3586,8 +4550,17 @@
       <c r="U108" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB108">
+        <v>21</v>
+      </c>
+      <c r="AC108">
+        <v>26</v>
+      </c>
+      <c r="AD108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>22</v>
       </c>
@@ -3615,8 +4588,17 @@
       <c r="U109" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB109">
+        <v>22</v>
+      </c>
+      <c r="AC109">
+        <v>26</v>
+      </c>
+      <c r="AD109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>23</v>
       </c>
@@ -3644,8 +4626,17 @@
       <c r="U110" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB110">
+        <v>23</v>
+      </c>
+      <c r="AC110">
+        <v>26</v>
+      </c>
+      <c r="AD110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>24</v>
       </c>
@@ -3673,8 +4664,17 @@
       <c r="U111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB111">
+        <v>24</v>
+      </c>
+      <c r="AC111">
+        <v>29</v>
+      </c>
+      <c r="AD111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>25</v>
       </c>
@@ -3702,8 +4702,17 @@
       <c r="U112" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB112">
+        <v>25</v>
+      </c>
+      <c r="AC112">
+        <v>26</v>
+      </c>
+      <c r="AD112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>26</v>
       </c>
@@ -3731,8 +4740,17 @@
       <c r="U113" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB113">
+        <v>26</v>
+      </c>
+      <c r="AC113">
+        <v>31</v>
+      </c>
+      <c r="AD113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>27</v>
       </c>
@@ -3760,8 +4778,17 @@
       <c r="U114" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB114">
+        <v>27</v>
+      </c>
+      <c r="AC114">
+        <v>41</v>
+      </c>
+      <c r="AD114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>28</v>
       </c>
@@ -3789,8 +4816,17 @@
       <c r="U115" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB115">
+        <v>28</v>
+      </c>
+      <c r="AC115">
+        <v>30</v>
+      </c>
+      <c r="AD115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>29</v>
       </c>
@@ -3818,8 +4854,17 @@
       <c r="U116" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB116">
+        <v>29</v>
+      </c>
+      <c r="AC116">
+        <v>21</v>
+      </c>
+      <c r="AD116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>30</v>
       </c>
@@ -3847,8 +4892,17 @@
       <c r="U117" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB117">
+        <v>30</v>
+      </c>
+      <c r="AC117">
+        <v>20</v>
+      </c>
+      <c r="AD117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>31</v>
       </c>
@@ -3876,8 +4930,17 @@
       <c r="U118" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB118">
+        <v>31</v>
+      </c>
+      <c r="AC118">
+        <v>27</v>
+      </c>
+      <c r="AD118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>14</v>
       </c>
@@ -3887,8 +4950,11 @@
       <c r="S120" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB120" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>0</v>
       </c>
@@ -3916,8 +4982,17 @@
       <c r="U121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB121">
+        <v>0</v>
+      </c>
+      <c r="AC121">
+        <v>26</v>
+      </c>
+      <c r="AD121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1</v>
       </c>
@@ -3945,8 +5020,17 @@
       <c r="U122" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB122">
+        <v>1</v>
+      </c>
+      <c r="AC122">
+        <v>41</v>
+      </c>
+      <c r="AD122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2</v>
       </c>
@@ -3974,8 +5058,17 @@
       <c r="U123" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB123">
+        <v>2</v>
+      </c>
+      <c r="AC123">
+        <v>34</v>
+      </c>
+      <c r="AD123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>3</v>
       </c>
@@ -4003,8 +5096,17 @@
       <c r="U124" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB124">
+        <v>3</v>
+      </c>
+      <c r="AC124">
+        <v>32</v>
+      </c>
+      <c r="AD124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>4</v>
       </c>
@@ -4032,8 +5134,17 @@
       <c r="U125" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB125">
+        <v>4</v>
+      </c>
+      <c r="AC125">
+        <v>34</v>
+      </c>
+      <c r="AD125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -4061,8 +5172,17 @@
       <c r="U126" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB126">
+        <v>5</v>
+      </c>
+      <c r="AC126">
+        <v>36</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>6</v>
       </c>
@@ -4090,8 +5210,17 @@
       <c r="U127" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB127">
+        <v>6</v>
+      </c>
+      <c r="AC127">
+        <v>34</v>
+      </c>
+      <c r="AD127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>7</v>
       </c>
@@ -4119,8 +5248,17 @@
       <c r="U128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB128">
+        <v>7</v>
+      </c>
+      <c r="AC128">
+        <v>32</v>
+      </c>
+      <c r="AD128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>8</v>
       </c>
@@ -4148,8 +5286,17 @@
       <c r="U129" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB129">
+        <v>8</v>
+      </c>
+      <c r="AC129">
+        <v>44</v>
+      </c>
+      <c r="AD129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>9</v>
       </c>
@@ -4177,8 +5324,17 @@
       <c r="U130" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB130">
+        <v>9</v>
+      </c>
+      <c r="AC130">
+        <v>39</v>
+      </c>
+      <c r="AD130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>10</v>
       </c>
@@ -4206,8 +5362,17 @@
       <c r="U131" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB131">
+        <v>10</v>
+      </c>
+      <c r="AC131">
+        <v>30</v>
+      </c>
+      <c r="AD131" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>11</v>
       </c>
@@ -4235,8 +5400,17 @@
       <c r="U132" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB132">
+        <v>11</v>
+      </c>
+      <c r="AC132">
+        <v>30</v>
+      </c>
+      <c r="AD132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>12</v>
       </c>
@@ -4264,8 +5438,17 @@
       <c r="U133" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB133">
+        <v>12</v>
+      </c>
+      <c r="AC133">
+        <v>34</v>
+      </c>
+      <c r="AD133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>13</v>
       </c>
@@ -4293,8 +5476,17 @@
       <c r="U134" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB134">
+        <v>13</v>
+      </c>
+      <c r="AC134">
+        <v>39</v>
+      </c>
+      <c r="AD134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>14</v>
       </c>
@@ -4322,8 +5514,17 @@
       <c r="U135" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB135">
+        <v>14</v>
+      </c>
+      <c r="AC135">
+        <v>30</v>
+      </c>
+      <c r="AD135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>15</v>
       </c>
@@ -4351,8 +5552,17 @@
       <c r="U136" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB136">
+        <v>15</v>
+      </c>
+      <c r="AC136">
+        <v>31</v>
+      </c>
+      <c r="AD136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>16</v>
       </c>
@@ -4380,8 +5590,17 @@
       <c r="U137" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB137">
+        <v>16</v>
+      </c>
+      <c r="AC137">
+        <v>42</v>
+      </c>
+      <c r="AD137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>17</v>
       </c>
@@ -4409,8 +5628,17 @@
       <c r="U138" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB138">
+        <v>17</v>
+      </c>
+      <c r="AC138">
+        <v>35</v>
+      </c>
+      <c r="AD138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>18</v>
       </c>
@@ -4438,8 +5666,17 @@
       <c r="U139" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB139">
+        <v>18</v>
+      </c>
+      <c r="AC139">
+        <v>30</v>
+      </c>
+      <c r="AD139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>19</v>
       </c>
@@ -4467,8 +5704,17 @@
       <c r="U140" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB140">
+        <v>19</v>
+      </c>
+      <c r="AC140">
+        <v>34</v>
+      </c>
+      <c r="AD140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>20</v>
       </c>
@@ -4496,8 +5742,17 @@
       <c r="U141" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB141">
+        <v>20</v>
+      </c>
+      <c r="AC141">
+        <v>30</v>
+      </c>
+      <c r="AD141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>21</v>
       </c>
@@ -4525,8 +5780,17 @@
       <c r="U142" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB142">
+        <v>21</v>
+      </c>
+      <c r="AC142">
+        <v>30</v>
+      </c>
+      <c r="AD142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>22</v>
       </c>
@@ -4554,8 +5818,17 @@
       <c r="U143" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB143">
+        <v>22</v>
+      </c>
+      <c r="AC143">
+        <v>30</v>
+      </c>
+      <c r="AD143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>23</v>
       </c>
@@ -4583,8 +5856,17 @@
       <c r="U144" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB144">
+        <v>23</v>
+      </c>
+      <c r="AC144">
+        <v>30</v>
+      </c>
+      <c r="AD144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>24</v>
       </c>
@@ -4612,8 +5894,17 @@
       <c r="U145" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB145">
+        <v>24</v>
+      </c>
+      <c r="AC145">
+        <v>31</v>
+      </c>
+      <c r="AD145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>25</v>
       </c>
@@ -4641,8 +5932,17 @@
       <c r="U146" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB146">
+        <v>25</v>
+      </c>
+      <c r="AC146">
+        <v>30</v>
+      </c>
+      <c r="AD146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>26</v>
       </c>
@@ -4670,8 +5970,17 @@
       <c r="U147" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB147">
+        <v>26</v>
+      </c>
+      <c r="AC147">
+        <v>37</v>
+      </c>
+      <c r="AD147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>27</v>
       </c>
@@ -4699,8 +6008,17 @@
       <c r="U148" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB148">
+        <v>27</v>
+      </c>
+      <c r="AC148">
+        <v>35</v>
+      </c>
+      <c r="AD148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>28</v>
       </c>
@@ -4728,8 +6046,17 @@
       <c r="U149" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB149">
+        <v>28</v>
+      </c>
+      <c r="AC149">
+        <v>28</v>
+      </c>
+      <c r="AD149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>29</v>
       </c>
@@ -4757,8 +6084,17 @@
       <c r="U150" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB150">
+        <v>29</v>
+      </c>
+      <c r="AC150">
+        <v>25</v>
+      </c>
+      <c r="AD150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>30</v>
       </c>
@@ -4786,8 +6122,17 @@
       <c r="U151" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AB151">
+        <v>30</v>
+      </c>
+      <c r="AC151">
+        <v>35</v>
+      </c>
+      <c r="AD151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>31</v>
       </c>
@@ -4813,6 +6158,15 @@
         <v>36</v>
       </c>
       <c r="U152" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB152">
+        <v>31</v>
+      </c>
+      <c r="AC152">
+        <v>36</v>
+      </c>
+      <c r="AD152" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Went back in time and re-recorded a previous run (the one prior to doing the "eliminate bank conflict" thing)
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="35">
   <si>
     <t>State</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>sort original data into copy buffer</t>
+  </si>
+  <si>
+    <t>sum of sort time</t>
+  </si>
+  <si>
+    <t>The difference is due to non-shader stuff</t>
   </si>
 </sst>
 </file>
@@ -486,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,14 +614,14 @@
       <c r="J9" t="s">
         <v>22</v>
       </c>
-      <c r="M9" t="s">
-        <v>23</v>
+      <c r="N9" t="s">
+        <v>33</v>
       </c>
       <c r="S9" t="s">
         <v>22</v>
       </c>
-      <c r="V9" t="s">
-        <v>23</v>
+      <c r="W9" t="s">
+        <v>33</v>
       </c>
       <c r="AB9" t="s">
         <v>22</v>
@@ -639,30 +645,24 @@
         <v>24</v>
       </c>
       <c r="J10">
-        <v>392545</v>
+        <v>6997</v>
       </c>
       <c r="K10" t="s">
         <v>9</v>
       </c>
-      <c r="M10">
-        <f>SUM(O37,O31,O25,O19)</f>
-        <v>7504</v>
-      </c>
-      <c r="N10" t="s">
-        <v>24</v>
+      <c r="N10">
+        <f>SUM(O19,O25,O31,O37)</f>
+        <v>3951</v>
       </c>
       <c r="S10">
-        <v>455535</v>
+        <v>6997</v>
       </c>
       <c r="T10" t="s">
         <v>9</v>
       </c>
-      <c r="V10">
-        <f>SUM(X37,X31,X25,X19)</f>
-        <v>4487</v>
-      </c>
-      <c r="W10" t="s">
-        <v>24</v>
+      <c r="W10">
+        <f>SUM(X19,X25,X31,X37)</f>
+        <v>3951</v>
       </c>
       <c r="AB10">
         <v>5332</v>
@@ -675,6 +675,14 @@
       </c>
       <c r="AG10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -702,15 +710,27 @@
         <v>9</v>
       </c>
       <c r="J13">
-        <v>3798</v>
+        <v>147</v>
       </c>
       <c r="K13" t="s">
         <v>9</v>
       </c>
       <c r="S13">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="T13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13">
+        <v>58</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF13">
+        <v>67</v>
+      </c>
+      <c r="AG13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -736,13 +756,13 @@
         <v>9</v>
       </c>
       <c r="J16">
-        <v>879025</v>
+        <v>891454</v>
       </c>
       <c r="K16" t="s">
         <v>9</v>
       </c>
       <c r="S16">
-        <v>894672</v>
+        <v>891454</v>
       </c>
       <c r="T16" t="s">
         <v>9</v>
@@ -801,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>256</v>
+        <v>52</v>
       </c>
       <c r="L19" t="s">
         <v>9</v>
@@ -811,13 +831,13 @@
       </c>
       <c r="O19">
         <f>SUM(K19:K50)</f>
-        <v>1359</v>
+        <v>1002</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
       <c r="T19">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="U19" t="s">
         <v>9</v>
@@ -827,7 +847,7 @@
       </c>
       <c r="X19">
         <f>SUM(T19:T50)</f>
-        <v>1384</v>
+        <v>1002</v>
       </c>
       <c r="AB19">
         <v>0</v>
@@ -867,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="L20" t="s">
         <v>9</v>
@@ -877,13 +897,13 @@
       </c>
       <c r="O20">
         <f>AVERAGE(K19:K50)</f>
-        <v>42.46875</v>
+        <v>31.3125</v>
       </c>
       <c r="S20">
         <v>1</v>
       </c>
       <c r="T20">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="U20" t="s">
         <v>9</v>
@@ -893,7 +913,7 @@
       </c>
       <c r="X20">
         <f>AVERAGE(T19:T50)</f>
-        <v>43.25</v>
+        <v>31.3125</v>
       </c>
       <c r="AB20">
         <v>1</v>
@@ -933,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="K21">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="L21" t="s">
         <v>9</v>
@@ -943,13 +963,13 @@
       </c>
       <c r="O21">
         <f>_xlfn.STDEV.P(K19:K50)</f>
-        <v>49.851018278842609</v>
+        <v>7.6503165784168701</v>
       </c>
       <c r="S21">
         <v>2</v>
       </c>
       <c r="T21">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="U21" t="s">
         <v>9</v>
@@ -959,7 +979,7 @@
       </c>
       <c r="X21">
         <f>_xlfn.STDEV.P(T19:T50)</f>
-        <v>15.817316460133179</v>
+        <v>7.6503165784168701</v>
       </c>
       <c r="AB21">
         <v>2</v>
@@ -999,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="K22">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="L22" t="s">
         <v>9</v>
@@ -1009,13 +1029,13 @@
       </c>
       <c r="O22">
         <f>MEDIAN(K19:K50)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S22">
         <v>3</v>
       </c>
       <c r="T22">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="U22" t="s">
         <v>9</v>
@@ -1025,7 +1045,7 @@
       </c>
       <c r="X22">
         <f>MEDIAN(T19:T50)</f>
-        <v>37.5</v>
+        <v>28</v>
       </c>
       <c r="AB22">
         <v>3</v>
@@ -1058,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="K23">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L23" t="s">
         <v>9</v>
@@ -1067,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="T23">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="U23" t="s">
         <v>9</v>
@@ -1099,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="K24">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L24" t="s">
         <v>9</v>
@@ -1111,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="T24">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="U24" t="s">
         <v>9</v>
@@ -1153,7 +1173,7 @@
         <v>6</v>
       </c>
       <c r="K25">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L25" t="s">
         <v>9</v>
@@ -1163,13 +1183,13 @@
       </c>
       <c r="O25">
         <f>SUM(K53:K84)</f>
-        <v>2610</v>
+        <v>1087</v>
       </c>
       <c r="S25">
         <v>6</v>
       </c>
       <c r="T25">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="U25" t="s">
         <v>9</v>
@@ -1179,7 +1199,7 @@
       </c>
       <c r="X25">
         <f>SUM(T53:T84)</f>
-        <v>1121</v>
+        <v>1087</v>
       </c>
       <c r="AB25">
         <v>6</v>
@@ -1219,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="K26">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L26" t="s">
         <v>9</v>
@@ -1229,13 +1249,13 @@
       </c>
       <c r="O26">
         <f>AVERAGE(K53:K84)</f>
-        <v>81.5625</v>
+        <v>33.96875</v>
       </c>
       <c r="S26">
         <v>7</v>
       </c>
       <c r="T26">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="U26" t="s">
         <v>9</v>
@@ -1245,7 +1265,7 @@
       </c>
       <c r="X26">
         <f>AVERAGE(T53:T84)</f>
-        <v>35.03125</v>
+        <v>33.96875</v>
       </c>
       <c r="AB26">
         <v>7</v>
@@ -1285,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="K27">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L27" t="s">
         <v>9</v>
@@ -1295,13 +1315,13 @@
       </c>
       <c r="O27">
         <f>_xlfn.STDEV.P(K53:K84)</f>
-        <v>250.36734729942322</v>
+        <v>27.379833334728318</v>
       </c>
       <c r="S27">
         <v>8</v>
       </c>
       <c r="T27">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="U27" t="s">
         <v>9</v>
@@ -1311,7 +1331,7 @@
       </c>
       <c r="X27">
         <f>_xlfn.STDEV.P(T53:T84)</f>
-        <v>15.611462885889329</v>
+        <v>27.379833334728318</v>
       </c>
       <c r="AB27">
         <v>8</v>
@@ -1351,7 +1371,7 @@
         <v>9</v>
       </c>
       <c r="K28">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L28" t="s">
         <v>9</v>
@@ -1361,13 +1381,13 @@
       </c>
       <c r="O28">
         <f>MEDIAN(K53:K84)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S28">
         <v>9</v>
       </c>
       <c r="T28">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="U28" t="s">
         <v>9</v>
@@ -1377,7 +1397,7 @@
       </c>
       <c r="X28">
         <f>MEDIAN(T53:T84)</f>
-        <v>30.5</v>
+        <v>28</v>
       </c>
       <c r="AB28">
         <v>9</v>
@@ -1410,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="K29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L29" t="s">
         <v>9</v>
@@ -1419,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="T29">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U29" t="s">
         <v>9</v>
@@ -1451,7 +1471,7 @@
         <v>11</v>
       </c>
       <c r="K30">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="L30" t="s">
         <v>9</v>
@@ -1463,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="T30">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="U30" t="s">
         <v>9</v>
@@ -1505,7 +1525,7 @@
         <v>12</v>
       </c>
       <c r="K31">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L31" t="s">
         <v>9</v>
@@ -1515,13 +1535,13 @@
       </c>
       <c r="O31">
         <f>SUM(K87:K118)</f>
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="S31">
         <v>12</v>
       </c>
       <c r="T31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U31" t="s">
         <v>9</v>
@@ -1531,7 +1551,7 @@
       </c>
       <c r="X31">
         <f>SUM(T87:T118)</f>
-        <v>918</v>
+        <v>870</v>
       </c>
       <c r="AB31">
         <v>12</v>
@@ -1571,7 +1591,7 @@
         <v>13</v>
       </c>
       <c r="K32">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L32" t="s">
         <v>9</v>
@@ -1581,13 +1601,13 @@
       </c>
       <c r="O32">
         <f>AVERAGE(K87:K118)</f>
-        <v>27.0625</v>
+        <v>27.1875</v>
       </c>
       <c r="S32">
         <v>13</v>
       </c>
       <c r="T32">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="U32" t="s">
         <v>9</v>
@@ -1597,7 +1617,7 @@
       </c>
       <c r="X32">
         <f>AVERAGE(T87:T118)</f>
-        <v>28.6875</v>
+        <v>27.1875</v>
       </c>
       <c r="AB32">
         <v>13</v>
@@ -1637,7 +1657,7 @@
         <v>14</v>
       </c>
       <c r="K33">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L33" t="s">
         <v>9</v>
@@ -1647,13 +1667,13 @@
       </c>
       <c r="O33">
         <f>_xlfn.STDEV.P(K87:K118)</f>
-        <v>7.8019929345007739</v>
+        <v>5.052459178459535</v>
       </c>
       <c r="S33">
         <v>14</v>
       </c>
       <c r="T33">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="U33" t="s">
         <v>9</v>
@@ -1663,7 +1683,7 @@
       </c>
       <c r="X33">
         <f>_xlfn.STDEV.P(T87:T118)</f>
-        <v>5.2881796253531332</v>
+        <v>5.052459178459535</v>
       </c>
       <c r="AB33">
         <v>14</v>
@@ -1703,7 +1723,7 @@
         <v>15</v>
       </c>
       <c r="K34">
-        <v>211</v>
+        <v>28</v>
       </c>
       <c r="L34" t="s">
         <v>9</v>
@@ -1719,7 +1739,7 @@
         <v>15</v>
       </c>
       <c r="T34">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U34" t="s">
         <v>9</v>
@@ -1729,7 +1749,7 @@
       </c>
       <c r="X34">
         <f>MEDIAN(T87:T118)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AB34">
         <v>15</v>
@@ -1762,7 +1782,7 @@
         <v>16</v>
       </c>
       <c r="K35">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L35" t="s">
         <v>9</v>
@@ -1771,7 +1791,7 @@
         <v>16</v>
       </c>
       <c r="T35">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="U35" t="s">
         <v>9</v>
@@ -1803,7 +1823,7 @@
         <v>17</v>
       </c>
       <c r="K36">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L36" t="s">
         <v>9</v>
@@ -1815,7 +1835,7 @@
         <v>17</v>
       </c>
       <c r="T36">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="U36" t="s">
         <v>9</v>
@@ -1857,7 +1877,7 @@
         <v>18</v>
       </c>
       <c r="K37">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="L37" t="s">
         <v>9</v>
@@ -1867,13 +1887,13 @@
       </c>
       <c r="O37">
         <f>SUM(K121:K152)</f>
-        <v>2669</v>
+        <v>992</v>
       </c>
       <c r="S37">
         <v>18</v>
       </c>
       <c r="T37">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="U37" t="s">
         <v>9</v>
@@ -1883,7 +1903,7 @@
       </c>
       <c r="X37">
         <f>SUM(T121:T152)</f>
-        <v>1064</v>
+        <v>992</v>
       </c>
       <c r="AB37">
         <v>18</v>
@@ -1923,7 +1943,7 @@
         <v>19</v>
       </c>
       <c r="K38">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L38" t="s">
         <v>9</v>
@@ -1933,13 +1953,13 @@
       </c>
       <c r="O38">
         <f>AVERAGE(K121:K152)</f>
-        <v>83.40625</v>
+        <v>31</v>
       </c>
       <c r="S38">
         <v>19</v>
       </c>
       <c r="T38">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="U38" t="s">
         <v>9</v>
@@ -1949,7 +1969,7 @@
       </c>
       <c r="X38">
         <f>AVERAGE(T121:T152)</f>
-        <v>33.25</v>
+        <v>31</v>
       </c>
       <c r="AB38">
         <v>19</v>
@@ -1989,7 +2009,7 @@
         <v>20</v>
       </c>
       <c r="K39">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L39" t="s">
         <v>9</v>
@@ -1999,13 +2019,13 @@
       </c>
       <c r="O39">
         <f>_xlfn.STDEV.P(K121:K152)</f>
-        <v>275.55578602333412</v>
+        <v>6.098155458825234</v>
       </c>
       <c r="S39">
         <v>20</v>
       </c>
       <c r="T39">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="U39" t="s">
         <v>9</v>
@@ -2015,7 +2035,7 @@
       </c>
       <c r="X39">
         <f>_xlfn.STDEV.P(T121:T152)</f>
-        <v>4.3874821936960613</v>
+        <v>6.098155458825234</v>
       </c>
       <c r="AB39">
         <v>20</v>
@@ -2065,13 +2085,13 @@
       </c>
       <c r="O40">
         <f>MEDIAN(K121:K152)</f>
-        <v>28.5</v>
+        <v>29</v>
       </c>
       <c r="S40">
         <v>21</v>
       </c>
       <c r="T40">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="U40" t="s">
         <v>9</v>
@@ -2081,7 +2101,7 @@
       </c>
       <c r="X40">
         <f>MEDIAN(T121:T152)</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AB40">
         <v>21</v>
@@ -2123,7 +2143,7 @@
         <v>22</v>
       </c>
       <c r="T41">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U41" t="s">
         <v>9</v>
@@ -2152,7 +2172,7 @@
         <v>23</v>
       </c>
       <c r="K42">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L42" t="s">
         <v>9</v>
@@ -2161,7 +2181,7 @@
         <v>23</v>
       </c>
       <c r="T42">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U42" t="s">
         <v>9</v>
@@ -2199,7 +2219,7 @@
         <v>24</v>
       </c>
       <c r="T43">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="U43" t="s">
         <v>9</v>
@@ -2228,7 +2248,7 @@
         <v>25</v>
       </c>
       <c r="K44">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L44" t="s">
         <v>9</v>
@@ -2237,7 +2257,7 @@
         <v>25</v>
       </c>
       <c r="T44">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="U44" t="s">
         <v>9</v>
@@ -2266,7 +2286,7 @@
         <v>26</v>
       </c>
       <c r="K45">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L45" t="s">
         <v>9</v>
@@ -2275,7 +2295,7 @@
         <v>26</v>
       </c>
       <c r="T45">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U45" t="s">
         <v>9</v>
@@ -2304,7 +2324,7 @@
         <v>27</v>
       </c>
       <c r="K46">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L46" t="s">
         <v>9</v>
@@ -2313,7 +2333,7 @@
         <v>27</v>
       </c>
       <c r="T46">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="U46" t="s">
         <v>9</v>
@@ -2342,7 +2362,7 @@
         <v>28</v>
       </c>
       <c r="K47">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="L47" t="s">
         <v>9</v>
@@ -2351,7 +2371,7 @@
         <v>28</v>
       </c>
       <c r="T47">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="U47" t="s">
         <v>9</v>
@@ -2380,7 +2400,7 @@
         <v>29</v>
       </c>
       <c r="K48">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L48" t="s">
         <v>9</v>
@@ -2389,7 +2409,7 @@
         <v>29</v>
       </c>
       <c r="T48">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="U48" t="s">
         <v>9</v>
@@ -2418,7 +2438,7 @@
         <v>30</v>
       </c>
       <c r="K49">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L49" t="s">
         <v>9</v>
@@ -2427,7 +2447,7 @@
         <v>30</v>
       </c>
       <c r="T49">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="U49" t="s">
         <v>9</v>
@@ -2456,7 +2476,7 @@
         <v>31</v>
       </c>
       <c r="K50">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L50" t="s">
         <v>9</v>
@@ -2465,7 +2485,7 @@
         <v>31</v>
       </c>
       <c r="T50">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="U50" t="s">
         <v>9</v>
@@ -2508,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>1464</v>
+        <v>45</v>
       </c>
       <c r="L53" t="s">
         <v>9</v>
@@ -2517,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="U53" t="s">
         <v>9</v>
@@ -2546,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="L54" t="s">
         <v>9</v>
@@ -2555,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="T54">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="U54" t="s">
         <v>9</v>
@@ -2584,7 +2604,7 @@
         <v>2</v>
       </c>
       <c r="K55">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
@@ -2593,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="T55">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="U55" t="s">
         <v>9</v>
@@ -2622,7 +2642,7 @@
         <v>3</v>
       </c>
       <c r="K56">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="L56" t="s">
         <v>9</v>
@@ -2631,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="T56">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="U56" t="s">
         <v>9</v>
@@ -2660,7 +2680,7 @@
         <v>4</v>
       </c>
       <c r="K57">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L57" t="s">
         <v>9</v>
@@ -2669,7 +2689,7 @@
         <v>4</v>
       </c>
       <c r="T57">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U57" t="s">
         <v>9</v>
@@ -2698,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="K58">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L58" t="s">
         <v>9</v>
@@ -2707,7 +2727,7 @@
         <v>5</v>
       </c>
       <c r="T58">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U58" t="s">
         <v>9</v>
@@ -2736,7 +2756,7 @@
         <v>6</v>
       </c>
       <c r="K59">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L59" t="s">
         <v>9</v>
@@ -2745,7 +2765,7 @@
         <v>6</v>
       </c>
       <c r="T59">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="U59" t="s">
         <v>9</v>
@@ -2774,7 +2794,7 @@
         <v>7</v>
       </c>
       <c r="K60">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L60" t="s">
         <v>9</v>
@@ -2783,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="T60">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="U60" t="s">
         <v>9</v>
@@ -2812,7 +2832,7 @@
         <v>8</v>
       </c>
       <c r="K61">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L61" t="s">
         <v>9</v>
@@ -2821,7 +2841,7 @@
         <v>8</v>
       </c>
       <c r="T61">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="U61" t="s">
         <v>9</v>
@@ -2850,7 +2870,7 @@
         <v>9</v>
       </c>
       <c r="K62">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L62" t="s">
         <v>9</v>
@@ -2859,7 +2879,7 @@
         <v>9</v>
       </c>
       <c r="T62">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="U62" t="s">
         <v>9</v>
@@ -2888,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="K63">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L63" t="s">
         <v>9</v>
@@ -2897,7 +2917,7 @@
         <v>10</v>
       </c>
       <c r="T63">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="U63" t="s">
         <v>9</v>
@@ -2935,7 +2955,7 @@
         <v>11</v>
       </c>
       <c r="T64">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U64" t="s">
         <v>9</v>
@@ -2964,7 +2984,7 @@
         <v>12</v>
       </c>
       <c r="K65">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L65" t="s">
         <v>9</v>
@@ -2973,7 +2993,7 @@
         <v>12</v>
       </c>
       <c r="T65">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U65" t="s">
         <v>9</v>
@@ -3002,7 +3022,7 @@
         <v>13</v>
       </c>
       <c r="K66">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L66" t="s">
         <v>9</v>
@@ -3011,7 +3031,7 @@
         <v>13</v>
       </c>
       <c r="T66">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U66" t="s">
         <v>9</v>
@@ -3040,7 +3060,7 @@
         <v>14</v>
       </c>
       <c r="K67">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L67" t="s">
         <v>9</v>
@@ -3049,7 +3069,7 @@
         <v>14</v>
       </c>
       <c r="T67">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U67" t="s">
         <v>9</v>
@@ -3078,7 +3098,7 @@
         <v>15</v>
       </c>
       <c r="K68">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L68" t="s">
         <v>9</v>
@@ -3087,7 +3107,7 @@
         <v>15</v>
       </c>
       <c r="T68">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="U68" t="s">
         <v>9</v>
@@ -3116,7 +3136,7 @@
         <v>16</v>
       </c>
       <c r="K69">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L69" t="s">
         <v>9</v>
@@ -3125,7 +3145,7 @@
         <v>16</v>
       </c>
       <c r="T69">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="U69" t="s">
         <v>9</v>
@@ -3154,7 +3174,7 @@
         <v>17</v>
       </c>
       <c r="K70">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L70" t="s">
         <v>9</v>
@@ -3163,7 +3183,7 @@
         <v>17</v>
       </c>
       <c r="T70">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="U70" t="s">
         <v>9</v>
@@ -3192,7 +3212,7 @@
         <v>18</v>
       </c>
       <c r="K71">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L71" t="s">
         <v>9</v>
@@ -3201,7 +3221,7 @@
         <v>18</v>
       </c>
       <c r="T71">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U71" t="s">
         <v>9</v>
@@ -3230,7 +3250,7 @@
         <v>19</v>
       </c>
       <c r="K72">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L72" t="s">
         <v>9</v>
@@ -3239,7 +3259,7 @@
         <v>19</v>
       </c>
       <c r="T72">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="U72" t="s">
         <v>9</v>
@@ -3268,7 +3288,7 @@
         <v>20</v>
       </c>
       <c r="K73">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L73" t="s">
         <v>9</v>
@@ -3277,7 +3297,7 @@
         <v>20</v>
       </c>
       <c r="T73">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="U73" t="s">
         <v>9</v>
@@ -3306,7 +3326,7 @@
         <v>21</v>
       </c>
       <c r="K74">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L74" t="s">
         <v>9</v>
@@ -3315,7 +3335,7 @@
         <v>21</v>
       </c>
       <c r="T74">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U74" t="s">
         <v>9</v>
@@ -3344,7 +3364,7 @@
         <v>22</v>
       </c>
       <c r="K75">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L75" t="s">
         <v>9</v>
@@ -3353,7 +3373,7 @@
         <v>22</v>
       </c>
       <c r="T75">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U75" t="s">
         <v>9</v>
@@ -3382,7 +3402,7 @@
         <v>23</v>
       </c>
       <c r="K76">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L76" t="s">
         <v>9</v>
@@ -3391,7 +3411,7 @@
         <v>23</v>
       </c>
       <c r="T76">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U76" t="s">
         <v>9</v>
@@ -3420,7 +3440,7 @@
         <v>24</v>
       </c>
       <c r="K77">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L77" t="s">
         <v>9</v>
@@ -3429,7 +3449,7 @@
         <v>24</v>
       </c>
       <c r="T77">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="U77" t="s">
         <v>9</v>
@@ -3467,7 +3487,7 @@
         <v>25</v>
       </c>
       <c r="T78">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U78" t="s">
         <v>9</v>
@@ -3496,7 +3516,7 @@
         <v>26</v>
       </c>
       <c r="K79">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L79" t="s">
         <v>9</v>
@@ -3505,7 +3525,7 @@
         <v>26</v>
       </c>
       <c r="T79">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="U79" t="s">
         <v>9</v>
@@ -3534,7 +3554,7 @@
         <v>27</v>
       </c>
       <c r="K80">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L80" t="s">
         <v>9</v>
@@ -3543,7 +3563,7 @@
         <v>27</v>
       </c>
       <c r="T80">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="U80" t="s">
         <v>9</v>
@@ -3572,7 +3592,7 @@
         <v>28</v>
       </c>
       <c r="K81">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L81" t="s">
         <v>9</v>
@@ -3581,7 +3601,7 @@
         <v>28</v>
       </c>
       <c r="T81">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="U81" t="s">
         <v>9</v>
@@ -3610,7 +3630,7 @@
         <v>29</v>
       </c>
       <c r="K82">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L82" t="s">
         <v>9</v>
@@ -3619,7 +3639,7 @@
         <v>29</v>
       </c>
       <c r="T82">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="U82" t="s">
         <v>9</v>
@@ -3648,7 +3668,7 @@
         <v>30</v>
       </c>
       <c r="K83">
-        <v>208</v>
+        <v>27</v>
       </c>
       <c r="L83" t="s">
         <v>9</v>
@@ -3657,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="T83">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U83" t="s">
         <v>9</v>
@@ -3686,7 +3706,7 @@
         <v>31</v>
       </c>
       <c r="K84">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="L84" t="s">
         <v>9</v>
@@ -3695,7 +3715,7 @@
         <v>31</v>
       </c>
       <c r="T84">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U84" t="s">
         <v>9</v>
@@ -3738,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="L87" t="s">
         <v>9</v>
@@ -3747,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="U87" t="s">
         <v>9</v>
@@ -3776,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="K88">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="L88" t="s">
         <v>9</v>
@@ -3785,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="T88">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="U88" t="s">
         <v>9</v>
@@ -3814,7 +3834,7 @@
         <v>2</v>
       </c>
       <c r="K89">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="L89" t="s">
         <v>9</v>
@@ -3823,7 +3843,7 @@
         <v>2</v>
       </c>
       <c r="T89">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="U89" t="s">
         <v>9</v>
@@ -3852,7 +3872,7 @@
         <v>3</v>
       </c>
       <c r="K90">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="L90" t="s">
         <v>9</v>
@@ -3861,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="T90">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="U90" t="s">
         <v>9</v>
@@ -3899,7 +3919,7 @@
         <v>4</v>
       </c>
       <c r="T91">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="U91" t="s">
         <v>9</v>
@@ -3928,7 +3948,7 @@
         <v>5</v>
       </c>
       <c r="K92">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L92" t="s">
         <v>9</v>
@@ -3937,7 +3957,7 @@
         <v>5</v>
       </c>
       <c r="T92">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U92" t="s">
         <v>9</v>
@@ -3966,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="K93">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L93" t="s">
         <v>9</v>
@@ -3975,7 +3995,7 @@
         <v>6</v>
       </c>
       <c r="T93">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="U93" t="s">
         <v>9</v>
@@ -4004,7 +4024,7 @@
         <v>7</v>
       </c>
       <c r="K94">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L94" t="s">
         <v>9</v>
@@ -4013,7 +4033,7 @@
         <v>7</v>
       </c>
       <c r="T94">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="U94" t="s">
         <v>9</v>
@@ -4042,7 +4062,7 @@
         <v>8</v>
       </c>
       <c r="K95">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L95" t="s">
         <v>9</v>
@@ -4051,7 +4071,7 @@
         <v>8</v>
       </c>
       <c r="T95">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="U95" t="s">
         <v>9</v>
@@ -4089,7 +4109,7 @@
         <v>9</v>
       </c>
       <c r="T96">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="U96" t="s">
         <v>9</v>
@@ -4118,7 +4138,7 @@
         <v>10</v>
       </c>
       <c r="K97">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L97" t="s">
         <v>9</v>
@@ -4127,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="T97">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U97" t="s">
         <v>9</v>
@@ -4156,7 +4176,7 @@
         <v>11</v>
       </c>
       <c r="K98">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="L98" t="s">
         <v>9</v>
@@ -4165,7 +4185,7 @@
         <v>11</v>
       </c>
       <c r="T98">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="U98" t="s">
         <v>9</v>
@@ -4194,7 +4214,7 @@
         <v>12</v>
       </c>
       <c r="K99">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L99" t="s">
         <v>9</v>
@@ -4203,7 +4223,7 @@
         <v>12</v>
       </c>
       <c r="T99">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U99" t="s">
         <v>9</v>
@@ -4232,7 +4252,7 @@
         <v>13</v>
       </c>
       <c r="K100">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L100" t="s">
         <v>9</v>
@@ -4241,7 +4261,7 @@
         <v>13</v>
       </c>
       <c r="T100">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U100" t="s">
         <v>9</v>
@@ -4270,7 +4290,7 @@
         <v>14</v>
       </c>
       <c r="K101">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L101" t="s">
         <v>9</v>
@@ -4279,7 +4299,7 @@
         <v>14</v>
       </c>
       <c r="T101">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U101" t="s">
         <v>9</v>
@@ -4308,7 +4328,7 @@
         <v>15</v>
       </c>
       <c r="K102">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L102" t="s">
         <v>9</v>
@@ -4317,7 +4337,7 @@
         <v>15</v>
       </c>
       <c r="T102">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U102" t="s">
         <v>9</v>
@@ -4355,7 +4375,7 @@
         <v>16</v>
       </c>
       <c r="T103">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U103" t="s">
         <v>9</v>
@@ -4384,7 +4404,7 @@
         <v>17</v>
       </c>
       <c r="K104">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L104" t="s">
         <v>9</v>
@@ -4393,7 +4413,7 @@
         <v>17</v>
       </c>
       <c r="T104">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U104" t="s">
         <v>9</v>
@@ -4431,7 +4451,7 @@
         <v>18</v>
       </c>
       <c r="T105">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U105" t="s">
         <v>9</v>
@@ -4460,7 +4480,7 @@
         <v>19</v>
       </c>
       <c r="K106">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L106" t="s">
         <v>9</v>
@@ -4469,7 +4489,7 @@
         <v>19</v>
       </c>
       <c r="T106">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="U106" t="s">
         <v>9</v>
@@ -4498,7 +4518,7 @@
         <v>20</v>
       </c>
       <c r="K107">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L107" t="s">
         <v>9</v>
@@ -4507,7 +4527,7 @@
         <v>20</v>
       </c>
       <c r="T107">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="U107" t="s">
         <v>9</v>
@@ -4545,7 +4565,7 @@
         <v>21</v>
       </c>
       <c r="T108">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U108" t="s">
         <v>9</v>
@@ -4574,7 +4594,7 @@
         <v>22</v>
       </c>
       <c r="K109">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L109" t="s">
         <v>9</v>
@@ -4583,7 +4603,7 @@
         <v>22</v>
       </c>
       <c r="T109">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U109" t="s">
         <v>9</v>
@@ -4612,7 +4632,7 @@
         <v>23</v>
       </c>
       <c r="K110">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L110" t="s">
         <v>9</v>
@@ -4621,7 +4641,7 @@
         <v>23</v>
       </c>
       <c r="T110">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U110" t="s">
         <v>9</v>
@@ -4659,7 +4679,7 @@
         <v>24</v>
       </c>
       <c r="T111">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="U111" t="s">
         <v>9</v>
@@ -4688,7 +4708,7 @@
         <v>25</v>
       </c>
       <c r="K112">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L112" t="s">
         <v>9</v>
@@ -4697,7 +4717,7 @@
         <v>25</v>
       </c>
       <c r="T112">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U112" t="s">
         <v>9</v>
@@ -4735,7 +4755,7 @@
         <v>26</v>
       </c>
       <c r="T113">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="U113" t="s">
         <v>9</v>
@@ -4764,7 +4784,7 @@
         <v>27</v>
       </c>
       <c r="K114">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="L114" t="s">
         <v>9</v>
@@ -4773,7 +4793,7 @@
         <v>27</v>
       </c>
       <c r="T114">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="U114" t="s">
         <v>9</v>
@@ -4802,7 +4822,7 @@
         <v>28</v>
       </c>
       <c r="K115">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L115" t="s">
         <v>9</v>
@@ -4811,7 +4831,7 @@
         <v>28</v>
       </c>
       <c r="T115">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U115" t="s">
         <v>9</v>
@@ -4840,7 +4860,7 @@
         <v>29</v>
       </c>
       <c r="K116">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L116" t="s">
         <v>9</v>
@@ -4849,7 +4869,7 @@
         <v>29</v>
       </c>
       <c r="T116">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U116" t="s">
         <v>9</v>
@@ -4878,7 +4898,7 @@
         <v>30</v>
       </c>
       <c r="K117">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L117" t="s">
         <v>9</v>
@@ -4887,7 +4907,7 @@
         <v>30</v>
       </c>
       <c r="T117">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="U117" t="s">
         <v>9</v>
@@ -4916,7 +4936,7 @@
         <v>31</v>
       </c>
       <c r="K118">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="L118" t="s">
         <v>9</v>
@@ -4925,7 +4945,7 @@
         <v>31</v>
       </c>
       <c r="T118">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U118" t="s">
         <v>9</v>
@@ -4968,7 +4988,7 @@
         <v>0</v>
       </c>
       <c r="K121">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="L121" t="s">
         <v>9</v>
@@ -4977,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="T121">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="U121" t="s">
         <v>9</v>
@@ -5006,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="K122">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="L122" t="s">
         <v>9</v>
@@ -5015,7 +5035,7 @@
         <v>1</v>
       </c>
       <c r="T122">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="U122" t="s">
         <v>9</v>
@@ -5044,7 +5064,7 @@
         <v>2</v>
       </c>
       <c r="K123">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L123" t="s">
         <v>9</v>
@@ -5053,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="T123">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="U123" t="s">
         <v>9</v>
@@ -5082,7 +5102,7 @@
         <v>3</v>
       </c>
       <c r="K124">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="L124" t="s">
         <v>9</v>
@@ -5091,7 +5111,7 @@
         <v>3</v>
       </c>
       <c r="T124">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="U124" t="s">
         <v>9</v>
@@ -5120,7 +5140,7 @@
         <v>4</v>
       </c>
       <c r="K125">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L125" t="s">
         <v>9</v>
@@ -5129,7 +5149,7 @@
         <v>4</v>
       </c>
       <c r="T125">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="U125" t="s">
         <v>9</v>
@@ -5158,7 +5178,7 @@
         <v>5</v>
       </c>
       <c r="K126">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L126" t="s">
         <v>9</v>
@@ -5167,7 +5187,7 @@
         <v>5</v>
       </c>
       <c r="T126">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="U126" t="s">
         <v>9</v>
@@ -5196,7 +5216,7 @@
         <v>6</v>
       </c>
       <c r="K127">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="L127" t="s">
         <v>9</v>
@@ -5205,7 +5225,7 @@
         <v>6</v>
       </c>
       <c r="T127">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="U127" t="s">
         <v>9</v>
@@ -5234,7 +5254,7 @@
         <v>7</v>
       </c>
       <c r="K128">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L128" t="s">
         <v>9</v>
@@ -5243,7 +5263,7 @@
         <v>7</v>
       </c>
       <c r="T128">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U128" t="s">
         <v>9</v>
@@ -5272,7 +5292,7 @@
         <v>8</v>
       </c>
       <c r="K129">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L129" t="s">
         <v>9</v>
@@ -5281,7 +5301,7 @@
         <v>8</v>
       </c>
       <c r="T129">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="U129" t="s">
         <v>9</v>
@@ -5310,7 +5330,7 @@
         <v>9</v>
       </c>
       <c r="K130">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L130" t="s">
         <v>9</v>
@@ -5319,7 +5339,7 @@
         <v>9</v>
       </c>
       <c r="T130">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="U130" t="s">
         <v>9</v>
@@ -5348,7 +5368,7 @@
         <v>10</v>
       </c>
       <c r="K131">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="L131" t="s">
         <v>9</v>
@@ -5357,7 +5377,7 @@
         <v>10</v>
       </c>
       <c r="T131">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U131" t="s">
         <v>9</v>
@@ -5386,7 +5406,7 @@
         <v>11</v>
       </c>
       <c r="K132">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L132" t="s">
         <v>9</v>
@@ -5395,7 +5415,7 @@
         <v>11</v>
       </c>
       <c r="T132">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U132" t="s">
         <v>9</v>
@@ -5424,7 +5444,7 @@
         <v>12</v>
       </c>
       <c r="K133">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L133" t="s">
         <v>9</v>
@@ -5433,7 +5453,7 @@
         <v>12</v>
       </c>
       <c r="T133">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="U133" t="s">
         <v>9</v>
@@ -5471,7 +5491,7 @@
         <v>13</v>
       </c>
       <c r="T134">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="U134" t="s">
         <v>9</v>
@@ -5500,7 +5520,7 @@
         <v>14</v>
       </c>
       <c r="K135">
-        <v>1613</v>
+        <v>29</v>
       </c>
       <c r="L135" t="s">
         <v>9</v>
@@ -5509,7 +5529,7 @@
         <v>14</v>
       </c>
       <c r="T135">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U135" t="s">
         <v>9</v>
@@ -5538,7 +5558,7 @@
         <v>15</v>
       </c>
       <c r="K136">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L136" t="s">
         <v>9</v>
@@ -5547,7 +5567,7 @@
         <v>15</v>
       </c>
       <c r="T136">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U136" t="s">
         <v>9</v>
@@ -5585,7 +5605,7 @@
         <v>16</v>
       </c>
       <c r="T137">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="U137" t="s">
         <v>9</v>
@@ -5614,7 +5634,7 @@
         <v>17</v>
       </c>
       <c r="K138">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L138" t="s">
         <v>9</v>
@@ -5623,7 +5643,7 @@
         <v>17</v>
       </c>
       <c r="T138">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U138" t="s">
         <v>9</v>
@@ -5652,7 +5672,7 @@
         <v>18</v>
       </c>
       <c r="K139">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L139" t="s">
         <v>9</v>
@@ -5661,7 +5681,7 @@
         <v>18</v>
       </c>
       <c r="T139">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U139" t="s">
         <v>9</v>
@@ -5690,7 +5710,7 @@
         <v>19</v>
       </c>
       <c r="K140">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L140" t="s">
         <v>9</v>
@@ -5699,7 +5719,7 @@
         <v>19</v>
       </c>
       <c r="T140">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="U140" t="s">
         <v>9</v>
@@ -5728,7 +5748,7 @@
         <v>20</v>
       </c>
       <c r="K141">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L141" t="s">
         <v>9</v>
@@ -5737,7 +5757,7 @@
         <v>20</v>
       </c>
       <c r="T141">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U141" t="s">
         <v>9</v>
@@ -5775,7 +5795,7 @@
         <v>21</v>
       </c>
       <c r="T142">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U142" t="s">
         <v>9</v>
@@ -5813,7 +5833,7 @@
         <v>22</v>
       </c>
       <c r="T143">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U143" t="s">
         <v>9</v>
@@ -5842,7 +5862,7 @@
         <v>23</v>
       </c>
       <c r="K144">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L144" t="s">
         <v>9</v>
@@ -5851,7 +5871,7 @@
         <v>23</v>
       </c>
       <c r="T144">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U144" t="s">
         <v>9</v>
@@ -5889,7 +5909,7 @@
         <v>24</v>
       </c>
       <c r="T145">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U145" t="s">
         <v>9</v>
@@ -5918,7 +5938,7 @@
         <v>25</v>
       </c>
       <c r="K146">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="L146" t="s">
         <v>9</v>
@@ -5927,7 +5947,7 @@
         <v>25</v>
       </c>
       <c r="T146">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U146" t="s">
         <v>9</v>
@@ -5956,7 +5976,7 @@
         <v>26</v>
       </c>
       <c r="K147">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L147" t="s">
         <v>9</v>
@@ -5965,7 +5985,7 @@
         <v>26</v>
       </c>
       <c r="T147">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="U147" t="s">
         <v>9</v>
@@ -5994,7 +6014,7 @@
         <v>27</v>
       </c>
       <c r="K148">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L148" t="s">
         <v>9</v>
@@ -6003,7 +6023,7 @@
         <v>27</v>
       </c>
       <c r="T148">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U148" t="s">
         <v>9</v>
@@ -6032,7 +6052,7 @@
         <v>28</v>
       </c>
       <c r="K149">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L149" t="s">
         <v>9</v>
@@ -6041,7 +6061,7 @@
         <v>28</v>
       </c>
       <c r="T149">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U149" t="s">
         <v>9</v>
@@ -6070,7 +6090,7 @@
         <v>29</v>
       </c>
       <c r="K150">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L150" t="s">
         <v>9</v>
@@ -6079,7 +6099,7 @@
         <v>29</v>
       </c>
       <c r="T150">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U150" t="s">
         <v>9</v>
@@ -6108,7 +6128,7 @@
         <v>30</v>
       </c>
       <c r="K151">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L151" t="s">
         <v>9</v>
@@ -6117,7 +6137,7 @@
         <v>30</v>
       </c>
       <c r="T151">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="U151" t="s">
         <v>9</v>
@@ -6146,7 +6166,7 @@
         <v>31</v>
       </c>
       <c r="K152">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L152" t="s">
         <v>9</v>
@@ -6155,7 +6175,7 @@
         <v>31</v>
       </c>
       <c r="T152">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="U152" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Went back in time and re-recorded the timings for sorting with bank conflict elimination
</commit_message>
<xml_diff>
--- a/Optimization Timings.xlsx
+++ b/Optimization Timings.xlsx
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,14 +655,14 @@
         <v>3951</v>
       </c>
       <c r="S10">
-        <v>6997</v>
+        <v>4760</v>
       </c>
       <c r="T10" t="s">
         <v>9</v>
       </c>
       <c r="W10">
         <f>SUM(X19,X25,X31,X37)</f>
-        <v>3951</v>
+        <v>4320</v>
       </c>
       <c r="AB10">
         <v>5332</v>
@@ -716,7 +716,7 @@
         <v>9</v>
       </c>
       <c r="S13">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="T13" t="s">
         <v>9</v>
@@ -762,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="S16">
-        <v>891454</v>
+        <v>891228</v>
       </c>
       <c r="T16" t="s">
         <v>9</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="U19" t="s">
         <v>9</v>
@@ -847,7 +847,7 @@
       </c>
       <c r="X19">
         <f>SUM(T19:T50)</f>
-        <v>1002</v>
+        <v>1120</v>
       </c>
       <c r="AB19">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="T20">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U20" t="s">
         <v>9</v>
@@ -913,7 +913,7 @@
       </c>
       <c r="X20">
         <f>AVERAGE(T19:T50)</f>
-        <v>31.3125</v>
+        <v>35</v>
       </c>
       <c r="AB20">
         <v>1</v>
@@ -969,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="T21">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U21" t="s">
         <v>9</v>
@@ -979,7 +979,7 @@
       </c>
       <c r="X21">
         <f>_xlfn.STDEV.P(T19:T50)</f>
-        <v>7.6503165784168701</v>
+        <v>12.359207094308275</v>
       </c>
       <c r="AB21">
         <v>2</v>
@@ -1035,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="T22">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="U22" t="s">
         <v>9</v>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="X22">
         <f>MEDIAN(T19:T50)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AB22">
         <v>3</v>
@@ -1087,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="T23">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U23" t="s">
         <v>9</v>
@@ -1131,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="T24">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="U24" t="s">
         <v>9</v>
@@ -1189,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="T25">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="U25" t="s">
         <v>9</v>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="X25">
         <f>SUM(T53:T84)</f>
-        <v>1087</v>
+        <v>1129</v>
       </c>
       <c r="AB25">
         <v>6</v>
@@ -1255,7 +1255,7 @@
         <v>7</v>
       </c>
       <c r="T26">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U26" t="s">
         <v>9</v>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="X26">
         <f>AVERAGE(T53:T84)</f>
-        <v>33.96875</v>
+        <v>35.28125</v>
       </c>
       <c r="AB26">
         <v>7</v>
@@ -1321,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="T27">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U27" t="s">
         <v>9</v>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="X27">
         <f>_xlfn.STDEV.P(T53:T84)</f>
-        <v>27.379833334728318</v>
+        <v>20.474426693744075</v>
       </c>
       <c r="AB27">
         <v>8</v>
@@ -1387,7 +1387,7 @@
         <v>9</v>
       </c>
       <c r="T28">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U28" t="s">
         <v>9</v>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="X28">
         <f>MEDIAN(T53:T84)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AB28">
         <v>9</v>
@@ -1439,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="T29">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="U29" t="s">
         <v>9</v>
@@ -1483,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="T30">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="U30" t="s">
         <v>9</v>
@@ -1541,7 +1541,7 @@
         <v>12</v>
       </c>
       <c r="T31">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U31" t="s">
         <v>9</v>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="X31">
         <f>SUM(T87:T118)</f>
-        <v>870</v>
+        <v>983</v>
       </c>
       <c r="AB31">
         <v>12</v>
@@ -1607,7 +1607,7 @@
         <v>13</v>
       </c>
       <c r="T32">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U32" t="s">
         <v>9</v>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="X32">
         <f>AVERAGE(T87:T118)</f>
-        <v>27.1875</v>
+        <v>30.71875</v>
       </c>
       <c r="AB32">
         <v>13</v>
@@ -1673,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="T33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U33" t="s">
         <v>9</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="X33">
         <f>_xlfn.STDEV.P(T87:T118)</f>
-        <v>5.052459178459535</v>
+        <v>6.2561688306422809</v>
       </c>
       <c r="AB33">
         <v>14</v>
@@ -1739,7 +1739,7 @@
         <v>15</v>
       </c>
       <c r="T34">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U34" t="s">
         <v>9</v>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="X34">
         <f>MEDIAN(T87:T118)</f>
-        <v>25</v>
+        <v>27.5</v>
       </c>
       <c r="AB34">
         <v>15</v>
@@ -1791,7 +1791,7 @@
         <v>16</v>
       </c>
       <c r="T35">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U35" t="s">
         <v>9</v>
@@ -1835,7 +1835,7 @@
         <v>17</v>
       </c>
       <c r="T36">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U36" t="s">
         <v>9</v>
@@ -1893,7 +1893,7 @@
         <v>18</v>
       </c>
       <c r="T37">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U37" t="s">
         <v>9</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="X37">
         <f>SUM(T121:T152)</f>
-        <v>992</v>
+        <v>1088</v>
       </c>
       <c r="AB37">
         <v>18</v>
@@ -1959,7 +1959,7 @@
         <v>19</v>
       </c>
       <c r="T38">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U38" t="s">
         <v>9</v>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="X38">
         <f>AVERAGE(T121:T152)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AB38">
         <v>19</v>
@@ -2025,7 +2025,7 @@
         <v>20</v>
       </c>
       <c r="T39">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="U39" t="s">
         <v>9</v>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="X39">
         <f>_xlfn.STDEV.P(T121:T152)</f>
-        <v>6.098155458825234</v>
+        <v>6.8920243760451108</v>
       </c>
       <c r="AB39">
         <v>20</v>
@@ -2091,7 +2091,7 @@
         <v>21</v>
       </c>
       <c r="T40">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U40" t="s">
         <v>9</v>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="X40">
         <f>MEDIAN(T121:T152)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AB40">
         <v>21</v>
@@ -2143,7 +2143,7 @@
         <v>22</v>
       </c>
       <c r="T41">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U41" t="s">
         <v>9</v>
@@ -2181,7 +2181,7 @@
         <v>23</v>
       </c>
       <c r="T42">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U42" t="s">
         <v>9</v>
@@ -2219,7 +2219,7 @@
         <v>24</v>
       </c>
       <c r="T43">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U43" t="s">
         <v>9</v>
@@ -2257,7 +2257,7 @@
         <v>25</v>
       </c>
       <c r="T44">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U44" t="s">
         <v>9</v>
@@ -2295,7 +2295,7 @@
         <v>26</v>
       </c>
       <c r="T45">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U45" t="s">
         <v>9</v>
@@ -2333,7 +2333,7 @@
         <v>27</v>
       </c>
       <c r="T46">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U46" t="s">
         <v>9</v>
@@ -2371,7 +2371,7 @@
         <v>28</v>
       </c>
       <c r="T47">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="U47" t="s">
         <v>9</v>
@@ -2409,7 +2409,7 @@
         <v>29</v>
       </c>
       <c r="T48">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U48" t="s">
         <v>9</v>
@@ -2447,7 +2447,7 @@
         <v>30</v>
       </c>
       <c r="T49">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="U49" t="s">
         <v>9</v>
@@ -2485,7 +2485,7 @@
         <v>31</v>
       </c>
       <c r="T50">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U50" t="s">
         <v>9</v>
@@ -2537,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="U53" t="s">
         <v>9</v>
@@ -2575,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="T54">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U54" t="s">
         <v>9</v>
@@ -2613,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="T55">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="U55" t="s">
         <v>9</v>
@@ -2651,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="T56">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="U56" t="s">
         <v>9</v>
@@ -2689,7 +2689,7 @@
         <v>4</v>
       </c>
       <c r="T57">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U57" t="s">
         <v>9</v>
@@ -2727,7 +2727,7 @@
         <v>5</v>
       </c>
       <c r="T58">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U58" t="s">
         <v>9</v>
@@ -2765,7 +2765,7 @@
         <v>6</v>
       </c>
       <c r="T59">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U59" t="s">
         <v>9</v>
@@ -2803,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="T60">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U60" t="s">
         <v>9</v>
@@ -2841,7 +2841,7 @@
         <v>8</v>
       </c>
       <c r="T61">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U61" t="s">
         <v>9</v>
@@ -2879,7 +2879,7 @@
         <v>9</v>
       </c>
       <c r="T62">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U62" t="s">
         <v>9</v>
@@ -2917,7 +2917,7 @@
         <v>10</v>
       </c>
       <c r="T63">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="U63" t="s">
         <v>9</v>
@@ -2955,7 +2955,7 @@
         <v>11</v>
       </c>
       <c r="T64">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U64" t="s">
         <v>9</v>
@@ -2993,7 +2993,7 @@
         <v>12</v>
       </c>
       <c r="T65">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U65" t="s">
         <v>9</v>
@@ -3031,7 +3031,7 @@
         <v>13</v>
       </c>
       <c r="T66">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U66" t="s">
         <v>9</v>
@@ -3069,7 +3069,7 @@
         <v>14</v>
       </c>
       <c r="T67">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U67" t="s">
         <v>9</v>
@@ -3107,7 +3107,7 @@
         <v>15</v>
       </c>
       <c r="T68">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="U68" t="s">
         <v>9</v>
@@ -3145,7 +3145,7 @@
         <v>16</v>
       </c>
       <c r="T69">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U69" t="s">
         <v>9</v>
@@ -3183,7 +3183,7 @@
         <v>17</v>
       </c>
       <c r="T70">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U70" t="s">
         <v>9</v>
@@ -3221,7 +3221,7 @@
         <v>18</v>
       </c>
       <c r="T71">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="U71" t="s">
         <v>9</v>
@@ -3259,7 +3259,7 @@
         <v>19</v>
       </c>
       <c r="T72">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="U72" t="s">
         <v>9</v>
@@ -3297,7 +3297,7 @@
         <v>20</v>
       </c>
       <c r="T73">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U73" t="s">
         <v>9</v>
@@ -3335,7 +3335,7 @@
         <v>21</v>
       </c>
       <c r="T74">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U74" t="s">
         <v>9</v>
@@ -3373,7 +3373,7 @@
         <v>22</v>
       </c>
       <c r="T75">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U75" t="s">
         <v>9</v>
@@ -3411,7 +3411,7 @@
         <v>23</v>
       </c>
       <c r="T76">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U76" t="s">
         <v>9</v>
@@ -3449,7 +3449,7 @@
         <v>24</v>
       </c>
       <c r="T77">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U77" t="s">
         <v>9</v>
@@ -3487,7 +3487,7 @@
         <v>25</v>
       </c>
       <c r="T78">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U78" t="s">
         <v>9</v>
@@ -3525,7 +3525,7 @@
         <v>26</v>
       </c>
       <c r="T79">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="U79" t="s">
         <v>9</v>
@@ -3563,7 +3563,7 @@
         <v>27</v>
       </c>
       <c r="T80">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U80" t="s">
         <v>9</v>
@@ -3601,7 +3601,7 @@
         <v>28</v>
       </c>
       <c r="T81">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U81" t="s">
         <v>9</v>
@@ -3639,7 +3639,7 @@
         <v>29</v>
       </c>
       <c r="T82">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U82" t="s">
         <v>9</v>
@@ -3677,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="T83">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U83" t="s">
         <v>9</v>
@@ -3715,7 +3715,7 @@
         <v>31</v>
       </c>
       <c r="T84">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U84" t="s">
         <v>9</v>
@@ -3767,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U87" t="s">
         <v>9</v>
@@ -3805,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="T88">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="U88" t="s">
         <v>9</v>
@@ -3843,7 +3843,7 @@
         <v>2</v>
       </c>
       <c r="T89">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U89" t="s">
         <v>9</v>
@@ -3881,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="T90">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="U90" t="s">
         <v>9</v>
@@ -3919,7 +3919,7 @@
         <v>4</v>
       </c>
       <c r="T91">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U91" t="s">
         <v>9</v>
@@ -3957,7 +3957,7 @@
         <v>5</v>
       </c>
       <c r="T92">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="U92" t="s">
         <v>9</v>
@@ -3995,7 +3995,7 @@
         <v>6</v>
       </c>
       <c r="T93">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U93" t="s">
         <v>9</v>
@@ -4033,7 +4033,7 @@
         <v>7</v>
       </c>
       <c r="T94">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U94" t="s">
         <v>9</v>
@@ -4071,7 +4071,7 @@
         <v>8</v>
       </c>
       <c r="T95">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U95" t="s">
         <v>9</v>
@@ -4109,7 +4109,7 @@
         <v>9</v>
       </c>
       <c r="T96">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U96" t="s">
         <v>9</v>
@@ -4147,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="T97">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="U97" t="s">
         <v>9</v>
@@ -4185,7 +4185,7 @@
         <v>11</v>
       </c>
       <c r="T98">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U98" t="s">
         <v>9</v>
@@ -4223,7 +4223,7 @@
         <v>12</v>
       </c>
       <c r="T99">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U99" t="s">
         <v>9</v>
@@ -4261,7 +4261,7 @@
         <v>13</v>
       </c>
       <c r="T100">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U100" t="s">
         <v>9</v>
@@ -4299,7 +4299,7 @@
         <v>14</v>
       </c>
       <c r="T101">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U101" t="s">
         <v>9</v>
@@ -4337,7 +4337,7 @@
         <v>15</v>
       </c>
       <c r="T102">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U102" t="s">
         <v>9</v>
@@ -4375,7 +4375,7 @@
         <v>16</v>
       </c>
       <c r="T103">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U103" t="s">
         <v>9</v>
@@ -4413,7 +4413,7 @@
         <v>17</v>
       </c>
       <c r="T104">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U104" t="s">
         <v>9</v>
@@ -4451,7 +4451,7 @@
         <v>18</v>
       </c>
       <c r="T105">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U105" t="s">
         <v>9</v>
@@ -4489,7 +4489,7 @@
         <v>19</v>
       </c>
       <c r="T106">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="U106" t="s">
         <v>9</v>
@@ -4527,7 +4527,7 @@
         <v>20</v>
       </c>
       <c r="T107">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U107" t="s">
         <v>9</v>
@@ -4565,7 +4565,7 @@
         <v>21</v>
       </c>
       <c r="T108">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U108" t="s">
         <v>9</v>
@@ -4603,7 +4603,7 @@
         <v>22</v>
       </c>
       <c r="T109">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U109" t="s">
         <v>9</v>
@@ -4641,7 +4641,7 @@
         <v>23</v>
       </c>
       <c r="T110">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="U110" t="s">
         <v>9</v>
@@ -4679,7 +4679,7 @@
         <v>24</v>
       </c>
       <c r="T111">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U111" t="s">
         <v>9</v>
@@ -4717,7 +4717,7 @@
         <v>25</v>
       </c>
       <c r="T112">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U112" t="s">
         <v>9</v>
@@ -4755,7 +4755,7 @@
         <v>26</v>
       </c>
       <c r="T113">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U113" t="s">
         <v>9</v>
@@ -4793,7 +4793,7 @@
         <v>27</v>
       </c>
       <c r="T114">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="U114" t="s">
         <v>9</v>
@@ -4831,7 +4831,7 @@
         <v>28</v>
       </c>
       <c r="T115">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U115" t="s">
         <v>9</v>
@@ -4869,7 +4869,7 @@
         <v>29</v>
       </c>
       <c r="T116">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U116" t="s">
         <v>9</v>
@@ -4907,7 +4907,7 @@
         <v>30</v>
       </c>
       <c r="T117">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U117" t="s">
         <v>9</v>
@@ -4945,7 +4945,7 @@
         <v>31</v>
       </c>
       <c r="T118">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U118" t="s">
         <v>9</v>
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="T121">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U121" t="s">
         <v>9</v>
@@ -5073,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="T123">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="U123" t="s">
         <v>9</v>
@@ -5111,7 +5111,7 @@
         <v>3</v>
       </c>
       <c r="T124">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="U124" t="s">
         <v>9</v>
@@ -5149,7 +5149,7 @@
         <v>4</v>
       </c>
       <c r="T125">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="U125" t="s">
         <v>9</v>
@@ -5187,7 +5187,7 @@
         <v>5</v>
       </c>
       <c r="T126">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="U126" t="s">
         <v>9</v>
@@ -5225,7 +5225,7 @@
         <v>6</v>
       </c>
       <c r="T127">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U127" t="s">
         <v>9</v>
@@ -5263,7 +5263,7 @@
         <v>7</v>
       </c>
       <c r="T128">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U128" t="s">
         <v>9</v>
@@ -5301,7 +5301,7 @@
         <v>8</v>
       </c>
       <c r="T129">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U129" t="s">
         <v>9</v>
@@ -5339,7 +5339,7 @@
         <v>9</v>
       </c>
       <c r="T130">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="U130" t="s">
         <v>9</v>
@@ -5415,7 +5415,7 @@
         <v>11</v>
       </c>
       <c r="T132">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U132" t="s">
         <v>9</v>
@@ -5453,7 +5453,7 @@
         <v>12</v>
       </c>
       <c r="T133">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U133" t="s">
         <v>9</v>
@@ -5491,7 +5491,7 @@
         <v>13</v>
       </c>
       <c r="T134">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U134" t="s">
         <v>9</v>
@@ -5529,7 +5529,7 @@
         <v>14</v>
       </c>
       <c r="T135">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U135" t="s">
         <v>9</v>
@@ -5567,7 +5567,7 @@
         <v>15</v>
       </c>
       <c r="T136">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U136" t="s">
         <v>9</v>
@@ -5605,7 +5605,7 @@
         <v>16</v>
       </c>
       <c r="T137">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U137" t="s">
         <v>9</v>
@@ -5643,7 +5643,7 @@
         <v>17</v>
       </c>
       <c r="T138">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U138" t="s">
         <v>9</v>
@@ -5681,7 +5681,7 @@
         <v>18</v>
       </c>
       <c r="T139">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U139" t="s">
         <v>9</v>
@@ -5719,7 +5719,7 @@
         <v>19</v>
       </c>
       <c r="T140">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U140" t="s">
         <v>9</v>
@@ -5757,7 +5757,7 @@
         <v>20</v>
       </c>
       <c r="T141">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U141" t="s">
         <v>9</v>
@@ -5795,7 +5795,7 @@
         <v>21</v>
       </c>
       <c r="T142">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U142" t="s">
         <v>9</v>
@@ -5833,7 +5833,7 @@
         <v>22</v>
       </c>
       <c r="T143">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U143" t="s">
         <v>9</v>
@@ -5871,7 +5871,7 @@
         <v>23</v>
       </c>
       <c r="T144">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U144" t="s">
         <v>9</v>
@@ -5909,7 +5909,7 @@
         <v>24</v>
       </c>
       <c r="T145">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U145" t="s">
         <v>9</v>
@@ -5947,7 +5947,7 @@
         <v>25</v>
       </c>
       <c r="T146">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U146" t="s">
         <v>9</v>
@@ -5985,7 +5985,7 @@
         <v>26</v>
       </c>
       <c r="T147">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U147" t="s">
         <v>9</v>
@@ -6023,7 +6023,7 @@
         <v>27</v>
       </c>
       <c r="T148">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U148" t="s">
         <v>9</v>
@@ -6061,7 +6061,7 @@
         <v>28</v>
       </c>
       <c r="T149">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U149" t="s">
         <v>9</v>
@@ -6099,7 +6099,7 @@
         <v>29</v>
       </c>
       <c r="T150">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U150" t="s">
         <v>9</v>
@@ -6137,7 +6137,7 @@
         <v>30</v>
       </c>
       <c r="T151">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U151" t="s">
         <v>9</v>
@@ -6175,7 +6175,7 @@
         <v>31</v>
       </c>
       <c r="T152">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U152" t="s">
         <v>9</v>

</xml_diff>